<commit_message>
updated system transition report to show all indirect costs
git-svn-id: svn://107.170.10.188:8080/Semoss/trunk@2470 ef391c1c-ee15-45f7-b1d6-dde3d27a2169

Former-commit-id: a9c2807242a191a2cea7d671f6f5730c8b46f718
</commit_message>
<xml_diff>
--- a/export/Reports/Individual_System_LPI_Transition_Report_Template.xlsx
+++ b/export/Reports/Individual_System_LPI_Transition_Report_Template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="1110" windowWidth="15120" windowHeight="6405" tabRatio="834" activeTab="5"/>
+    <workbookView xWindow="240" yWindow="1110" windowWidth="15120" windowHeight="6405" tabRatio="834" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="32" r:id="rId1"/>
@@ -894,6 +894,12 @@
     <xf numFmtId="0" fontId="26" fillId="6" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="5" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="7" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -902,6 +908,18 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="10" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="3" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="5" borderId="5" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -912,28 +930,10 @@
     <xf numFmtId="0" fontId="13" fillId="5" borderId="7" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="10" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="5" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="7" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="3" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -981,12 +981,6 @@
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -996,7 +990,13 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -43500,22 +43500,22 @@
     <row r="1" spans="1:13" ht="7.5" customHeight="1"/>
     <row r="2" spans="1:13" s="4" customFormat="1" ht="250.5" customHeight="1">
       <c r="A2" s="3"/>
-      <c r="B2" s="57" t="s">
+      <c r="B2" s="46" t="s">
         <v>37</v>
       </c>
-      <c r="C2" s="58"/>
-      <c r="D2" s="46" t="s">
+      <c r="C2" s="47"/>
+      <c r="D2" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="E2" s="47"/>
-      <c r="F2" s="47"/>
-      <c r="G2" s="47"/>
-      <c r="H2" s="47"/>
-      <c r="I2" s="47"/>
-      <c r="J2" s="47"/>
-      <c r="K2" s="47"/>
-      <c r="L2" s="47"/>
-      <c r="M2" s="48"/>
+      <c r="E2" s="49"/>
+      <c r="F2" s="49"/>
+      <c r="G2" s="49"/>
+      <c r="H2" s="49"/>
+      <c r="I2" s="49"/>
+      <c r="J2" s="49"/>
+      <c r="K2" s="49"/>
+      <c r="L2" s="49"/>
+      <c r="M2" s="50"/>
     </row>
     <row r="3" spans="1:13" s="20" customFormat="1" ht="7.5" customHeight="1">
       <c r="A3" s="16"/>
@@ -43573,22 +43573,22 @@
     </row>
     <row r="7" spans="1:13" s="4" customFormat="1" ht="168.75" customHeight="1">
       <c r="A7" s="3"/>
-      <c r="B7" s="57" t="s">
+      <c r="B7" s="46" t="s">
         <v>30</v>
       </c>
-      <c r="C7" s="58"/>
-      <c r="D7" s="46" t="s">
+      <c r="C7" s="47"/>
+      <c r="D7" s="48" t="s">
         <v>63</v>
       </c>
-      <c r="E7" s="47"/>
-      <c r="F7" s="47"/>
-      <c r="G7" s="47"/>
-      <c r="H7" s="47"/>
-      <c r="I7" s="47"/>
-      <c r="J7" s="47"/>
-      <c r="K7" s="47"/>
-      <c r="L7" s="47"/>
-      <c r="M7" s="48"/>
+      <c r="E7" s="49"/>
+      <c r="F7" s="49"/>
+      <c r="G7" s="49"/>
+      <c r="H7" s="49"/>
+      <c r="I7" s="49"/>
+      <c r="J7" s="49"/>
+      <c r="K7" s="49"/>
+      <c r="L7" s="49"/>
+      <c r="M7" s="50"/>
     </row>
     <row r="8" spans="1:13" ht="8.25" customHeight="1">
       <c r="A8" s="5"/>
@@ -43599,65 +43599,67 @@
     </row>
     <row r="9" spans="1:13" s="8" customFormat="1" ht="18" customHeight="1">
       <c r="A9" s="7"/>
-      <c r="B9" s="49" t="s">
+      <c r="B9" s="55" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="50"/>
-      <c r="D9" s="50"/>
-      <c r="E9" s="50"/>
-      <c r="F9" s="50"/>
-      <c r="G9" s="50"/>
-      <c r="H9" s="50"/>
-      <c r="I9" s="50"/>
-      <c r="J9" s="50"/>
-      <c r="K9" s="50"/>
-      <c r="L9" s="50"/>
-      <c r="M9" s="51"/>
+      <c r="C9" s="56"/>
+      <c r="D9" s="56"/>
+      <c r="E9" s="56"/>
+      <c r="F9" s="56"/>
+      <c r="G9" s="56"/>
+      <c r="H9" s="56"/>
+      <c r="I9" s="56"/>
+      <c r="J9" s="56"/>
+      <c r="K9" s="56"/>
+      <c r="L9" s="56"/>
+      <c r="M9" s="57"/>
     </row>
     <row r="10" spans="1:13" s="8" customFormat="1" ht="28.5" customHeight="1">
       <c r="A10" s="7"/>
-      <c r="B10" s="52" t="s">
+      <c r="B10" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="C10" s="52"/>
-      <c r="D10" s="52" t="s">
+      <c r="C10" s="51"/>
+      <c r="D10" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="E10" s="59"/>
-      <c r="F10" s="52" t="s">
+      <c r="E10" s="54"/>
+      <c r="F10" s="51" t="s">
         <v>49</v>
       </c>
-      <c r="G10" s="52"/>
-      <c r="H10" s="53" t="s">
+      <c r="G10" s="51"/>
+      <c r="H10" s="58" t="s">
         <v>50</v>
       </c>
-      <c r="I10" s="54"/>
-      <c r="J10" s="52" t="s">
+      <c r="I10" s="59"/>
+      <c r="J10" s="51" t="s">
         <v>51</v>
       </c>
-      <c r="K10" s="52"/>
-      <c r="L10" s="52" t="s">
+      <c r="K10" s="51"/>
+      <c r="L10" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="M10" s="52"/>
+      <c r="M10" s="51"/>
     </row>
     <row r="11" spans="1:13" ht="42.75" customHeight="1">
       <c r="A11" s="5"/>
-      <c r="B11" s="55"/>
-      <c r="C11" s="56"/>
-      <c r="D11" s="55"/>
-      <c r="E11" s="56"/>
-      <c r="F11" s="55"/>
-      <c r="G11" s="56"/>
-      <c r="H11" s="55"/>
-      <c r="I11" s="56"/>
-      <c r="J11" s="55"/>
-      <c r="K11" s="56"/>
-      <c r="L11" s="55"/>
-      <c r="M11" s="56"/>
+      <c r="B11" s="52"/>
+      <c r="C11" s="53"/>
+      <c r="D11" s="52"/>
+      <c r="E11" s="53"/>
+      <c r="F11" s="52"/>
+      <c r="G11" s="53"/>
+      <c r="H11" s="52"/>
+      <c r="I11" s="53"/>
+      <c r="J11" s="52"/>
+      <c r="K11" s="53"/>
+      <c r="L11" s="52"/>
+      <c r="M11" s="53"/>
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="B11:C11"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B4:M4"/>
     <mergeCell ref="D2:M2"/>
@@ -43674,8 +43676,6 @@
     <mergeCell ref="D7:M7"/>
     <mergeCell ref="B9:M9"/>
     <mergeCell ref="B10:C10"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="B11:C11"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -44092,8 +44092,8 @@
   </sheetPr>
   <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="80" workbookViewId="0">
+      <selection activeCell="M23" sqref="M23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10" defaultRowHeight="12.75"/>
@@ -44123,17 +44123,17 @@
       <c r="A4" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="77" t="s">
+      <c r="B4" s="75" t="s">
         <v>64</v>
       </c>
-      <c r="C4" s="78"/>
-      <c r="D4" s="78"/>
-      <c r="E4" s="78"/>
-      <c r="F4" s="78"/>
-      <c r="G4" s="78"/>
-      <c r="H4" s="78"/>
-      <c r="I4" s="78"/>
-      <c r="J4" s="79"/>
+      <c r="C4" s="76"/>
+      <c r="D4" s="76"/>
+      <c r="E4" s="76"/>
+      <c r="F4" s="76"/>
+      <c r="G4" s="76"/>
+      <c r="H4" s="76"/>
+      <c r="I4" s="76"/>
+      <c r="J4" s="77"/>
     </row>
     <row r="6" spans="1:10" ht="39.75" customHeight="1">
       <c r="A6" s="35" t="s">
@@ -44299,8 +44299,8 @@
   </sheetPr>
   <dimension ref="A1:M8"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="80" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -44340,11 +44340,11 @@
       <c r="M2" s="74"/>
     </row>
     <row r="4" spans="1:13" ht="20.25" customHeight="1">
-      <c r="A4" s="75" t="s">
+      <c r="A4" s="78" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="80"/>
-      <c r="C4" s="76"/>
+      <c r="B4" s="79"/>
+      <c r="C4" s="80"/>
       <c r="D4" s="81" t="s">
         <v>44</v>
       </c>

</xml_diff>

<commit_message>
updated templates with new text
git-svn-id: svn://107.170.10.188:8080/Semoss/trunk@2483 ef391c1c-ee15-45f7-b1d6-dde3d27a2169

Former-commit-id: d882b6aec2948c00b9961318cb712c435115719e
</commit_message>
<xml_diff>
--- a/export/Reports/Individual_System_LPI_Transition_Report_Template.xlsx
+++ b/export/Reports/Individual_System_LPI_Transition_Report_Template.xlsx
@@ -9,10 +9,10 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="1110" windowWidth="15120" windowHeight="6405" tabRatio="834" activeTab="8"/>
+    <workbookView xWindow="240" yWindow="1110" windowWidth="15120" windowHeight="6405" tabRatio="834" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Instructions" sheetId="32" r:id="rId1"/>
+    <sheet name="Instructions" sheetId="33" r:id="rId1"/>
     <sheet name="System Overview" sheetId="21" r:id="rId2"/>
     <sheet name="Software Lifecycles" sheetId="22" r:id="rId3"/>
     <sheet name="Hardware Lifecycles" sheetId="23" r:id="rId4"/>
@@ -34,6 +34,7 @@
     <externalReference r:id="rId18"/>
     <externalReference r:id="rId19"/>
     <externalReference r:id="rId20"/>
+    <externalReference r:id="rId21"/>
   </externalReferences>
   <definedNames>
     <definedName name="Additional">[1]Data!$D$3:$D$15</definedName>
@@ -76,8 +77,8 @@
     <definedName name="Portal_SUM">'[2]POM 2 Enabler - FY12'!$N$102</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">'System Overview'!$A$2:$M$11</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="7">'DHMSM Data Requirements'!$6:$6</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="3">'Hardware Lifecycles'!$7:$7</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="2">'Software Lifecycles'!$7:$7</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="3">'Hardware Lifecycles'!$9:$9</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="2">'Software Lifecycles'!$9:$9</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="6">'SOR Overlap With DHMSM'!$6:$6</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="5">'System Data'!$6:$6</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="8">'System Interfaces'!$6:$6</definedName>
@@ -111,7 +112,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="67">
   <si>
     <t>Garrison / Theater</t>
   </si>
@@ -218,32 +219,6 @@
     <t>This section displays data objects for which @SYSTEM@ is Source of Record (SOR) and which of those that DHMSM is also SOR for.</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">This section displays </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>@SYSTEM@</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> that are source of record for the data objects that DHMSM capabilities consume. </t>
-    </r>
-  </si>
-  <si>
     <t>System Name</t>
   </si>
   <si>
@@ -256,9 +231,6 @@
   </si>
   <si>
     <t>System Modernization Timeline</t>
-  </si>
-  <si>
-    <t>This section displays the cost to upgrade software and hardware that @SYSTEM@ uses as they retire.</t>
   </si>
   <si>
     <t>Software Cost</t>
@@ -361,7 +333,19 @@
     <t>NA</t>
   </si>
   <si>
-    <t>This section displays the data objects @SYSTEM@ is a source of record of and consumes and also shows the number of low probability systems that @SYSTEM@ provides the data object to. It also shows the other systems that are a source of the data object and the number of low probability systems they provide data for.</t>
+    <t>Software characteristics are based upon TAP data submissions provided by the DHA and Services program offices. Projected upgrade costs are based solely upon data provided to OTM.</t>
+  </si>
+  <si>
+    <t>Hardware characteristics are based upon TAP data submissions provided by the DHA and Services program offices. Projected upgrade costs are based solely upon data provided to OTM.</t>
+  </si>
+  <si>
+    <t>This section displays the cost to upgrade software and hardware that @SYSTEM@ uses as the modules reach end-of-life.</t>
+  </si>
+  <si>
+    <t>This section displays the data objects that @SYSTEM@ is a source of record of and the numbers of systems which DMHRSi sends the data to. Additionally, this section displays the data objects that @SYSTEM@ consumes, the other systems that are a source of the data object and the number of low probability systems they provide data for.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This section displays @SYSTEM@ that are source of record for the data objects that DHMSM capabilities consume. </t>
   </si>
 </sst>
 </file>
@@ -372,7 +356,7 @@
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="27">
+  <fonts count="26">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -509,14 +493,6 @@
       <color theme="1"/>
       <name val="Impact"/>
       <family val="2"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="9.5"/>
@@ -781,7 +757,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="84">
+  <cellXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -836,14 +812,14 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="22" fillId="0" borderId="1" xfId="49" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="21" fillId="0" borderId="1" xfId="49" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="23" fillId="0" borderId="1" xfId="49" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="22" fillId="0" borderId="1" xfId="49" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="10" fillId="0" borderId="1" xfId="49" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -855,12 +831,12 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="7" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -885,14 +861,26 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="6" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="6" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="6" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="6" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="6" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="6" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="4" borderId="5" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -912,12 +900,6 @@
     <xf numFmtId="0" fontId="17" fillId="4" borderId="10" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="4" borderId="3" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -929,12 +911,6 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="5" borderId="7" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1007,6 +983,15 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="51">
@@ -2078,6 +2063,35 @@
           </cell>
         </row>
       </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink12.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Instructions"/>
+      <sheetName val="System Overview"/>
+      <sheetName val="Software Lifecycles"/>
+      <sheetName val="Hardware Lifecycles"/>
+      <sheetName val="Modernization Timeline"/>
+      <sheetName val="System Data"/>
+      <sheetName val="SOR Overlap With DHMSM"/>
+      <sheetName val="DHMSM Data Requirements"/>
+      <sheetName val="System Interfaces"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -43318,12 +43332,12 @@
   <sheetData>
     <row r="1" spans="1:12" s="1" customFormat="1" ht="7.5" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="32.25" customHeight="1">
       <c r="A2" s="38" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B2" s="39"/>
       <c r="C2" s="39"/>
@@ -43339,12 +43353,12 @@
     </row>
     <row r="3" spans="1:12" s="1" customFormat="1" ht="7.5" customHeight="1">
       <c r="A3" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="281.25" customHeight="1">
       <c r="A4" s="40" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B4" s="41"/>
       <c r="C4" s="41"/>
@@ -43360,12 +43374,12 @@
     </row>
     <row r="5" spans="1:12" s="1" customFormat="1" ht="7.5" customHeight="1">
       <c r="A5" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:12" s="32" customFormat="1" ht="29.25" customHeight="1">
       <c r="A6" s="38" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B6" s="39"/>
       <c r="C6" s="39"/>
@@ -43381,12 +43395,12 @@
     </row>
     <row r="7" spans="1:12" s="1" customFormat="1" ht="7.5" customHeight="1">
       <c r="A7" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="134.25" customHeight="1">
       <c r="A8" s="43" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B8" s="44"/>
       <c r="C8" s="44"/>
@@ -43481,7 +43495,7 @@
   <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11:C11"/>
+      <selection activeCell="D7" sqref="D7:M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -43500,22 +43514,22 @@
     <row r="1" spans="1:13" ht="7.5" customHeight="1"/>
     <row r="2" spans="1:13" s="4" customFormat="1" ht="250.5" customHeight="1">
       <c r="A2" s="3"/>
-      <c r="B2" s="46" t="s">
+      <c r="B2" s="50" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" s="51"/>
+      <c r="D2" s="52" t="s">
         <v>37</v>
       </c>
-      <c r="C2" s="47"/>
-      <c r="D2" s="48" t="s">
-        <v>38</v>
-      </c>
-      <c r="E2" s="49"/>
-      <c r="F2" s="49"/>
-      <c r="G2" s="49"/>
-      <c r="H2" s="49"/>
-      <c r="I2" s="49"/>
-      <c r="J2" s="49"/>
-      <c r="K2" s="49"/>
-      <c r="L2" s="49"/>
-      <c r="M2" s="50"/>
+      <c r="E2" s="53"/>
+      <c r="F2" s="53"/>
+      <c r="G2" s="53"/>
+      <c r="H2" s="53"/>
+      <c r="I2" s="53"/>
+      <c r="J2" s="53"/>
+      <c r="K2" s="53"/>
+      <c r="L2" s="53"/>
+      <c r="M2" s="54"/>
     </row>
     <row r="3" spans="1:13" s="20" customFormat="1" ht="7.5" customHeight="1">
       <c r="A3" s="16"/>
@@ -43535,7 +43549,7 @@
     <row r="4" spans="1:13" ht="32.25" customHeight="1">
       <c r="A4" s="5"/>
       <c r="B4" s="38" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C4" s="39"/>
       <c r="D4" s="39"/>
@@ -43573,22 +43587,22 @@
     </row>
     <row r="7" spans="1:13" s="4" customFormat="1" ht="168.75" customHeight="1">
       <c r="A7" s="3"/>
-      <c r="B7" s="46" t="s">
+      <c r="B7" s="50" t="s">
         <v>30</v>
       </c>
-      <c r="C7" s="47"/>
-      <c r="D7" s="48" t="s">
-        <v>63</v>
+      <c r="C7" s="51"/>
+      <c r="D7" s="52" t="s">
+        <v>61</v>
       </c>
-      <c r="E7" s="49"/>
-      <c r="F7" s="49"/>
-      <c r="G7" s="49"/>
-      <c r="H7" s="49"/>
-      <c r="I7" s="49"/>
-      <c r="J7" s="49"/>
-      <c r="K7" s="49"/>
-      <c r="L7" s="49"/>
-      <c r="M7" s="50"/>
+      <c r="E7" s="53"/>
+      <c r="F7" s="53"/>
+      <c r="G7" s="53"/>
+      <c r="H7" s="53"/>
+      <c r="I7" s="53"/>
+      <c r="J7" s="53"/>
+      <c r="K7" s="53"/>
+      <c r="L7" s="53"/>
+      <c r="M7" s="54"/>
     </row>
     <row r="8" spans="1:13" ht="8.25" customHeight="1">
       <c r="A8" s="5"/>
@@ -43599,65 +43613,67 @@
     </row>
     <row r="9" spans="1:13" s="8" customFormat="1" ht="18" customHeight="1">
       <c r="A9" s="7"/>
-      <c r="B9" s="55" t="s">
+      <c r="B9" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="56"/>
-      <c r="D9" s="56"/>
-      <c r="E9" s="56"/>
-      <c r="F9" s="56"/>
-      <c r="G9" s="56"/>
-      <c r="H9" s="56"/>
-      <c r="I9" s="56"/>
-      <c r="J9" s="56"/>
-      <c r="K9" s="56"/>
-      <c r="L9" s="56"/>
-      <c r="M9" s="57"/>
+      <c r="C9" s="58"/>
+      <c r="D9" s="58"/>
+      <c r="E9" s="58"/>
+      <c r="F9" s="58"/>
+      <c r="G9" s="58"/>
+      <c r="H9" s="58"/>
+      <c r="I9" s="58"/>
+      <c r="J9" s="58"/>
+      <c r="K9" s="58"/>
+      <c r="L9" s="58"/>
+      <c r="M9" s="59"/>
     </row>
     <row r="10" spans="1:13" s="8" customFormat="1" ht="28.5" customHeight="1">
       <c r="A10" s="7"/>
-      <c r="B10" s="51" t="s">
+      <c r="B10" s="55" t="s">
         <v>0</v>
       </c>
-      <c r="C10" s="51"/>
-      <c r="D10" s="51" t="s">
+      <c r="C10" s="55"/>
+      <c r="D10" s="55" t="s">
         <v>5</v>
       </c>
-      <c r="E10" s="54"/>
-      <c r="F10" s="51" t="s">
+      <c r="E10" s="56"/>
+      <c r="F10" s="55" t="s">
+        <v>47</v>
+      </c>
+      <c r="G10" s="55"/>
+      <c r="H10" s="46" t="s">
+        <v>48</v>
+      </c>
+      <c r="I10" s="47"/>
+      <c r="J10" s="55" t="s">
         <v>49</v>
       </c>
-      <c r="G10" s="51"/>
-      <c r="H10" s="58" t="s">
-        <v>50</v>
-      </c>
-      <c r="I10" s="59"/>
-      <c r="J10" s="51" t="s">
-        <v>51</v>
-      </c>
-      <c r="K10" s="51"/>
-      <c r="L10" s="51" t="s">
+      <c r="K10" s="55"/>
+      <c r="L10" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="M10" s="51"/>
+      <c r="M10" s="55"/>
     </row>
     <row r="11" spans="1:13" ht="42.75" customHeight="1">
       <c r="A11" s="5"/>
-      <c r="B11" s="52"/>
-      <c r="C11" s="53"/>
-      <c r="D11" s="52"/>
-      <c r="E11" s="53"/>
-      <c r="F11" s="52"/>
-      <c r="G11" s="53"/>
-      <c r="H11" s="52"/>
-      <c r="I11" s="53"/>
-      <c r="J11" s="52"/>
-      <c r="K11" s="53"/>
-      <c r="L11" s="52"/>
-      <c r="M11" s="53"/>
+      <c r="B11" s="48"/>
+      <c r="C11" s="49"/>
+      <c r="D11" s="48"/>
+      <c r="E11" s="49"/>
+      <c r="F11" s="48"/>
+      <c r="G11" s="49"/>
+      <c r="H11" s="48"/>
+      <c r="I11" s="49"/>
+      <c r="J11" s="48"/>
+      <c r="K11" s="49"/>
+      <c r="L11" s="48"/>
+      <c r="M11" s="49"/>
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="B9:M9"/>
+    <mergeCell ref="B10:C10"/>
     <mergeCell ref="H10:I10"/>
     <mergeCell ref="B11:C11"/>
     <mergeCell ref="B2:C2"/>
@@ -43674,8 +43690,6 @@
     <mergeCell ref="D10:E10"/>
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="D7:M7"/>
-    <mergeCell ref="B9:M9"/>
-    <mergeCell ref="B10:C10"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -43688,10 +43702,10 @@
   <sheetPr>
     <tabColor rgb="FF366092"/>
   </sheetPr>
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5:G5"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -43708,7 +43722,7 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="18" customHeight="1">
@@ -43735,70 +43749,87 @@
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="18.75" customHeight="1">
-      <c r="A5" s="64" t="s">
-        <v>21</v>
+    <row r="5" spans="1:7" ht="25.5" customHeight="1">
+      <c r="A5" s="84" t="s">
+        <v>62</v>
       </c>
-      <c r="B5" s="65"/>
-      <c r="C5" s="61" t="s">
-        <v>55</v>
-      </c>
-      <c r="D5" s="62"/>
-      <c r="E5" s="62"/>
-      <c r="F5" s="62"/>
-      <c r="G5" s="63"/>
+      <c r="B5" s="85"/>
+      <c r="C5" s="85"/>
+      <c r="D5" s="85"/>
+      <c r="E5" s="85"/>
+      <c r="F5" s="85"/>
+      <c r="G5" s="86"/>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="25.5">
-      <c r="A7" s="35" t="s">
+    <row r="7" spans="1:7" ht="18.75" customHeight="1">
+      <c r="A7" s="64" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="65"/>
+      <c r="C7" s="61" t="s">
+        <v>53</v>
+      </c>
+      <c r="D7" s="62"/>
+      <c r="E7" s="62"/>
+      <c r="F7" s="62"/>
+      <c r="G7" s="63"/>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="25.5">
+      <c r="A9" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="35" t="s">
-        <v>52</v>
+      <c r="B9" s="35" t="s">
+        <v>50</v>
       </c>
-      <c r="C7" s="35" t="s">
+      <c r="C9" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="D7" s="35" t="s">
+      <c r="D9" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="E7" s="35" t="s">
+      <c r="E9" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="F7" s="35" t="s">
+      <c r="F9" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="G7" s="35" t="s">
+      <c r="G9" s="35" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
-      <c r="A8" s="23"/>
-      <c r="B8" s="14"/>
-      <c r="C8" s="14"/>
-      <c r="D8" s="28"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="29"/>
-      <c r="G8" s="28"/>
+    <row r="10" spans="1:7">
+      <c r="A10" s="23"/>
+      <c r="B10" s="14"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="28"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="29"/>
+      <c r="G10" s="28"/>
     </row>
-    <row r="9" spans="1:7">
-      <c r="A9" s="1" t="s">
-        <v>54</v>
+    <row r="11" spans="1:7">
+      <c r="A11" s="1" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="A2:G2"/>
-    <mergeCell ref="C5:G5"/>
-    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="A7:B7"/>
     <mergeCell ref="A3:G3"/>
+    <mergeCell ref="A5:G5"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup scale="89" orientation="portrait" r:id="rId1"/>
@@ -43811,10 +43842,10 @@
   <sheetPr>
     <tabColor rgb="FF366092"/>
   </sheetPr>
-  <dimension ref="A2:G8"/>
+  <dimension ref="A2:G10"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K25" sqref="K25"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -43851,57 +43882,69 @@
       <c r="F3" s="66"/>
       <c r="G3" s="66"/>
     </row>
-    <row r="5" spans="1:7" ht="18.75" customHeight="1">
-      <c r="A5" s="66" t="s">
+    <row r="5" spans="1:7" ht="25.5" customHeight="1">
+      <c r="A5" s="84" t="s">
+        <v>63</v>
+      </c>
+      <c r="B5" s="85"/>
+      <c r="C5" s="85"/>
+      <c r="D5" s="85"/>
+      <c r="E5" s="85"/>
+      <c r="F5" s="85"/>
+      <c r="G5" s="86"/>
+    </row>
+    <row r="7" spans="1:7" ht="18.75" customHeight="1">
+      <c r="A7" s="66" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="66"/>
-      <c r="C5" s="70" t="s">
-        <v>56</v>
+      <c r="B7" s="66"/>
+      <c r="C7" s="70" t="s">
+        <v>54</v>
       </c>
-      <c r="D5" s="70"/>
-      <c r="E5" s="70"/>
-      <c r="F5" s="70"/>
-      <c r="G5" s="70"/>
+      <c r="D7" s="70"/>
+      <c r="E7" s="70"/>
+      <c r="F7" s="70"/>
+      <c r="G7" s="70"/>
     </row>
-    <row r="7" spans="1:7" ht="25.5">
-      <c r="A7" s="35" t="s">
+    <row r="9" spans="1:7" ht="25.5">
+      <c r="A9" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="35" t="s">
-        <v>52</v>
+      <c r="B9" s="35" t="s">
+        <v>50</v>
       </c>
-      <c r="C7" s="35" t="s">
+      <c r="C9" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="D7" s="35" t="s">
+      <c r="D9" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="E7" s="35" t="s">
+      <c r="E9" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="F7" s="35" t="s">
+      <c r="F9" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="G7" s="35" t="s">
+      <c r="G9" s="35" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
-      <c r="A8" s="23"/>
-      <c r="B8" s="14"/>
-      <c r="C8" s="14"/>
-      <c r="D8" s="28"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="29"/>
-      <c r="G8" s="28"/>
+    <row r="10" spans="1:7">
+      <c r="A10" s="23"/>
+      <c r="B10" s="14"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="28"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="29"/>
+      <c r="G10" s="28"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="A3:G3"/>
     <mergeCell ref="A2:G2"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C5:G5"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="A5:G5"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup scale="89" orientation="portrait" r:id="rId1"/>
@@ -43916,20 +43959,20 @@
   </sheetPr>
   <dimension ref="A2:J11"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+    <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" style="1" customWidth="1"/>
-    <col min="2" max="10" width="12.85546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="9.7109375" style="1" customWidth="1"/>
+    <col min="2" max="10" width="12" style="1" customWidth="1"/>
     <col min="11" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:10" ht="18" customHeight="1">
       <c r="A2" s="74" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B2" s="74"/>
       <c r="C2" s="74"/>
@@ -43950,7 +43993,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="71" t="s">
-        <v>40</v>
+        <v>64</v>
       </c>
       <c r="C4" s="72"/>
       <c r="D4" s="72"/>
@@ -43991,12 +44034,12 @@
         <v>2022</v>
       </c>
       <c r="J6" s="35" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="41.25" customHeight="1">
       <c r="A7" s="35" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B7" s="24">
         <v>0</v>
@@ -44028,7 +44071,7 @@
     </row>
     <row r="8" spans="1:10" ht="41.25" customHeight="1">
       <c r="A8" s="35" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B8" s="24">
         <v>0</v>
@@ -44060,7 +44103,7 @@
     </row>
     <row r="10" spans="1:10" ht="41.25" customHeight="1">
       <c r="A10" s="35" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B10" s="25">
         <v>0</v>
@@ -44068,7 +44111,7 @@
     </row>
     <row r="11" spans="1:10" ht="41.25" customHeight="1">
       <c r="A11" s="35" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B11" s="25">
         <v>0</v>
@@ -44092,8 +44135,8 @@
   </sheetPr>
   <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="M23" sqref="M23"/>
+    <sheetView topLeftCell="A2" zoomScaleNormal="100" zoomScalePageLayoutView="80" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10" defaultRowHeight="12.75"/>
@@ -44124,7 +44167,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="75" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C4" s="76"/>
       <c r="D4" s="76"/>
@@ -44140,7 +44183,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="35" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -44166,7 +44209,7 @@
   <dimension ref="A2:B7"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -44178,7 +44221,7 @@
   <sheetData>
     <row r="2" spans="1:2" ht="18">
       <c r="A2" s="74" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B2" s="74"/>
     </row>
@@ -44186,7 +44229,7 @@
       <c r="A3" s="12"/>
       <c r="B3" s="12"/>
     </row>
-    <row r="4" spans="1:2" ht="50.25" customHeight="1">
+    <row r="4" spans="1:2" ht="55.5" customHeight="1">
       <c r="A4" s="13" t="s">
         <v>3</v>
       </c>
@@ -44228,7 +44271,7 @@
   <dimension ref="A2:C7"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:C4"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -44256,7 +44299,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="71" t="s">
-        <v>35</v>
+        <v>66</v>
       </c>
       <c r="C4" s="73"/>
     </row>
@@ -44273,7 +44316,7 @@
         <v>6</v>
       </c>
       <c r="C6" s="35" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -44299,8 +44342,8 @@
   </sheetPr>
   <dimension ref="A1:M8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+    <sheetView topLeftCell="C1" zoomScaleNormal="100" zoomScalePageLayoutView="80" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -44346,7 +44389,7 @@
       <c r="B4" s="79"/>
       <c r="C4" s="80"/>
       <c r="D4" s="81" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E4" s="82"/>
       <c r="F4" s="82"/>
@@ -44393,10 +44436,10 @@
         <v>15</v>
       </c>
       <c r="L6" s="36" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="M6" s="36" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:13">

</xml_diff>

<commit_message>
Updated formatting for Modernization Timeline and System Data tabs.
git-svn-id: svn://107.170.10.188:8080/Semoss/trunk@2484 ef391c1c-ee15-45f7-b1d6-dde3d27a2169

Former-commit-id: cce86696dd3120632e23bffbec47e4c988400a1e
</commit_message>
<xml_diff>
--- a/export/Reports/Individual_System_LPI_Transition_Report_Template.xlsx
+++ b/export/Reports/Individual_System_LPI_Transition_Report_Template.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ksmart\workspace64bitNew\SEMOSS_2014\export\Reports\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="1110" windowWidth="15120" windowHeight="6405" tabRatio="834" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="1110" windowWidth="15120" windowHeight="6405" tabRatio="834" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="33" r:id="rId1"/>
@@ -34,7 +29,6 @@
     <externalReference r:id="rId18"/>
     <externalReference r:id="rId19"/>
     <externalReference r:id="rId20"/>
-    <externalReference r:id="rId21"/>
   </externalReferences>
   <definedNames>
     <definedName name="Additional">[1]Data!$D$3:$D$15</definedName>
@@ -870,6 +864,18 @@
     <xf numFmtId="0" fontId="25" fillId="6" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="5" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="6" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="7" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="10" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -897,20 +903,8 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="10" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="4" borderId="3" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="5" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="6" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="7" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -932,6 +926,15 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -983,15 +986,6 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="51">
@@ -2068,35 +2062,6 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink12.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Instructions"/>
-      <sheetName val="System Overview"/>
-      <sheetName val="Software Lifecycles"/>
-      <sheetName val="Hardware Lifecycles"/>
-      <sheetName val="Modernization Timeline"/>
-      <sheetName val="System Data"/>
-      <sheetName val="SOR Overlap With DHMSM"/>
-      <sheetName val="DHMSM Data Requirements"/>
-      <sheetName val="System Interfaces"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
-      <sheetData sheetId="8"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
 <file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
@@ -43069,7 +43034,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -43104,7 +43069,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -43514,22 +43479,22 @@
     <row r="1" spans="1:13" ht="7.5" customHeight="1"/>
     <row r="2" spans="1:13" s="4" customFormat="1" ht="250.5" customHeight="1">
       <c r="A2" s="3"/>
-      <c r="B2" s="50" t="s">
+      <c r="B2" s="54" t="s">
         <v>36</v>
       </c>
-      <c r="C2" s="51"/>
-      <c r="D2" s="52" t="s">
+      <c r="C2" s="55"/>
+      <c r="D2" s="56" t="s">
         <v>37</v>
       </c>
-      <c r="E2" s="53"/>
-      <c r="F2" s="53"/>
-      <c r="G2" s="53"/>
-      <c r="H2" s="53"/>
-      <c r="I2" s="53"/>
-      <c r="J2" s="53"/>
-      <c r="K2" s="53"/>
-      <c r="L2" s="53"/>
-      <c r="M2" s="54"/>
+      <c r="E2" s="57"/>
+      <c r="F2" s="57"/>
+      <c r="G2" s="57"/>
+      <c r="H2" s="57"/>
+      <c r="I2" s="57"/>
+      <c r="J2" s="57"/>
+      <c r="K2" s="57"/>
+      <c r="L2" s="57"/>
+      <c r="M2" s="58"/>
     </row>
     <row r="3" spans="1:13" s="20" customFormat="1" ht="7.5" customHeight="1">
       <c r="A3" s="16"/>
@@ -43587,22 +43552,22 @@
     </row>
     <row r="7" spans="1:13" s="4" customFormat="1" ht="168.75" customHeight="1">
       <c r="A7" s="3"/>
-      <c r="B7" s="50" t="s">
+      <c r="B7" s="54" t="s">
         <v>30</v>
       </c>
-      <c r="C7" s="51"/>
-      <c r="D7" s="52" t="s">
+      <c r="C7" s="55"/>
+      <c r="D7" s="56" t="s">
         <v>61</v>
       </c>
-      <c r="E7" s="53"/>
-      <c r="F7" s="53"/>
-      <c r="G7" s="53"/>
-      <c r="H7" s="53"/>
-      <c r="I7" s="53"/>
-      <c r="J7" s="53"/>
-      <c r="K7" s="53"/>
-      <c r="L7" s="53"/>
-      <c r="M7" s="54"/>
+      <c r="E7" s="57"/>
+      <c r="F7" s="57"/>
+      <c r="G7" s="57"/>
+      <c r="H7" s="57"/>
+      <c r="I7" s="57"/>
+      <c r="J7" s="57"/>
+      <c r="K7" s="57"/>
+      <c r="L7" s="57"/>
+      <c r="M7" s="58"/>
     </row>
     <row r="8" spans="1:13" ht="8.25" customHeight="1">
       <c r="A8" s="5"/>
@@ -43613,65 +43578,67 @@
     </row>
     <row r="9" spans="1:13" s="8" customFormat="1" ht="18" customHeight="1">
       <c r="A9" s="7"/>
-      <c r="B9" s="57" t="s">
+      <c r="B9" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="58"/>
-      <c r="D9" s="58"/>
-      <c r="E9" s="58"/>
-      <c r="F9" s="58"/>
-      <c r="G9" s="58"/>
-      <c r="H9" s="58"/>
-      <c r="I9" s="58"/>
-      <c r="J9" s="58"/>
-      <c r="K9" s="58"/>
-      <c r="L9" s="58"/>
-      <c r="M9" s="59"/>
+      <c r="C9" s="47"/>
+      <c r="D9" s="47"/>
+      <c r="E9" s="47"/>
+      <c r="F9" s="47"/>
+      <c r="G9" s="47"/>
+      <c r="H9" s="47"/>
+      <c r="I9" s="47"/>
+      <c r="J9" s="47"/>
+      <c r="K9" s="47"/>
+      <c r="L9" s="47"/>
+      <c r="M9" s="48"/>
     </row>
     <row r="10" spans="1:13" s="8" customFormat="1" ht="28.5" customHeight="1">
       <c r="A10" s="7"/>
-      <c r="B10" s="55" t="s">
+      <c r="B10" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="C10" s="55"/>
-      <c r="D10" s="55" t="s">
+      <c r="C10" s="49"/>
+      <c r="D10" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="E10" s="56"/>
-      <c r="F10" s="55" t="s">
+      <c r="E10" s="59"/>
+      <c r="F10" s="49" t="s">
         <v>47</v>
       </c>
-      <c r="G10" s="55"/>
-      <c r="H10" s="46" t="s">
+      <c r="G10" s="49"/>
+      <c r="H10" s="50" t="s">
         <v>48</v>
       </c>
-      <c r="I10" s="47"/>
-      <c r="J10" s="55" t="s">
+      <c r="I10" s="51"/>
+      <c r="J10" s="49" t="s">
         <v>49</v>
       </c>
-      <c r="K10" s="55"/>
-      <c r="L10" s="55" t="s">
+      <c r="K10" s="49"/>
+      <c r="L10" s="49" t="s">
         <v>1</v>
       </c>
-      <c r="M10" s="55"/>
+      <c r="M10" s="49"/>
     </row>
     <row r="11" spans="1:13" ht="42.75" customHeight="1">
       <c r="A11" s="5"/>
-      <c r="B11" s="48"/>
-      <c r="C11" s="49"/>
-      <c r="D11" s="48"/>
-      <c r="E11" s="49"/>
-      <c r="F11" s="48"/>
-      <c r="G11" s="49"/>
-      <c r="H11" s="48"/>
-      <c r="I11" s="49"/>
-      <c r="J11" s="48"/>
-      <c r="K11" s="49"/>
-      <c r="L11" s="48"/>
-      <c r="M11" s="49"/>
+      <c r="B11" s="52"/>
+      <c r="C11" s="53"/>
+      <c r="D11" s="52"/>
+      <c r="E11" s="53"/>
+      <c r="F11" s="52"/>
+      <c r="G11" s="53"/>
+      <c r="H11" s="52"/>
+      <c r="I11" s="53"/>
+      <c r="J11" s="52"/>
+      <c r="K11" s="53"/>
+      <c r="L11" s="52"/>
+      <c r="M11" s="53"/>
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:M7"/>
     <mergeCell ref="B9:M9"/>
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="H10:I10"/>
@@ -43688,8 +43655,6 @@
     <mergeCell ref="L11:M11"/>
     <mergeCell ref="J10:K10"/>
     <mergeCell ref="D10:E10"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:M7"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -43704,7 +43669,7 @@
   </sheetPr>
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
@@ -43753,15 +43718,15 @@
       </c>
     </row>
     <row r="5" spans="1:7" ht="25.5" customHeight="1">
-      <c r="A5" s="84" t="s">
+      <c r="A5" s="67" t="s">
         <v>62</v>
       </c>
-      <c r="B5" s="85"/>
-      <c r="C5" s="85"/>
-      <c r="D5" s="85"/>
-      <c r="E5" s="85"/>
-      <c r="F5" s="85"/>
-      <c r="G5" s="86"/>
+      <c r="B5" s="68"/>
+      <c r="C5" s="68"/>
+      <c r="D5" s="68"/>
+      <c r="E5" s="68"/>
+      <c r="F5" s="68"/>
+      <c r="G5" s="69"/>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="1" t="s">
@@ -43861,15 +43826,15 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:7" ht="18" customHeight="1">
-      <c r="A2" s="67" t="s">
+      <c r="A2" s="70" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="68"/>
-      <c r="C2" s="68"/>
-      <c r="D2" s="68"/>
-      <c r="E2" s="68"/>
-      <c r="F2" s="68"/>
-      <c r="G2" s="69"/>
+      <c r="B2" s="71"/>
+      <c r="C2" s="71"/>
+      <c r="D2" s="71"/>
+      <c r="E2" s="71"/>
+      <c r="F2" s="71"/>
+      <c r="G2" s="72"/>
     </row>
     <row r="3" spans="1:7" ht="18" customHeight="1">
       <c r="A3" s="66" t="s">
@@ -43883,28 +43848,28 @@
       <c r="G3" s="66"/>
     </row>
     <row r="5" spans="1:7" ht="25.5" customHeight="1">
-      <c r="A5" s="84" t="s">
+      <c r="A5" s="67" t="s">
         <v>63</v>
       </c>
-      <c r="B5" s="85"/>
-      <c r="C5" s="85"/>
-      <c r="D5" s="85"/>
-      <c r="E5" s="85"/>
-      <c r="F5" s="85"/>
-      <c r="G5" s="86"/>
+      <c r="B5" s="68"/>
+      <c r="C5" s="68"/>
+      <c r="D5" s="68"/>
+      <c r="E5" s="68"/>
+      <c r="F5" s="68"/>
+      <c r="G5" s="69"/>
     </row>
     <row r="7" spans="1:7" ht="18.75" customHeight="1">
       <c r="A7" s="66" t="s">
         <v>21</v>
       </c>
       <c r="B7" s="66"/>
-      <c r="C7" s="70" t="s">
+      <c r="C7" s="73" t="s">
         <v>54</v>
       </c>
-      <c r="D7" s="70"/>
-      <c r="E7" s="70"/>
-      <c r="F7" s="70"/>
-      <c r="G7" s="70"/>
+      <c r="D7" s="73"/>
+      <c r="E7" s="73"/>
+      <c r="F7" s="73"/>
+      <c r="G7" s="73"/>
     </row>
     <row r="9" spans="1:7" ht="25.5">
       <c r="A9" s="35" t="s">
@@ -43956,6 +43921,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF366092"/>
+    <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A2:J11"/>
   <sheetViews>
@@ -43971,18 +43937,18 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:10" ht="18" customHeight="1">
-      <c r="A2" s="74" t="s">
+      <c r="A2" s="77" t="s">
         <v>38</v>
       </c>
-      <c r="B2" s="74"/>
-      <c r="C2" s="74"/>
-      <c r="D2" s="74"/>
-      <c r="E2" s="74"/>
-      <c r="F2" s="74"/>
-      <c r="G2" s="74"/>
-      <c r="H2" s="74"/>
-      <c r="I2" s="74"/>
-      <c r="J2" s="74"/>
+      <c r="B2" s="77"/>
+      <c r="C2" s="77"/>
+      <c r="D2" s="77"/>
+      <c r="E2" s="77"/>
+      <c r="F2" s="77"/>
+      <c r="G2" s="77"/>
+      <c r="H2" s="77"/>
+      <c r="I2" s="77"/>
+      <c r="J2" s="77"/>
     </row>
     <row r="3" spans="1:10" ht="18">
       <c r="A3" s="12"/>
@@ -43992,17 +43958,17 @@
       <c r="A4" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="71" t="s">
+      <c r="B4" s="74" t="s">
         <v>64</v>
       </c>
-      <c r="C4" s="72"/>
-      <c r="D4" s="72"/>
-      <c r="E4" s="72"/>
-      <c r="F4" s="72"/>
-      <c r="G4" s="72"/>
-      <c r="H4" s="72"/>
-      <c r="I4" s="72"/>
-      <c r="J4" s="73"/>
+      <c r="C4" s="75"/>
+      <c r="D4" s="75"/>
+      <c r="E4" s="75"/>
+      <c r="F4" s="75"/>
+      <c r="G4" s="75"/>
+      <c r="H4" s="75"/>
+      <c r="I4" s="75"/>
+      <c r="J4" s="76"/>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="2"/>
@@ -44123,7 +44089,7 @@
     <mergeCell ref="A2:J2"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup scale="75" orientation="portrait" r:id="rId1"/>
+  <pageSetup scale="75" fitToHeight="0" orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
@@ -44132,10 +44098,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF366092"/>
+    <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScaleNormal="100" zoomScalePageLayoutView="80" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" zoomScalePageLayoutView="80" workbookViewId="0">
       <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
@@ -44149,34 +44116,34 @@
   <sheetData>
     <row r="1" spans="1:10" ht="18" customHeight="1"/>
     <row r="2" spans="1:10" ht="18" customHeight="1">
-      <c r="A2" s="74" t="s">
+      <c r="A2" s="77" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="74"/>
-      <c r="C2" s="74"/>
-      <c r="D2" s="74"/>
-      <c r="E2" s="74"/>
-      <c r="F2" s="74"/>
-      <c r="G2" s="74"/>
-      <c r="H2" s="74"/>
-      <c r="I2" s="74"/>
-      <c r="J2" s="74"/>
+      <c r="B2" s="77"/>
+      <c r="C2" s="77"/>
+      <c r="D2" s="77"/>
+      <c r="E2" s="77"/>
+      <c r="F2" s="77"/>
+      <c r="G2" s="77"/>
+      <c r="H2" s="77"/>
+      <c r="I2" s="77"/>
+      <c r="J2" s="77"/>
     </row>
     <row r="4" spans="1:10" ht="53.25" customHeight="1">
       <c r="A4" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="75" t="s">
+      <c r="B4" s="78" t="s">
         <v>65</v>
       </c>
-      <c r="C4" s="76"/>
-      <c r="D4" s="76"/>
-      <c r="E4" s="76"/>
-      <c r="F4" s="76"/>
-      <c r="G4" s="76"/>
-      <c r="H4" s="76"/>
-      <c r="I4" s="76"/>
-      <c r="J4" s="77"/>
+      <c r="C4" s="79"/>
+      <c r="D4" s="79"/>
+      <c r="E4" s="79"/>
+      <c r="F4" s="79"/>
+      <c r="G4" s="79"/>
+      <c r="H4" s="79"/>
+      <c r="I4" s="79"/>
+      <c r="J4" s="80"/>
     </row>
     <row r="6" spans="1:10" ht="39.75" customHeight="1">
       <c r="A6" s="35" t="s">
@@ -44196,7 +44163,7 @@
     <mergeCell ref="B4:J4"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup scale="48" orientation="landscape" r:id="rId1"/>
+  <pageSetup fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
@@ -44220,10 +44187,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:2" ht="18">
-      <c r="A2" s="74" t="s">
+      <c r="A2" s="77" t="s">
         <v>57</v>
       </c>
-      <c r="B2" s="74"/>
+      <c r="B2" s="77"/>
     </row>
     <row r="3" spans="1:2" ht="18">
       <c r="A3" s="12"/>
@@ -44283,11 +44250,11 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:3" ht="18">
-      <c r="A2" s="74" t="s">
+      <c r="A2" s="77" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="74"/>
-      <c r="C2" s="74"/>
+      <c r="B2" s="77"/>
+      <c r="C2" s="77"/>
     </row>
     <row r="3" spans="1:3" ht="18">
       <c r="A3" s="12"/>
@@ -44298,10 +44265,10 @@
       <c r="A4" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="71" t="s">
+      <c r="B4" s="74" t="s">
         <v>66</v>
       </c>
-      <c r="C4" s="73"/>
+      <c r="C4" s="76"/>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="2"/>
@@ -44366,40 +44333,40 @@
   <sheetData>
     <row r="1" spans="1:13" ht="18" customHeight="1"/>
     <row r="2" spans="1:13" ht="18" customHeight="1">
-      <c r="A2" s="74" t="s">
+      <c r="A2" s="77" t="s">
         <v>33</v>
       </c>
-      <c r="B2" s="74"/>
-      <c r="C2" s="74"/>
-      <c r="D2" s="74"/>
-      <c r="E2" s="74"/>
-      <c r="F2" s="74"/>
-      <c r="G2" s="74"/>
-      <c r="H2" s="74"/>
-      <c r="I2" s="74"/>
-      <c r="J2" s="74"/>
-      <c r="K2" s="74"/>
-      <c r="L2" s="74"/>
-      <c r="M2" s="74"/>
+      <c r="B2" s="77"/>
+      <c r="C2" s="77"/>
+      <c r="D2" s="77"/>
+      <c r="E2" s="77"/>
+      <c r="F2" s="77"/>
+      <c r="G2" s="77"/>
+      <c r="H2" s="77"/>
+      <c r="I2" s="77"/>
+      <c r="J2" s="77"/>
+      <c r="K2" s="77"/>
+      <c r="L2" s="77"/>
+      <c r="M2" s="77"/>
     </row>
     <row r="4" spans="1:13" ht="20.25" customHeight="1">
-      <c r="A4" s="78" t="s">
+      <c r="A4" s="81" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="79"/>
-      <c r="C4" s="80"/>
-      <c r="D4" s="81" t="s">
+      <c r="B4" s="82"/>
+      <c r="C4" s="83"/>
+      <c r="D4" s="84" t="s">
         <v>42</v>
       </c>
-      <c r="E4" s="82"/>
-      <c r="F4" s="82"/>
-      <c r="G4" s="82"/>
-      <c r="H4" s="82"/>
-      <c r="I4" s="82"/>
-      <c r="J4" s="82"/>
-      <c r="K4" s="82"/>
-      <c r="L4" s="82"/>
-      <c r="M4" s="83"/>
+      <c r="E4" s="85"/>
+      <c r="F4" s="85"/>
+      <c r="G4" s="85"/>
+      <c r="H4" s="85"/>
+      <c r="I4" s="85"/>
+      <c r="J4" s="85"/>
+      <c r="K4" s="85"/>
+      <c r="L4" s="85"/>
+      <c r="M4" s="86"/>
     </row>
     <row r="6" spans="1:13" ht="39.75" customHeight="1">
       <c r="A6" s="35" t="s">

</xml_diff>

<commit_message>
changed definition of High = High and question, and low= low and medium and medium-high
git-svn-id: svn://107.170.10.188:8080/Semoss/trunk@2486 ef391c1c-ee15-45f7-b1d6-dde3d27a2169
</commit_message>
<xml_diff>
--- a/export/Reports/Individual_System_LPI_Transition_Report_Template.xlsx
+++ b/export/Reports/Individual_System_LPI_Transition_Report_Template.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ksmart\workspace64bitNew\SEMOSS_2014\export\Reports\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="1110" windowWidth="15120" windowHeight="6405" tabRatio="834" activeTab="5"/>
   </bookViews>
@@ -864,6 +869,21 @@
     <xf numFmtId="0" fontId="25" fillId="6" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="5" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="7" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="5" borderId="5" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -887,21 +907,6 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="5" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="7" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="4" borderId="3" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -43034,7 +43039,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -43069,7 +43074,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -43479,22 +43484,22 @@
     <row r="1" spans="1:13" ht="7.5" customHeight="1"/>
     <row r="2" spans="1:13" s="4" customFormat="1" ht="250.5" customHeight="1">
       <c r="A2" s="3"/>
-      <c r="B2" s="54" t="s">
+      <c r="B2" s="46" t="s">
         <v>36</v>
       </c>
-      <c r="C2" s="55"/>
-      <c r="D2" s="56" t="s">
+      <c r="C2" s="47"/>
+      <c r="D2" s="48" t="s">
         <v>37</v>
       </c>
-      <c r="E2" s="57"/>
-      <c r="F2" s="57"/>
-      <c r="G2" s="57"/>
-      <c r="H2" s="57"/>
-      <c r="I2" s="57"/>
-      <c r="J2" s="57"/>
-      <c r="K2" s="57"/>
-      <c r="L2" s="57"/>
-      <c r="M2" s="58"/>
+      <c r="E2" s="49"/>
+      <c r="F2" s="49"/>
+      <c r="G2" s="49"/>
+      <c r="H2" s="49"/>
+      <c r="I2" s="49"/>
+      <c r="J2" s="49"/>
+      <c r="K2" s="49"/>
+      <c r="L2" s="49"/>
+      <c r="M2" s="50"/>
     </row>
     <row r="3" spans="1:13" s="20" customFormat="1" ht="7.5" customHeight="1">
       <c r="A3" s="16"/>
@@ -43552,22 +43557,22 @@
     </row>
     <row r="7" spans="1:13" s="4" customFormat="1" ht="168.75" customHeight="1">
       <c r="A7" s="3"/>
-      <c r="B7" s="54" t="s">
+      <c r="B7" s="46" t="s">
         <v>30</v>
       </c>
-      <c r="C7" s="55"/>
-      <c r="D7" s="56" t="s">
+      <c r="C7" s="47"/>
+      <c r="D7" s="48" t="s">
         <v>61</v>
       </c>
-      <c r="E7" s="57"/>
-      <c r="F7" s="57"/>
-      <c r="G7" s="57"/>
-      <c r="H7" s="57"/>
-      <c r="I7" s="57"/>
-      <c r="J7" s="57"/>
-      <c r="K7" s="57"/>
-      <c r="L7" s="57"/>
-      <c r="M7" s="58"/>
+      <c r="E7" s="49"/>
+      <c r="F7" s="49"/>
+      <c r="G7" s="49"/>
+      <c r="H7" s="49"/>
+      <c r="I7" s="49"/>
+      <c r="J7" s="49"/>
+      <c r="K7" s="49"/>
+      <c r="L7" s="49"/>
+      <c r="M7" s="50"/>
     </row>
     <row r="8" spans="1:13" ht="8.25" customHeight="1">
       <c r="A8" s="5"/>
@@ -43578,70 +43583,65 @@
     </row>
     <row r="9" spans="1:13" s="8" customFormat="1" ht="18" customHeight="1">
       <c r="A9" s="7"/>
-      <c r="B9" s="46" t="s">
+      <c r="B9" s="51" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="47"/>
-      <c r="D9" s="47"/>
-      <c r="E9" s="47"/>
-      <c r="F9" s="47"/>
-      <c r="G9" s="47"/>
-      <c r="H9" s="47"/>
-      <c r="I9" s="47"/>
-      <c r="J9" s="47"/>
-      <c r="K9" s="47"/>
-      <c r="L9" s="47"/>
-      <c r="M9" s="48"/>
+      <c r="C9" s="52"/>
+      <c r="D9" s="52"/>
+      <c r="E9" s="52"/>
+      <c r="F9" s="52"/>
+      <c r="G9" s="52"/>
+      <c r="H9" s="52"/>
+      <c r="I9" s="52"/>
+      <c r="J9" s="52"/>
+      <c r="K9" s="52"/>
+      <c r="L9" s="52"/>
+      <c r="M9" s="53"/>
     </row>
     <row r="10" spans="1:13" s="8" customFormat="1" ht="28.5" customHeight="1">
       <c r="A10" s="7"/>
-      <c r="B10" s="49" t="s">
+      <c r="B10" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="C10" s="49"/>
-      <c r="D10" s="49" t="s">
+      <c r="C10" s="54"/>
+      <c r="D10" s="54" t="s">
         <v>5</v>
       </c>
       <c r="E10" s="59"/>
-      <c r="F10" s="49" t="s">
+      <c r="F10" s="54" t="s">
         <v>47</v>
       </c>
-      <c r="G10" s="49"/>
-      <c r="H10" s="50" t="s">
+      <c r="G10" s="54"/>
+      <c r="H10" s="55" t="s">
         <v>48</v>
       </c>
-      <c r="I10" s="51"/>
-      <c r="J10" s="49" t="s">
+      <c r="I10" s="56"/>
+      <c r="J10" s="54" t="s">
         <v>49</v>
       </c>
-      <c r="K10" s="49"/>
-      <c r="L10" s="49" t="s">
+      <c r="K10" s="54"/>
+      <c r="L10" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="M10" s="49"/>
+      <c r="M10" s="54"/>
     </row>
     <row r="11" spans="1:13" ht="42.75" customHeight="1">
       <c r="A11" s="5"/>
-      <c r="B11" s="52"/>
-      <c r="C11" s="53"/>
-      <c r="D11" s="52"/>
-      <c r="E11" s="53"/>
-      <c r="F11" s="52"/>
-      <c r="G11" s="53"/>
-      <c r="H11" s="52"/>
-      <c r="I11" s="53"/>
-      <c r="J11" s="52"/>
-      <c r="K11" s="53"/>
-      <c r="L11" s="52"/>
-      <c r="M11" s="53"/>
+      <c r="B11" s="57"/>
+      <c r="C11" s="58"/>
+      <c r="D11" s="57"/>
+      <c r="E11" s="58"/>
+      <c r="F11" s="57"/>
+      <c r="G11" s="58"/>
+      <c r="H11" s="57"/>
+      <c r="I11" s="58"/>
+      <c r="J11" s="57"/>
+      <c r="K11" s="58"/>
+      <c r="L11" s="57"/>
+      <c r="M11" s="58"/>
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:M7"/>
-    <mergeCell ref="B9:M9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="H10:I10"/>
     <mergeCell ref="B11:C11"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B4:M4"/>
@@ -43655,6 +43655,11 @@
     <mergeCell ref="L11:M11"/>
     <mergeCell ref="J10:K10"/>
     <mergeCell ref="D10:E10"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:M7"/>
+    <mergeCell ref="B9:M9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="H10:I10"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -43926,13 +43931,13 @@
   <dimension ref="A2:J11"/>
   <sheetViews>
     <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="9.7109375" style="1" customWidth="1"/>
-    <col min="2" max="10" width="12" style="1" customWidth="1"/>
+    <col min="2" max="10" width="12.85546875" style="1" customWidth="1"/>
     <col min="11" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
@@ -44089,7 +44094,7 @@
     <mergeCell ref="A2:J2"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup scale="75" fitToHeight="0" orientation="portrait" r:id="rId1"/>
+  <pageSetup scale="96" fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
@@ -44103,7 +44108,7 @@
   <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10" defaultRowHeight="12.75"/>

</xml_diff>

<commit_message>
updated LPI and LPNI reports to include bar charts
git-svn-id: svn://107.170.10.188:8080/Semoss/trunk@2522 ef391c1c-ee15-45f7-b1d6-dde3d27a2169

Former-commit-id: 9b8abd64367352abb4ce957c14869a04db799c97
</commit_message>
<xml_diff>
--- a/export/Reports/Individual_System_LPI_Transition_Report_Template.xlsx
+++ b/export/Reports/Individual_System_LPI_Transition_Report_Template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="1110" windowWidth="15120" windowHeight="6405" tabRatio="834" activeTab="5"/>
+    <workbookView xWindow="240" yWindow="1110" windowWidth="15120" windowHeight="6405" tabRatio="834"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="33" r:id="rId1"/>
@@ -21,9 +21,9 @@
     <sheet name="SOR Overlap With DHMSM" sheetId="28" r:id="rId7"/>
     <sheet name="DHMSM Data Requirements" sheetId="26" r:id="rId8"/>
     <sheet name="System Interfaces" sheetId="27" r:id="rId9"/>
+    <sheet name="Summary Charts" sheetId="34" r:id="rId10"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId10"/>
     <externalReference r:id="rId11"/>
     <externalReference r:id="rId12"/>
     <externalReference r:id="rId13"/>
@@ -34,6 +34,7 @@
     <externalReference r:id="rId18"/>
     <externalReference r:id="rId19"/>
     <externalReference r:id="rId20"/>
+    <externalReference r:id="rId21"/>
   </externalReferences>
   <definedNames>
     <definedName name="Additional">[1]Data!$D$3:$D$15</definedName>
@@ -111,7 +112,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="85">
   <si>
     <t>Garrison / Theater</t>
   </si>
@@ -346,6 +347,60 @@
   <si>
     <t xml:space="preserve">This section displays @SYSTEM@ that are source of record for the data objects that DHMSM capabilities consume. </t>
   </si>
+  <si>
+    <t>System Maturity</t>
+  </si>
+  <si>
+    <t>Software Maturity</t>
+  </si>
+  <si>
+    <t>Hardware Maturity</t>
+  </si>
+  <si>
+    <t>Software Lifecycle</t>
+  </si>
+  <si>
+    <t>Count</t>
+  </si>
+  <si>
+    <t>Retired (Not Supported)</t>
+  </si>
+  <si>
+    <t>Supported</t>
+  </si>
+  <si>
+    <t>GA (Generally Available)</t>
+  </si>
+  <si>
+    <t>TBD</t>
+  </si>
+  <si>
+    <t>Hardware Lifecycle</t>
+  </si>
+  <si>
+    <t>Interfaces Summary</t>
+  </si>
+  <si>
+    <t>Required Direct Interfaces with DHMSM - Legacy Provider</t>
+  </si>
+  <si>
+    <t>Required Direct Interfaces with DHMSM - Legacy Consumer</t>
+  </si>
+  <si>
+    <t>Existing Legacy Interfaces Required to Endure</t>
+  </si>
+  <si>
+    <t>Existing Legacy Interfaces Recommended for Removal</t>
+  </si>
+  <si>
+    <t>Proposed Future Interfaces with DHMSM - Legacy Provider</t>
+  </si>
+  <si>
+    <t>The following graph illustrates the number of interfaces @SYSTEM@ will have in the future state based upon the business rules established for each interface type.</t>
+  </si>
+  <si>
+    <t>The following graphs provide an overview of the hardware and software maturity for @SYSTEM@, illustrating the number of software and hardware products in each lifecycle phase.</t>
+  </si>
 </sst>
 </file>
 
@@ -355,7 +410,7 @@
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="26">
+  <fonts count="27">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -524,6 +579,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="8">
     <fill>
@@ -569,7 +631,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -693,6 +755,35 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -756,7 +847,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="87">
+  <cellXfs count="109">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -845,6 +936,19 @@
     <xf numFmtId="0" fontId="18" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="48" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" xfId="48" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="48" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" xfId="48" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="48" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="12" xfId="48" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="48" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" xfId="48" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="13" xfId="48" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="7" borderId="5" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -869,11 +973,32 @@
     <xf numFmtId="0" fontId="25" fillId="6" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="5" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="5" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="7" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="6" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="7" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="48" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="48" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="48" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -884,14 +1009,14 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="5" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="5" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="6" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="6" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="7" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="7" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="4" borderId="10" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -907,6 +1032,12 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="5" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="7" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="4" borderId="3" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1062,6 +1193,798 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FFC000"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FFFF00"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Summary Charts'!$A$4:$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Retired (Not Supported)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Supported</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>GA (Generally Available)</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>TBD</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Summary Charts'!$B$4:$B$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FFC000"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FFFF00"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Summary Charts'!$A$4:$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Retired (Not Supported)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Supported</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>GA (Generally Available)</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>TBD</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Summary Charts'!$B$4:$B$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="457379368"/>
+        <c:axId val="457379760"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="457379368"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="457379760"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="457379760"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="457379368"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FFC000"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FFFF00"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Summary Charts'!$A$12:$A$15</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Retired (Not Supported)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Supported</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>GA (Generally Available)</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>TBD</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Summary Charts'!$B$12:$B$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="457380936"/>
+        <c:axId val="457381328"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="457380936"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="457381328"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="457381328"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="457380936"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Summary Charts'!$A$20</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Required Direct Interfaces with DHMSM - Legacy Provider</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Summary Charts'!$B$19</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Count</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Summary Charts'!$B$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Summary Charts'!$A$21</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Required Direct Interfaces with DHMSM - Legacy Consumer</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Summary Charts'!$B$19</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Count</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Summary Charts'!$B$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Summary Charts'!$A$22</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Existing Legacy Interfaces Required to Endure</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Summary Charts'!$B$19</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Count</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Summary Charts'!$B$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Summary Charts'!$A$23</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Existing Legacy Interfaces Recommended for Removal</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Summary Charts'!$B$19</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Count</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Summary Charts'!$B$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Summary Charts'!$A$24</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Proposed Future Interfaces with DHMSM - Legacy Provider</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Summary Charts'!$B$19</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Count</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Summary Charts'!$B$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="414560496"/>
+        <c:axId val="414560104"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="414560496"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="414560104"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="414560104"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="414560496"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>107155</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>134541</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>488157</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>20241</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>83344</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>134540</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>428625</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>20240</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>59532</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>63102</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>428626</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>130968</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -43288,8 +44211,8 @@
   </sheetPr>
   <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:L8"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25"/>
@@ -43306,20 +44229,20 @@
       </c>
     </row>
     <row r="2" spans="1:12" ht="32.25" customHeight="1">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="51" t="s">
         <v>56</v>
       </c>
-      <c r="B2" s="39"/>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
-      <c r="I2" s="39"/>
-      <c r="J2" s="39"/>
-      <c r="K2" s="39"/>
-      <c r="L2" s="39"/>
+      <c r="B2" s="52"/>
+      <c r="C2" s="52"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="52"/>
+      <c r="F2" s="52"/>
+      <c r="G2" s="52"/>
+      <c r="H2" s="52"/>
+      <c r="I2" s="52"/>
+      <c r="J2" s="52"/>
+      <c r="K2" s="52"/>
+      <c r="L2" s="52"/>
     </row>
     <row r="3" spans="1:12" s="1" customFormat="1" ht="7.5" customHeight="1">
       <c r="A3" s="1" t="s">
@@ -43327,20 +44250,20 @@
       </c>
     </row>
     <row r="4" spans="1:12" ht="281.25" customHeight="1">
-      <c r="A4" s="40" t="s">
+      <c r="A4" s="53" t="s">
         <v>58</v>
       </c>
-      <c r="B4" s="41"/>
-      <c r="C4" s="41"/>
-      <c r="D4" s="41"/>
-      <c r="E4" s="41"/>
-      <c r="F4" s="41"/>
-      <c r="G4" s="41"/>
-      <c r="H4" s="41"/>
-      <c r="I4" s="41"/>
-      <c r="J4" s="41"/>
-      <c r="K4" s="41"/>
-      <c r="L4" s="42"/>
+      <c r="B4" s="54"/>
+      <c r="C4" s="54"/>
+      <c r="D4" s="54"/>
+      <c r="E4" s="54"/>
+      <c r="F4" s="54"/>
+      <c r="G4" s="54"/>
+      <c r="H4" s="54"/>
+      <c r="I4" s="54"/>
+      <c r="J4" s="54"/>
+      <c r="K4" s="54"/>
+      <c r="L4" s="55"/>
     </row>
     <row r="5" spans="1:12" s="1" customFormat="1" ht="7.5" customHeight="1">
       <c r="A5" s="1" t="s">
@@ -43348,20 +44271,20 @@
       </c>
     </row>
     <row r="6" spans="1:12" s="32" customFormat="1" ht="29.25" customHeight="1">
-      <c r="A6" s="38" t="s">
+      <c r="A6" s="51" t="s">
         <v>59</v>
       </c>
-      <c r="B6" s="39"/>
-      <c r="C6" s="39"/>
-      <c r="D6" s="39"/>
-      <c r="E6" s="39"/>
-      <c r="F6" s="39"/>
-      <c r="G6" s="39"/>
-      <c r="H6" s="39"/>
-      <c r="I6" s="39"/>
-      <c r="J6" s="39"/>
-      <c r="K6" s="39"/>
-      <c r="L6" s="39"/>
+      <c r="B6" s="52"/>
+      <c r="C6" s="52"/>
+      <c r="D6" s="52"/>
+      <c r="E6" s="52"/>
+      <c r="F6" s="52"/>
+      <c r="G6" s="52"/>
+      <c r="H6" s="52"/>
+      <c r="I6" s="52"/>
+      <c r="J6" s="52"/>
+      <c r="K6" s="52"/>
+      <c r="L6" s="52"/>
     </row>
     <row r="7" spans="1:12" s="1" customFormat="1" ht="7.5" customHeight="1">
       <c r="A7" s="1" t="s">
@@ -43369,20 +44292,20 @@
       </c>
     </row>
     <row r="8" spans="1:12" ht="134.25" customHeight="1">
-      <c r="A8" s="43" t="s">
+      <c r="A8" s="56" t="s">
         <v>60</v>
       </c>
-      <c r="B8" s="44"/>
-      <c r="C8" s="44"/>
-      <c r="D8" s="44"/>
-      <c r="E8" s="44"/>
-      <c r="F8" s="44"/>
-      <c r="G8" s="44"/>
-      <c r="H8" s="44"/>
-      <c r="I8" s="44"/>
-      <c r="J8" s="44"/>
-      <c r="K8" s="44"/>
-      <c r="L8" s="45"/>
+      <c r="B8" s="57"/>
+      <c r="C8" s="57"/>
+      <c r="D8" s="57"/>
+      <c r="E8" s="57"/>
+      <c r="F8" s="57"/>
+      <c r="G8" s="57"/>
+      <c r="H8" s="57"/>
+      <c r="I8" s="57"/>
+      <c r="J8" s="57"/>
+      <c r="K8" s="57"/>
+      <c r="L8" s="58"/>
     </row>
     <row r="9" spans="1:12">
       <c r="A9" s="33"/>
@@ -43456,16 +44379,183 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FFFF0000"/>
+  </sheetPr>
+  <dimension ref="A1:C24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <cols>
+    <col min="1" max="1" width="38.7109375" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="41" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="39" t="s">
+        <v>70</v>
+      </c>
+      <c r="B3" s="39" t="s">
+        <v>71</v>
+      </c>
+      <c r="C3" s="38"/>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="40" t="s">
+        <v>72</v>
+      </c>
+      <c r="B4" s="40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="40" t="s">
+        <v>73</v>
+      </c>
+      <c r="B5" s="40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="40" t="s">
+        <v>74</v>
+      </c>
+      <c r="B6" s="40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="40" t="s">
+        <v>75</v>
+      </c>
+      <c r="B7" s="40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="41" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="39" t="s">
+        <v>76</v>
+      </c>
+      <c r="B11" s="39" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="40" t="s">
+        <v>72</v>
+      </c>
+      <c r="B12" s="40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="40" t="s">
+        <v>73</v>
+      </c>
+      <c r="B13" s="40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="40" t="s">
+        <v>74</v>
+      </c>
+      <c r="B14" s="40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="40" t="s">
+        <v>75</v>
+      </c>
+      <c r="B15" s="40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="41" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="39" t="s">
+        <v>2</v>
+      </c>
+      <c r="B19" s="39" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="B20" s="40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="40" t="s">
+        <v>79</v>
+      </c>
+      <c r="B21" s="40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" s="40" t="s">
+        <v>80</v>
+      </c>
+      <c r="B22" s="40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" s="40" t="s">
+        <v>81</v>
+      </c>
+      <c r="B23" s="40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" s="40" t="s">
+        <v>82</v>
+      </c>
+      <c r="B24" s="40">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter alignWithMargins="0"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1">
     <tabColor rgb="FF366092"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:M11"/>
+  <dimension ref="A1:M50"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7:M7"/>
+      <selection activeCell="B34" sqref="B34:M34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -43484,22 +44574,22 @@
     <row r="1" spans="1:13" ht="7.5" customHeight="1"/>
     <row r="2" spans="1:13" s="4" customFormat="1" ht="250.5" customHeight="1">
       <c r="A2" s="3"/>
-      <c r="B2" s="46" t="s">
+      <c r="B2" s="79" t="s">
         <v>36</v>
       </c>
-      <c r="C2" s="47"/>
-      <c r="D2" s="48" t="s">
+      <c r="C2" s="80"/>
+      <c r="D2" s="68" t="s">
         <v>37</v>
       </c>
-      <c r="E2" s="49"/>
-      <c r="F2" s="49"/>
-      <c r="G2" s="49"/>
-      <c r="H2" s="49"/>
-      <c r="I2" s="49"/>
-      <c r="J2" s="49"/>
-      <c r="K2" s="49"/>
-      <c r="L2" s="49"/>
-      <c r="M2" s="50"/>
+      <c r="E2" s="69"/>
+      <c r="F2" s="69"/>
+      <c r="G2" s="69"/>
+      <c r="H2" s="69"/>
+      <c r="I2" s="69"/>
+      <c r="J2" s="69"/>
+      <c r="K2" s="69"/>
+      <c r="L2" s="69"/>
+      <c r="M2" s="70"/>
     </row>
     <row r="3" spans="1:13" s="20" customFormat="1" ht="7.5" customHeight="1">
       <c r="A3" s="16"/>
@@ -43518,20 +44608,20 @@
     </row>
     <row r="4" spans="1:13" ht="32.25" customHeight="1">
       <c r="A4" s="5"/>
-      <c r="B4" s="38" t="s">
+      <c r="B4" s="51" t="s">
         <v>35</v>
       </c>
-      <c r="C4" s="39"/>
-      <c r="D4" s="39"/>
-      <c r="E4" s="39"/>
-      <c r="F4" s="39"/>
-      <c r="G4" s="39"/>
-      <c r="H4" s="39"/>
-      <c r="I4" s="39"/>
-      <c r="J4" s="39"/>
-      <c r="K4" s="39"/>
-      <c r="L4" s="39"/>
-      <c r="M4" s="39"/>
+      <c r="C4" s="52"/>
+      <c r="D4" s="52"/>
+      <c r="E4" s="52"/>
+      <c r="F4" s="52"/>
+      <c r="G4" s="52"/>
+      <c r="H4" s="52"/>
+      <c r="I4" s="52"/>
+      <c r="J4" s="52"/>
+      <c r="K4" s="52"/>
+      <c r="L4" s="52"/>
+      <c r="M4" s="52"/>
     </row>
     <row r="5" spans="1:13" ht="7.5" customHeight="1">
       <c r="A5" s="5"/>
@@ -43557,22 +44647,22 @@
     </row>
     <row r="7" spans="1:13" s="4" customFormat="1" ht="168.75" customHeight="1">
       <c r="A7" s="3"/>
-      <c r="B7" s="46" t="s">
+      <c r="B7" s="79" t="s">
         <v>30</v>
       </c>
-      <c r="C7" s="47"/>
-      <c r="D7" s="48" t="s">
+      <c r="C7" s="80"/>
+      <c r="D7" s="68" t="s">
         <v>61</v>
       </c>
-      <c r="E7" s="49"/>
-      <c r="F7" s="49"/>
-      <c r="G7" s="49"/>
-      <c r="H7" s="49"/>
-      <c r="I7" s="49"/>
-      <c r="J7" s="49"/>
-      <c r="K7" s="49"/>
-      <c r="L7" s="49"/>
-      <c r="M7" s="50"/>
+      <c r="E7" s="69"/>
+      <c r="F7" s="69"/>
+      <c r="G7" s="69"/>
+      <c r="H7" s="69"/>
+      <c r="I7" s="69"/>
+      <c r="J7" s="69"/>
+      <c r="K7" s="69"/>
+      <c r="L7" s="69"/>
+      <c r="M7" s="70"/>
     </row>
     <row r="8" spans="1:13" ht="8.25" customHeight="1">
       <c r="A8" s="5"/>
@@ -43583,66 +44673,595 @@
     </row>
     <row r="9" spans="1:13" s="8" customFormat="1" ht="18" customHeight="1">
       <c r="A9" s="7"/>
-      <c r="B9" s="51" t="s">
+      <c r="B9" s="59" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="52"/>
-      <c r="D9" s="52"/>
-      <c r="E9" s="52"/>
-      <c r="F9" s="52"/>
-      <c r="G9" s="52"/>
-      <c r="H9" s="52"/>
-      <c r="I9" s="52"/>
-      <c r="J9" s="52"/>
-      <c r="K9" s="52"/>
-      <c r="L9" s="52"/>
-      <c r="M9" s="53"/>
+      <c r="C9" s="60"/>
+      <c r="D9" s="60"/>
+      <c r="E9" s="60"/>
+      <c r="F9" s="60"/>
+      <c r="G9" s="60"/>
+      <c r="H9" s="60"/>
+      <c r="I9" s="60"/>
+      <c r="J9" s="60"/>
+      <c r="K9" s="60"/>
+      <c r="L9" s="60"/>
+      <c r="M9" s="61"/>
     </row>
     <row r="10" spans="1:13" s="8" customFormat="1" ht="28.5" customHeight="1">
       <c r="A10" s="7"/>
-      <c r="B10" s="54" t="s">
+      <c r="B10" s="74" t="s">
         <v>0</v>
       </c>
-      <c r="C10" s="54"/>
-      <c r="D10" s="54" t="s">
+      <c r="C10" s="74"/>
+      <c r="D10" s="74" t="s">
         <v>5</v>
       </c>
-      <c r="E10" s="59"/>
-      <c r="F10" s="54" t="s">
+      <c r="E10" s="81"/>
+      <c r="F10" s="74" t="s">
         <v>47</v>
       </c>
-      <c r="G10" s="54"/>
-      <c r="H10" s="55" t="s">
+      <c r="G10" s="74"/>
+      <c r="H10" s="75" t="s">
         <v>48</v>
       </c>
-      <c r="I10" s="56"/>
-      <c r="J10" s="54" t="s">
+      <c r="I10" s="76"/>
+      <c r="J10" s="74" t="s">
         <v>49</v>
       </c>
-      <c r="K10" s="54"/>
-      <c r="L10" s="54" t="s">
+      <c r="K10" s="74"/>
+      <c r="L10" s="74" t="s">
         <v>1</v>
       </c>
-      <c r="M10" s="54"/>
+      <c r="M10" s="74"/>
     </row>
     <row r="11" spans="1:13" ht="42.75" customHeight="1">
       <c r="A11" s="5"/>
-      <c r="B11" s="57"/>
-      <c r="C11" s="58"/>
-      <c r="D11" s="57"/>
-      <c r="E11" s="58"/>
-      <c r="F11" s="57"/>
-      <c r="G11" s="58"/>
-      <c r="H11" s="57"/>
-      <c r="I11" s="58"/>
-      <c r="J11" s="57"/>
-      <c r="K11" s="58"/>
-      <c r="L11" s="57"/>
-      <c r="M11" s="58"/>
+      <c r="B11" s="77"/>
+      <c r="C11" s="78"/>
+      <c r="D11" s="77"/>
+      <c r="E11" s="78"/>
+      <c r="F11" s="77"/>
+      <c r="G11" s="78"/>
+      <c r="H11" s="77"/>
+      <c r="I11" s="78"/>
+      <c r="J11" s="77"/>
+      <c r="K11" s="78"/>
+      <c r="L11" s="77"/>
+      <c r="M11" s="78"/>
+    </row>
+    <row r="13" spans="1:13" ht="16.5">
+      <c r="B13" s="59" t="s">
+        <v>67</v>
+      </c>
+      <c r="C13" s="60"/>
+      <c r="D13" s="60"/>
+      <c r="E13" s="60"/>
+      <c r="F13" s="60"/>
+      <c r="G13" s="60"/>
+      <c r="H13" s="60"/>
+      <c r="I13" s="60"/>
+      <c r="J13" s="60"/>
+      <c r="K13" s="60"/>
+      <c r="L13" s="60"/>
+      <c r="M13" s="61"/>
+    </row>
+    <row r="14" spans="1:13" ht="34.5" customHeight="1">
+      <c r="B14" s="65" t="s">
+        <v>84</v>
+      </c>
+      <c r="C14" s="66"/>
+      <c r="D14" s="66"/>
+      <c r="E14" s="66"/>
+      <c r="F14" s="66"/>
+      <c r="G14" s="66"/>
+      <c r="H14" s="66"/>
+      <c r="I14" s="66"/>
+      <c r="J14" s="66"/>
+      <c r="K14" s="66"/>
+      <c r="L14" s="66"/>
+      <c r="M14" s="67"/>
+    </row>
+    <row r="15" spans="1:13">
+      <c r="B15" s="71" t="s">
+        <v>70</v>
+      </c>
+      <c r="C15" s="72"/>
+      <c r="D15" s="72"/>
+      <c r="E15" s="72"/>
+      <c r="F15" s="72"/>
+      <c r="G15" s="73"/>
+      <c r="H15" s="71" t="s">
+        <v>76</v>
+      </c>
+      <c r="I15" s="72"/>
+      <c r="J15" s="72"/>
+      <c r="K15" s="72"/>
+      <c r="L15" s="72"/>
+      <c r="M15" s="73"/>
+    </row>
+    <row r="16" spans="1:13">
+      <c r="B16" s="42"/>
+      <c r="C16" s="43"/>
+      <c r="D16" s="43"/>
+      <c r="E16" s="43"/>
+      <c r="F16" s="43"/>
+      <c r="G16" s="44"/>
+      <c r="H16" s="42"/>
+      <c r="I16" s="43"/>
+      <c r="J16" s="43"/>
+      <c r="K16" s="43"/>
+      <c r="L16" s="43"/>
+      <c r="M16" s="44"/>
+    </row>
+    <row r="17" spans="2:13">
+      <c r="B17" s="45"/>
+      <c r="C17" s="46"/>
+      <c r="D17" s="46"/>
+      <c r="E17" s="46"/>
+      <c r="F17" s="46"/>
+      <c r="G17" s="47"/>
+      <c r="H17" s="45"/>
+      <c r="I17" s="46"/>
+      <c r="J17" s="46"/>
+      <c r="K17" s="46"/>
+      <c r="L17" s="46"/>
+      <c r="M17" s="47"/>
+    </row>
+    <row r="18" spans="2:13">
+      <c r="B18" s="45"/>
+      <c r="C18" s="46"/>
+      <c r="D18" s="46"/>
+      <c r="E18" s="46"/>
+      <c r="F18" s="46"/>
+      <c r="G18" s="47"/>
+      <c r="H18" s="45"/>
+      <c r="I18" s="46"/>
+      <c r="J18" s="46"/>
+      <c r="K18" s="46"/>
+      <c r="L18" s="46"/>
+      <c r="M18" s="47"/>
+    </row>
+    <row r="19" spans="2:13">
+      <c r="B19" s="45"/>
+      <c r="C19" s="46"/>
+      <c r="D19" s="46"/>
+      <c r="E19" s="46"/>
+      <c r="F19" s="46"/>
+      <c r="G19" s="47"/>
+      <c r="H19" s="45"/>
+      <c r="I19" s="46"/>
+      <c r="J19" s="46"/>
+      <c r="K19" s="46"/>
+      <c r="L19" s="46"/>
+      <c r="M19" s="47"/>
+    </row>
+    <row r="20" spans="2:13">
+      <c r="B20" s="45"/>
+      <c r="C20" s="46"/>
+      <c r="D20" s="46"/>
+      <c r="E20" s="46"/>
+      <c r="F20" s="46"/>
+      <c r="G20" s="47"/>
+      <c r="H20" s="45"/>
+      <c r="I20" s="46"/>
+      <c r="J20" s="46"/>
+      <c r="K20" s="46"/>
+      <c r="L20" s="46"/>
+      <c r="M20" s="47"/>
+    </row>
+    <row r="21" spans="2:13">
+      <c r="B21" s="45"/>
+      <c r="C21" s="46"/>
+      <c r="D21" s="46"/>
+      <c r="E21" s="46"/>
+      <c r="F21" s="46"/>
+      <c r="G21" s="47"/>
+      <c r="H21" s="45"/>
+      <c r="I21" s="46"/>
+      <c r="J21" s="46"/>
+      <c r="K21" s="46"/>
+      <c r="L21" s="46"/>
+      <c r="M21" s="47"/>
+    </row>
+    <row r="22" spans="2:13">
+      <c r="B22" s="45"/>
+      <c r="C22" s="46"/>
+      <c r="D22" s="46"/>
+      <c r="E22" s="46"/>
+      <c r="F22" s="46"/>
+      <c r="G22" s="47"/>
+      <c r="H22" s="45"/>
+      <c r="I22" s="46"/>
+      <c r="J22" s="46"/>
+      <c r="K22" s="46"/>
+      <c r="L22" s="46"/>
+      <c r="M22" s="47"/>
+    </row>
+    <row r="23" spans="2:13">
+      <c r="B23" s="45"/>
+      <c r="C23" s="46"/>
+      <c r="D23" s="46"/>
+      <c r="E23" s="46"/>
+      <c r="F23" s="46"/>
+      <c r="G23" s="47"/>
+      <c r="H23" s="45"/>
+      <c r="I23" s="46"/>
+      <c r="J23" s="46"/>
+      <c r="K23" s="46"/>
+      <c r="L23" s="46"/>
+      <c r="M23" s="47"/>
+    </row>
+    <row r="24" spans="2:13">
+      <c r="B24" s="45"/>
+      <c r="C24" s="46"/>
+      <c r="D24" s="46"/>
+      <c r="E24" s="46"/>
+      <c r="F24" s="46"/>
+      <c r="G24" s="47"/>
+      <c r="H24" s="45"/>
+      <c r="I24" s="46"/>
+      <c r="J24" s="46"/>
+      <c r="K24" s="46"/>
+      <c r="L24" s="46"/>
+      <c r="M24" s="47"/>
+    </row>
+    <row r="25" spans="2:13">
+      <c r="B25" s="45"/>
+      <c r="C25" s="46"/>
+      <c r="D25" s="46"/>
+      <c r="E25" s="46"/>
+      <c r="F25" s="46"/>
+      <c r="G25" s="47"/>
+      <c r="H25" s="45"/>
+      <c r="I25" s="46"/>
+      <c r="J25" s="46"/>
+      <c r="K25" s="46"/>
+      <c r="L25" s="46"/>
+      <c r="M25" s="47"/>
+    </row>
+    <row r="26" spans="2:13">
+      <c r="B26" s="45"/>
+      <c r="C26" s="46"/>
+      <c r="D26" s="46"/>
+      <c r="E26" s="46"/>
+      <c r="F26" s="46"/>
+      <c r="G26" s="47"/>
+      <c r="H26" s="45"/>
+      <c r="I26" s="46"/>
+      <c r="J26" s="46"/>
+      <c r="K26" s="46"/>
+      <c r="L26" s="46"/>
+      <c r="M26" s="47"/>
+    </row>
+    <row r="27" spans="2:13">
+      <c r="B27" s="45"/>
+      <c r="C27" s="46"/>
+      <c r="D27" s="46"/>
+      <c r="E27" s="46"/>
+      <c r="F27" s="46"/>
+      <c r="G27" s="47"/>
+      <c r="H27" s="45"/>
+      <c r="I27" s="46"/>
+      <c r="J27" s="46"/>
+      <c r="K27" s="46"/>
+      <c r="L27" s="46"/>
+      <c r="M27" s="47"/>
+    </row>
+    <row r="28" spans="2:13">
+      <c r="B28" s="45"/>
+      <c r="C28" s="46"/>
+      <c r="D28" s="46"/>
+      <c r="E28" s="46"/>
+      <c r="F28" s="46"/>
+      <c r="G28" s="47"/>
+      <c r="H28" s="45"/>
+      <c r="I28" s="46"/>
+      <c r="J28" s="46"/>
+      <c r="K28" s="46"/>
+      <c r="L28" s="46"/>
+      <c r="M28" s="47"/>
+    </row>
+    <row r="29" spans="2:13">
+      <c r="B29" s="45"/>
+      <c r="C29" s="46"/>
+      <c r="D29" s="46"/>
+      <c r="E29" s="46"/>
+      <c r="F29" s="46"/>
+      <c r="G29" s="47"/>
+      <c r="H29" s="45"/>
+      <c r="I29" s="46"/>
+      <c r="J29" s="46"/>
+      <c r="K29" s="46"/>
+      <c r="L29" s="46"/>
+      <c r="M29" s="47"/>
+    </row>
+    <row r="30" spans="2:13">
+      <c r="B30" s="45"/>
+      <c r="C30" s="46"/>
+      <c r="D30" s="46"/>
+      <c r="E30" s="46"/>
+      <c r="F30" s="46"/>
+      <c r="G30" s="47"/>
+      <c r="H30" s="45"/>
+      <c r="I30" s="46"/>
+      <c r="J30" s="46"/>
+      <c r="K30" s="46"/>
+      <c r="L30" s="46"/>
+      <c r="M30" s="47"/>
+    </row>
+    <row r="31" spans="2:13">
+      <c r="B31" s="48"/>
+      <c r="C31" s="49"/>
+      <c r="D31" s="49"/>
+      <c r="E31" s="49"/>
+      <c r="F31" s="49"/>
+      <c r="G31" s="50"/>
+      <c r="H31" s="48"/>
+      <c r="I31" s="49"/>
+      <c r="J31" s="49"/>
+      <c r="K31" s="49"/>
+      <c r="L31" s="49"/>
+      <c r="M31" s="50"/>
+    </row>
+    <row r="33" spans="2:13" ht="16.5">
+      <c r="B33" s="59" t="s">
+        <v>77</v>
+      </c>
+      <c r="C33" s="60"/>
+      <c r="D33" s="60"/>
+      <c r="E33" s="60"/>
+      <c r="F33" s="60"/>
+      <c r="G33" s="60"/>
+      <c r="H33" s="60"/>
+      <c r="I33" s="60"/>
+      <c r="J33" s="60"/>
+      <c r="K33" s="60"/>
+      <c r="L33" s="60"/>
+      <c r="M33" s="61"/>
+    </row>
+    <row r="34" spans="2:13" ht="33.75" customHeight="1">
+      <c r="B34" s="62" t="s">
+        <v>83</v>
+      </c>
+      <c r="C34" s="63"/>
+      <c r="D34" s="63"/>
+      <c r="E34" s="63"/>
+      <c r="F34" s="63"/>
+      <c r="G34" s="63"/>
+      <c r="H34" s="63"/>
+      <c r="I34" s="63"/>
+      <c r="J34" s="63"/>
+      <c r="K34" s="63"/>
+      <c r="L34" s="63"/>
+      <c r="M34" s="64"/>
+    </row>
+    <row r="35" spans="2:13">
+      <c r="B35" s="42"/>
+      <c r="C35" s="43"/>
+      <c r="D35" s="43"/>
+      <c r="E35" s="43"/>
+      <c r="F35" s="43"/>
+      <c r="G35" s="43"/>
+      <c r="H35" s="43"/>
+      <c r="I35" s="43"/>
+      <c r="J35" s="43"/>
+      <c r="K35" s="43"/>
+      <c r="L35" s="43"/>
+      <c r="M35" s="44"/>
+    </row>
+    <row r="36" spans="2:13">
+      <c r="B36" s="45"/>
+      <c r="C36" s="46"/>
+      <c r="D36" s="46"/>
+      <c r="E36" s="46"/>
+      <c r="F36" s="46"/>
+      <c r="G36" s="46"/>
+      <c r="H36" s="46"/>
+      <c r="I36" s="46"/>
+      <c r="J36" s="46"/>
+      <c r="K36" s="46"/>
+      <c r="L36" s="46"/>
+      <c r="M36" s="47"/>
+    </row>
+    <row r="37" spans="2:13">
+      <c r="B37" s="45"/>
+      <c r="C37" s="46"/>
+      <c r="D37" s="46"/>
+      <c r="E37" s="46"/>
+      <c r="F37" s="46"/>
+      <c r="G37" s="46"/>
+      <c r="H37" s="46"/>
+      <c r="I37" s="46"/>
+      <c r="J37" s="46"/>
+      <c r="K37" s="46"/>
+      <c r="L37" s="46"/>
+      <c r="M37" s="47"/>
+    </row>
+    <row r="38" spans="2:13">
+      <c r="B38" s="45"/>
+      <c r="C38" s="46"/>
+      <c r="D38" s="46"/>
+      <c r="E38" s="46"/>
+      <c r="F38" s="46"/>
+      <c r="G38" s="46"/>
+      <c r="H38" s="46"/>
+      <c r="I38" s="46"/>
+      <c r="J38" s="46"/>
+      <c r="K38" s="46"/>
+      <c r="L38" s="46"/>
+      <c r="M38" s="47"/>
+    </row>
+    <row r="39" spans="2:13">
+      <c r="B39" s="45"/>
+      <c r="C39" s="46"/>
+      <c r="D39" s="46"/>
+      <c r="E39" s="46"/>
+      <c r="F39" s="46"/>
+      <c r="G39" s="46"/>
+      <c r="H39" s="46"/>
+      <c r="I39" s="46"/>
+      <c r="J39" s="46"/>
+      <c r="K39" s="46"/>
+      <c r="L39" s="46"/>
+      <c r="M39" s="47"/>
+    </row>
+    <row r="40" spans="2:13">
+      <c r="B40" s="45"/>
+      <c r="C40" s="46"/>
+      <c r="D40" s="46"/>
+      <c r="E40" s="46"/>
+      <c r="F40" s="46"/>
+      <c r="G40" s="46"/>
+      <c r="H40" s="46"/>
+      <c r="I40" s="46"/>
+      <c r="J40" s="46"/>
+      <c r="K40" s="46"/>
+      <c r="L40" s="46"/>
+      <c r="M40" s="47"/>
+    </row>
+    <row r="41" spans="2:13">
+      <c r="B41" s="45"/>
+      <c r="C41" s="46"/>
+      <c r="D41" s="46"/>
+      <c r="E41" s="46"/>
+      <c r="F41" s="46"/>
+      <c r="G41" s="46"/>
+      <c r="H41" s="46"/>
+      <c r="I41" s="46"/>
+      <c r="J41" s="46"/>
+      <c r="K41" s="46"/>
+      <c r="L41" s="46"/>
+      <c r="M41" s="47"/>
+    </row>
+    <row r="42" spans="2:13">
+      <c r="B42" s="45"/>
+      <c r="C42" s="46"/>
+      <c r="D42" s="46"/>
+      <c r="E42" s="46"/>
+      <c r="F42" s="46"/>
+      <c r="G42" s="46"/>
+      <c r="H42" s="46"/>
+      <c r="I42" s="46"/>
+      <c r="J42" s="46"/>
+      <c r="K42" s="46"/>
+      <c r="L42" s="46"/>
+      <c r="M42" s="47"/>
+    </row>
+    <row r="43" spans="2:13">
+      <c r="B43" s="45"/>
+      <c r="C43" s="46"/>
+      <c r="D43" s="46"/>
+      <c r="E43" s="46"/>
+      <c r="F43" s="46"/>
+      <c r="G43" s="46"/>
+      <c r="H43" s="46"/>
+      <c r="I43" s="46"/>
+      <c r="J43" s="46"/>
+      <c r="K43" s="46"/>
+      <c r="L43" s="46"/>
+      <c r="M43" s="47"/>
+    </row>
+    <row r="44" spans="2:13">
+      <c r="B44" s="45"/>
+      <c r="C44" s="46"/>
+      <c r="D44" s="46"/>
+      <c r="E44" s="46"/>
+      <c r="F44" s="46"/>
+      <c r="G44" s="46"/>
+      <c r="H44" s="46"/>
+      <c r="I44" s="46"/>
+      <c r="J44" s="46"/>
+      <c r="K44" s="46"/>
+      <c r="L44" s="46"/>
+      <c r="M44" s="47"/>
+    </row>
+    <row r="45" spans="2:13">
+      <c r="B45" s="45"/>
+      <c r="C45" s="46"/>
+      <c r="D45" s="46"/>
+      <c r="E45" s="46"/>
+      <c r="F45" s="46"/>
+      <c r="G45" s="46"/>
+      <c r="H45" s="46"/>
+      <c r="I45" s="46"/>
+      <c r="J45" s="46"/>
+      <c r="K45" s="46"/>
+      <c r="L45" s="46"/>
+      <c r="M45" s="47"/>
+    </row>
+    <row r="46" spans="2:13">
+      <c r="B46" s="45"/>
+      <c r="C46" s="46"/>
+      <c r="D46" s="46"/>
+      <c r="E46" s="46"/>
+      <c r="F46" s="46"/>
+      <c r="G46" s="46"/>
+      <c r="H46" s="46"/>
+      <c r="I46" s="46"/>
+      <c r="J46" s="46"/>
+      <c r="K46" s="46"/>
+      <c r="L46" s="46"/>
+      <c r="M46" s="47"/>
+    </row>
+    <row r="47" spans="2:13">
+      <c r="B47" s="45"/>
+      <c r="C47" s="46"/>
+      <c r="D47" s="46"/>
+      <c r="E47" s="46"/>
+      <c r="F47" s="46"/>
+      <c r="G47" s="46"/>
+      <c r="H47" s="46"/>
+      <c r="I47" s="46"/>
+      <c r="J47" s="46"/>
+      <c r="K47" s="46"/>
+      <c r="L47" s="46"/>
+      <c r="M47" s="47"/>
+    </row>
+    <row r="48" spans="2:13">
+      <c r="B48" s="45"/>
+      <c r="C48" s="46"/>
+      <c r="D48" s="46"/>
+      <c r="E48" s="46"/>
+      <c r="F48" s="46"/>
+      <c r="G48" s="46"/>
+      <c r="H48" s="46"/>
+      <c r="I48" s="46"/>
+      <c r="J48" s="46"/>
+      <c r="K48" s="46"/>
+      <c r="L48" s="46"/>
+      <c r="M48" s="47"/>
+    </row>
+    <row r="49" spans="2:13">
+      <c r="B49" s="45"/>
+      <c r="C49" s="46"/>
+      <c r="D49" s="46"/>
+      <c r="E49" s="46"/>
+      <c r="F49" s="46"/>
+      <c r="G49" s="46"/>
+      <c r="H49" s="46"/>
+      <c r="I49" s="46"/>
+      <c r="J49" s="46"/>
+      <c r="K49" s="46"/>
+      <c r="L49" s="46"/>
+      <c r="M49" s="47"/>
+    </row>
+    <row r="50" spans="2:13">
+      <c r="B50" s="48"/>
+      <c r="C50" s="49"/>
+      <c r="D50" s="49"/>
+      <c r="E50" s="49"/>
+      <c r="F50" s="49"/>
+      <c r="G50" s="49"/>
+      <c r="H50" s="49"/>
+      <c r="I50" s="49"/>
+      <c r="J50" s="49"/>
+      <c r="K50" s="49"/>
+      <c r="L50" s="49"/>
+      <c r="M50" s="50"/>
     </row>
   </sheetData>
-  <mergeCells count="18">
-    <mergeCell ref="B11:C11"/>
+  <mergeCells count="24">
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B4:M4"/>
     <mergeCell ref="D2:M2"/>
@@ -43656,14 +45275,22 @@
     <mergeCell ref="J10:K10"/>
     <mergeCell ref="D10:E10"/>
     <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B33:M33"/>
+    <mergeCell ref="B34:M34"/>
+    <mergeCell ref="B14:M14"/>
     <mergeCell ref="D7:M7"/>
     <mergeCell ref="B9:M9"/>
+    <mergeCell ref="B13:M13"/>
+    <mergeCell ref="B15:G15"/>
+    <mergeCell ref="H15:M15"/>
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="H10:I10"/>
+    <mergeCell ref="B11:C11"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup fitToWidth="0" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -43675,7 +45302,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -43685,7 +45312,7 @@
     <col min="3" max="3" width="17.140625" style="1" customWidth="1"/>
     <col min="4" max="4" width="12" style="1" customWidth="1"/>
     <col min="5" max="5" width="10.5703125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="12.140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="14.28515625" style="1" customWidth="1"/>
     <col min="7" max="7" width="15.85546875" style="1" customWidth="1"/>
     <col min="8" max="16384" width="9.140625" style="1"/>
   </cols>
@@ -43696,26 +45323,26 @@
       </c>
     </row>
     <row r="2" spans="1:7" ht="18" customHeight="1">
-      <c r="A2" s="60" t="s">
+      <c r="A2" s="82" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="60"/>
-      <c r="C2" s="60"/>
-      <c r="D2" s="60"/>
-      <c r="E2" s="60"/>
-      <c r="F2" s="60"/>
-      <c r="G2" s="60"/>
+      <c r="B2" s="82"/>
+      <c r="C2" s="82"/>
+      <c r="D2" s="82"/>
+      <c r="E2" s="82"/>
+      <c r="F2" s="82"/>
+      <c r="G2" s="82"/>
     </row>
     <row r="3" spans="1:7" ht="18" customHeight="1">
-      <c r="A3" s="66" t="s">
+      <c r="A3" s="88" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="66"/>
-      <c r="C3" s="66"/>
-      <c r="D3" s="66"/>
-      <c r="E3" s="66"/>
-      <c r="F3" s="66"/>
-      <c r="G3" s="66"/>
+      <c r="B3" s="88"/>
+      <c r="C3" s="88"/>
+      <c r="D3" s="88"/>
+      <c r="E3" s="88"/>
+      <c r="F3" s="88"/>
+      <c r="G3" s="88"/>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="1" t="s">
@@ -43723,15 +45350,15 @@
       </c>
     </row>
     <row r="5" spans="1:7" ht="25.5" customHeight="1">
-      <c r="A5" s="67" t="s">
+      <c r="A5" s="89" t="s">
         <v>62</v>
       </c>
-      <c r="B5" s="68"/>
-      <c r="C5" s="68"/>
-      <c r="D5" s="68"/>
-      <c r="E5" s="68"/>
-      <c r="F5" s="68"/>
-      <c r="G5" s="69"/>
+      <c r="B5" s="90"/>
+      <c r="C5" s="90"/>
+      <c r="D5" s="90"/>
+      <c r="E5" s="90"/>
+      <c r="F5" s="90"/>
+      <c r="G5" s="91"/>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="1" t="s">
@@ -43739,17 +45366,17 @@
       </c>
     </row>
     <row r="7" spans="1:7" ht="18.75" customHeight="1">
-      <c r="A7" s="64" t="s">
+      <c r="A7" s="86" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="65"/>
-      <c r="C7" s="61" t="s">
+      <c r="B7" s="87"/>
+      <c r="C7" s="83" t="s">
         <v>53</v>
       </c>
-      <c r="D7" s="62"/>
-      <c r="E7" s="62"/>
-      <c r="F7" s="62"/>
-      <c r="G7" s="63"/>
+      <c r="D7" s="84"/>
+      <c r="E7" s="84"/>
+      <c r="F7" s="84"/>
+      <c r="G7" s="85"/>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="1" t="s">
@@ -43815,7 +45442,7 @@
   <dimension ref="A2:G10"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -43825,56 +45452,56 @@
     <col min="3" max="3" width="17.140625" style="1" customWidth="1"/>
     <col min="4" max="4" width="12" style="1" customWidth="1"/>
     <col min="5" max="5" width="10.5703125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="12.140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="14.28515625" style="1" customWidth="1"/>
     <col min="7" max="7" width="15.85546875" style="1" customWidth="1"/>
     <col min="8" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:7" ht="18" customHeight="1">
-      <c r="A2" s="70" t="s">
+      <c r="A2" s="92" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="71"/>
-      <c r="C2" s="71"/>
-      <c r="D2" s="71"/>
-      <c r="E2" s="71"/>
-      <c r="F2" s="71"/>
-      <c r="G2" s="72"/>
+      <c r="B2" s="93"/>
+      <c r="C2" s="93"/>
+      <c r="D2" s="93"/>
+      <c r="E2" s="93"/>
+      <c r="F2" s="93"/>
+      <c r="G2" s="94"/>
     </row>
     <row r="3" spans="1:7" ht="18" customHeight="1">
-      <c r="A3" s="66" t="s">
+      <c r="A3" s="88" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="66"/>
-      <c r="C3" s="66"/>
-      <c r="D3" s="66"/>
-      <c r="E3" s="66"/>
-      <c r="F3" s="66"/>
-      <c r="G3" s="66"/>
+      <c r="B3" s="88"/>
+      <c r="C3" s="88"/>
+      <c r="D3" s="88"/>
+      <c r="E3" s="88"/>
+      <c r="F3" s="88"/>
+      <c r="G3" s="88"/>
     </row>
     <row r="5" spans="1:7" ht="25.5" customHeight="1">
-      <c r="A5" s="67" t="s">
+      <c r="A5" s="89" t="s">
         <v>63</v>
       </c>
-      <c r="B5" s="68"/>
-      <c r="C5" s="68"/>
-      <c r="D5" s="68"/>
-      <c r="E5" s="68"/>
-      <c r="F5" s="68"/>
-      <c r="G5" s="69"/>
+      <c r="B5" s="90"/>
+      <c r="C5" s="90"/>
+      <c r="D5" s="90"/>
+      <c r="E5" s="90"/>
+      <c r="F5" s="90"/>
+      <c r="G5" s="91"/>
     </row>
     <row r="7" spans="1:7" ht="18.75" customHeight="1">
-      <c r="A7" s="66" t="s">
+      <c r="A7" s="88" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="66"/>
-      <c r="C7" s="73" t="s">
+      <c r="B7" s="88"/>
+      <c r="C7" s="95" t="s">
         <v>54</v>
       </c>
-      <c r="D7" s="73"/>
-      <c r="E7" s="73"/>
-      <c r="F7" s="73"/>
-      <c r="G7" s="73"/>
+      <c r="D7" s="95"/>
+      <c r="E7" s="95"/>
+      <c r="F7" s="95"/>
+      <c r="G7" s="95"/>
     </row>
     <row r="9" spans="1:7" ht="25.5">
       <c r="A9" s="35" t="s">
@@ -43931,29 +45558,29 @@
   <dimension ref="A2:J11"/>
   <sheetViews>
     <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="9.7109375" style="1" customWidth="1"/>
-    <col min="2" max="10" width="12.85546875" style="1" customWidth="1"/>
+    <col min="2" max="10" width="15" style="1" customWidth="1"/>
     <col min="11" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:10" ht="18" customHeight="1">
-      <c r="A2" s="77" t="s">
+      <c r="A2" s="99" t="s">
         <v>38</v>
       </c>
-      <c r="B2" s="77"/>
-      <c r="C2" s="77"/>
-      <c r="D2" s="77"/>
-      <c r="E2" s="77"/>
-      <c r="F2" s="77"/>
-      <c r="G2" s="77"/>
-      <c r="H2" s="77"/>
-      <c r="I2" s="77"/>
-      <c r="J2" s="77"/>
+      <c r="B2" s="99"/>
+      <c r="C2" s="99"/>
+      <c r="D2" s="99"/>
+      <c r="E2" s="99"/>
+      <c r="F2" s="99"/>
+      <c r="G2" s="99"/>
+      <c r="H2" s="99"/>
+      <c r="I2" s="99"/>
+      <c r="J2" s="99"/>
     </row>
     <row r="3" spans="1:10" ht="18">
       <c r="A3" s="12"/>
@@ -43963,17 +45590,17 @@
       <c r="A4" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="74" t="s">
+      <c r="B4" s="96" t="s">
         <v>64</v>
       </c>
-      <c r="C4" s="75"/>
-      <c r="D4" s="75"/>
-      <c r="E4" s="75"/>
-      <c r="F4" s="75"/>
-      <c r="G4" s="75"/>
-      <c r="H4" s="75"/>
-      <c r="I4" s="75"/>
-      <c r="J4" s="76"/>
+      <c r="C4" s="97"/>
+      <c r="D4" s="97"/>
+      <c r="E4" s="97"/>
+      <c r="F4" s="97"/>
+      <c r="G4" s="97"/>
+      <c r="H4" s="97"/>
+      <c r="I4" s="97"/>
+      <c r="J4" s="98"/>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="2"/>
@@ -44094,7 +45721,7 @@
     <mergeCell ref="A2:J2"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup scale="96" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <pageSetup scale="75" fitToHeight="0" orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
@@ -44107,8 +45734,8 @@
   </sheetPr>
   <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="80" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10" defaultRowHeight="12.75"/>
@@ -44121,34 +45748,34 @@
   <sheetData>
     <row r="1" spans="1:10" ht="18" customHeight="1"/>
     <row r="2" spans="1:10" ht="18" customHeight="1">
-      <c r="A2" s="77" t="s">
+      <c r="A2" s="99" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="77"/>
-      <c r="C2" s="77"/>
-      <c r="D2" s="77"/>
-      <c r="E2" s="77"/>
-      <c r="F2" s="77"/>
-      <c r="G2" s="77"/>
-      <c r="H2" s="77"/>
-      <c r="I2" s="77"/>
-      <c r="J2" s="77"/>
+      <c r="B2" s="99"/>
+      <c r="C2" s="99"/>
+      <c r="D2" s="99"/>
+      <c r="E2" s="99"/>
+      <c r="F2" s="99"/>
+      <c r="G2" s="99"/>
+      <c r="H2" s="99"/>
+      <c r="I2" s="99"/>
+      <c r="J2" s="99"/>
     </row>
     <row r="4" spans="1:10" ht="53.25" customHeight="1">
       <c r="A4" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="78" t="s">
+      <c r="B4" s="100" t="s">
         <v>65</v>
       </c>
-      <c r="C4" s="79"/>
-      <c r="D4" s="79"/>
-      <c r="E4" s="79"/>
-      <c r="F4" s="79"/>
-      <c r="G4" s="79"/>
-      <c r="H4" s="79"/>
-      <c r="I4" s="79"/>
-      <c r="J4" s="80"/>
+      <c r="C4" s="101"/>
+      <c r="D4" s="101"/>
+      <c r="E4" s="101"/>
+      <c r="F4" s="101"/>
+      <c r="G4" s="101"/>
+      <c r="H4" s="101"/>
+      <c r="I4" s="101"/>
+      <c r="J4" s="102"/>
     </row>
     <row r="6" spans="1:10" ht="39.75" customHeight="1">
       <c r="A6" s="35" t="s">
@@ -44192,10 +45819,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:2" ht="18">
-      <c r="A2" s="77" t="s">
+      <c r="A2" s="99" t="s">
         <v>57</v>
       </c>
-      <c r="B2" s="77"/>
+      <c r="B2" s="99"/>
     </row>
     <row r="3" spans="1:2" ht="18">
       <c r="A3" s="12"/>
@@ -44255,11 +45882,11 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:3" ht="18">
-      <c r="A2" s="77" t="s">
+      <c r="A2" s="99" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="77"/>
-      <c r="C2" s="77"/>
+      <c r="B2" s="99"/>
+      <c r="C2" s="99"/>
     </row>
     <row r="3" spans="1:3" ht="18">
       <c r="A3" s="12"/>
@@ -44270,10 +45897,10 @@
       <c r="A4" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="74" t="s">
+      <c r="B4" s="96" t="s">
         <v>66</v>
       </c>
-      <c r="C4" s="76"/>
+      <c r="C4" s="98"/>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="2"/>
@@ -44314,7 +45941,7 @@
   </sheetPr>
   <dimension ref="A1:M8"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScaleNormal="100" zoomScalePageLayoutView="80" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="80" workbookViewId="0">
       <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
@@ -44338,40 +45965,40 @@
   <sheetData>
     <row r="1" spans="1:13" ht="18" customHeight="1"/>
     <row r="2" spans="1:13" ht="18" customHeight="1">
-      <c r="A2" s="77" t="s">
+      <c r="A2" s="99" t="s">
         <v>33</v>
       </c>
-      <c r="B2" s="77"/>
-      <c r="C2" s="77"/>
-      <c r="D2" s="77"/>
-      <c r="E2" s="77"/>
-      <c r="F2" s="77"/>
-      <c r="G2" s="77"/>
-      <c r="H2" s="77"/>
-      <c r="I2" s="77"/>
-      <c r="J2" s="77"/>
-      <c r="K2" s="77"/>
-      <c r="L2" s="77"/>
-      <c r="M2" s="77"/>
+      <c r="B2" s="99"/>
+      <c r="C2" s="99"/>
+      <c r="D2" s="99"/>
+      <c r="E2" s="99"/>
+      <c r="F2" s="99"/>
+      <c r="G2" s="99"/>
+      <c r="H2" s="99"/>
+      <c r="I2" s="99"/>
+      <c r="J2" s="99"/>
+      <c r="K2" s="99"/>
+      <c r="L2" s="99"/>
+      <c r="M2" s="99"/>
     </row>
     <row r="4" spans="1:13" ht="20.25" customHeight="1">
-      <c r="A4" s="81" t="s">
+      <c r="A4" s="103" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="82"/>
-      <c r="C4" s="83"/>
-      <c r="D4" s="84" t="s">
+      <c r="B4" s="104"/>
+      <c r="C4" s="105"/>
+      <c r="D4" s="106" t="s">
         <v>42</v>
       </c>
-      <c r="E4" s="85"/>
-      <c r="F4" s="85"/>
-      <c r="G4" s="85"/>
-      <c r="H4" s="85"/>
-      <c r="I4" s="85"/>
-      <c r="J4" s="85"/>
-      <c r="K4" s="85"/>
-      <c r="L4" s="85"/>
-      <c r="M4" s="86"/>
+      <c r="E4" s="107"/>
+      <c r="F4" s="107"/>
+      <c r="G4" s="107"/>
+      <c r="H4" s="107"/>
+      <c r="I4" s="107"/>
+      <c r="J4" s="107"/>
+      <c r="K4" s="107"/>
+      <c r="L4" s="107"/>
+      <c r="M4" s="108"/>
     </row>
     <row r="6" spans="1:13" ht="39.75" customHeight="1">
       <c r="A6" s="35" t="s">

</xml_diff>

<commit_message>
updated lpi and lpni reports to include before ioc date
git-svn-id: svn://107.170.10.188:8080/Semoss/trunk@2536 ef391c1c-ee15-45f7-b1d6-dde3d27a2169

Former-commit-id: 307802c0a30e35ec651380dd2893a4abc4b494d8
</commit_message>
<xml_diff>
--- a/export/Reports/Individual_System_LPI_Transition_Report_Template.xlsx
+++ b/export/Reports/Individual_System_LPI_Transition_Report_Template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="1110" windowWidth="15120" windowHeight="6405" tabRatio="834"/>
+    <workbookView xWindow="240" yWindow="1110" windowWidth="15120" windowHeight="6405" tabRatio="834" firstSheet="3" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="33" r:id="rId1"/>
@@ -342,9 +342,6 @@
     <t>This section displays the cost to upgrade software and hardware that @SYSTEM@ uses as the modules reach end-of-life.</t>
   </si>
   <si>
-    <t>This section displays the data objects that @SYSTEM@ is a source of record of and the numbers of systems which DMHRSi sends the data to. Additionally, this section displays the data objects that @SYSTEM@ consumes, the other systems that are a source of the data object and the number of low probability systems they provide data for.</t>
-  </si>
-  <si>
     <t xml:space="preserve">This section displays @SYSTEM@ that are source of record for the data objects that DHMSM capabilities consume. </t>
   </si>
   <si>
@@ -399,7 +396,10 @@
     <t>The following graph illustrates the number of interfaces @SYSTEM@ will have in the future state based upon the business rules established for each interface type.</t>
   </si>
   <si>
-    <t>The following graphs provide an overview of the hardware and software maturity for @SYSTEM@, illustrating the number of software and hardware products in each lifecycle phase.</t>
+    <t>The following graphs provide an overview of the hardware and software maturity for @SYSTEM@, illustrating the number of software and hardware products in each lifecycle phase  at the start of IOC (expected @DATE@).</t>
+  </si>
+  <si>
+    <t>This section displays the data objects that @SYSTEM@ is a source of record of and the numbers of systems which @SYSTEM@ sends the data to. Additionally, this section displays the data objects that @SYSTEM@ consumes, the other systems that are a source of the data object and the number of low probability systems they provide data for.</t>
   </si>
 </sst>
 </file>
@@ -1397,11 +1397,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="457379368"/>
-        <c:axId val="457379760"/>
+        <c:axId val="417183784"/>
+        <c:axId val="417183392"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="457379368"/>
+        <c:axId val="417183784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1411,7 +1411,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="457379760"/>
+        <c:crossAx val="417183392"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1419,7 +1419,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="457379760"/>
+        <c:axId val="417183392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1430,7 +1430,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="457379368"/>
+        <c:crossAx val="417183784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1563,11 +1563,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="457380936"/>
-        <c:axId val="457381328"/>
+        <c:axId val="441473776"/>
+        <c:axId val="441474168"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="457380936"/>
+        <c:axId val="441473776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1577,7 +1577,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="457381328"/>
+        <c:crossAx val="441474168"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1585,7 +1585,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="457381328"/>
+        <c:axId val="441474168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1596,7 +1596,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="457380936"/>
+        <c:crossAx val="441473776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1838,11 +1838,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="414560496"/>
-        <c:axId val="414560104"/>
+        <c:axId val="441474952"/>
+        <c:axId val="441475344"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="414560496"/>
+        <c:axId val="441474952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1852,7 +1852,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="414560104"/>
+        <c:crossAx val="441475344"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1860,7 +1860,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="414560104"/>
+        <c:axId val="441475344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1871,7 +1871,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="414560496"/>
+        <c:crossAx val="441474952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1927,7 +1927,7 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>83344</xdr:colOff>
+      <xdr:colOff>35718</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>134540</xdr:rowOff>
     </xdr:from>
@@ -44211,7 +44211,7 @@
   </sheetPr>
   <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="A4" sqref="A4:L4"/>
     </sheetView>
   </sheetViews>
@@ -44386,8 +44386,8 @@
   </sheetPr>
   <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -44398,21 +44398,21 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="41" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="39" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B3" s="39" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C3" s="38"/>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="40" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B4" s="40">
         <v>0</v>
@@ -44420,7 +44420,7 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="40" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B5" s="40">
         <v>0</v>
@@ -44428,7 +44428,7 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="40" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B6" s="40">
         <v>0</v>
@@ -44436,7 +44436,7 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="40" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B7" s="40">
         <v>0</v>
@@ -44444,20 +44444,20 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="41" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="39" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B11" s="39" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="40" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B12" s="40">
         <v>0</v>
@@ -44465,7 +44465,7 @@
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="40" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B13" s="40">
         <v>0</v>
@@ -44473,7 +44473,7 @@
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="40" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B14" s="40">
         <v>0</v>
@@ -44481,7 +44481,7 @@
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="40" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B15" s="40">
         <v>0</v>
@@ -44489,7 +44489,7 @@
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="41" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -44497,12 +44497,12 @@
         <v>2</v>
       </c>
       <c r="B19" s="39" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="40" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B20" s="40">
         <v>0</v>
@@ -44510,7 +44510,7 @@
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="40" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B21" s="40">
         <v>0</v>
@@ -44518,7 +44518,7 @@
     </row>
     <row r="22" spans="1:2">
       <c r="A22" s="40" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B22" s="40">
         <v>0</v>
@@ -44526,7 +44526,7 @@
     </row>
     <row r="23" spans="1:2">
       <c r="A23" s="40" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B23" s="40">
         <v>0</v>
@@ -44534,7 +44534,7 @@
     </row>
     <row r="24" spans="1:2">
       <c r="A24" s="40" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B24" s="40">
         <v>0</v>
@@ -44554,8 +44554,8 @@
   </sheetPr>
   <dimension ref="A1:M50"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34:M34"/>
+    <sheetView topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7:M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -44565,8 +44565,9 @@
     <col min="3" max="3" width="6.7109375" style="6" customWidth="1"/>
     <col min="4" max="5" width="8" style="6" customWidth="1"/>
     <col min="6" max="6" width="8.85546875" style="6" customWidth="1"/>
-    <col min="7" max="7" width="9" style="6" customWidth="1"/>
-    <col min="8" max="10" width="7.5703125" style="6" customWidth="1"/>
+    <col min="7" max="7" width="8.140625" style="6" customWidth="1"/>
+    <col min="8" max="8" width="8.42578125" style="6" customWidth="1"/>
+    <col min="9" max="10" width="7.5703125" style="6" customWidth="1"/>
     <col min="11" max="13" width="7.42578125" style="6" customWidth="1"/>
     <col min="14" max="16384" width="9.140625" style="6"/>
   </cols>
@@ -44645,7 +44646,7 @@
       <c r="L6" s="11"/>
       <c r="M6" s="11"/>
     </row>
-    <row r="7" spans="1:13" s="4" customFormat="1" ht="168.75" customHeight="1">
+    <row r="7" spans="1:13" s="4" customFormat="1" ht="375" customHeight="1">
       <c r="A7" s="3"/>
       <c r="B7" s="79" t="s">
         <v>30</v>
@@ -44732,7 +44733,7 @@
     </row>
     <row r="13" spans="1:13" ht="16.5">
       <c r="B13" s="59" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C13" s="60"/>
       <c r="D13" s="60"/>
@@ -44746,9 +44747,9 @@
       <c r="L13" s="60"/>
       <c r="M13" s="61"/>
     </row>
-    <row r="14" spans="1:13" ht="34.5" customHeight="1">
+    <row r="14" spans="1:13" ht="51" customHeight="1">
       <c r="B14" s="65" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C14" s="66"/>
       <c r="D14" s="66"/>
@@ -44764,7 +44765,7 @@
     </row>
     <row r="15" spans="1:13">
       <c r="B15" s="71" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C15" s="72"/>
       <c r="D15" s="72"/>
@@ -44772,7 +44773,7 @@
       <c r="F15" s="72"/>
       <c r="G15" s="73"/>
       <c r="H15" s="71" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I15" s="72"/>
       <c r="J15" s="72"/>
@@ -45006,7 +45007,7 @@
     </row>
     <row r="33" spans="2:13" ht="16.5">
       <c r="B33" s="59" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C33" s="60"/>
       <c r="D33" s="60"/>
@@ -45022,7 +45023,7 @@
     </row>
     <row r="34" spans="2:13" ht="33.75" customHeight="1">
       <c r="B34" s="62" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C34" s="63"/>
       <c r="D34" s="63"/>
@@ -45302,7 +45303,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -45735,7 +45736,7 @@
   <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10" defaultRowHeight="12.75"/>
@@ -45766,7 +45767,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="100" t="s">
-        <v>65</v>
+        <v>84</v>
       </c>
       <c r="C4" s="101"/>
       <c r="D4" s="101"/>
@@ -45898,7 +45899,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="96" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C4" s="98"/>
     </row>

</xml_diff>

<commit_message>
updated LPI and LPNI to highlight nonzero values on the system data sheet
git-svn-id: svn://107.170.10.188:8080/Semoss/trunk@2564 ef391c1c-ee15-45f7-b1d6-dde3d27a2169

Former-commit-id: 61edf92ddb00c0517a31b953ddcaac2b3a56255a
</commit_message>
<xml_diff>
--- a/export/Reports/Individual_System_LPI_Transition_Report_Template.xlsx
+++ b/export/Reports/Individual_System_LPI_Transition_Report_Template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="1110" windowWidth="15120" windowHeight="6405" tabRatio="834" firstSheet="3" activeTab="9"/>
+    <workbookView xWindow="240" yWindow="1110" windowWidth="15120" windowHeight="6405" tabRatio="834"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="33" r:id="rId1"/>
@@ -973,6 +973,33 @@
     <xf numFmtId="0" fontId="25" fillId="6" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="5" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="7" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="10" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="3" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="5" borderId="5" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1000,15 +1027,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="4" borderId="5" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1018,28 +1036,10 @@
     <xf numFmtId="0" fontId="17" fillId="4" borderId="7" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="10" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="5" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="7" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="3" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1397,11 +1397,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="417183784"/>
-        <c:axId val="417183392"/>
+        <c:axId val="419035744"/>
+        <c:axId val="419036136"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="417183784"/>
+        <c:axId val="419035744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1411,7 +1411,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="417183392"/>
+        <c:crossAx val="419036136"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1419,7 +1419,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="417183392"/>
+        <c:axId val="419036136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1430,7 +1430,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="417183784"/>
+        <c:crossAx val="419035744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1563,11 +1563,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="441473776"/>
-        <c:axId val="441474168"/>
+        <c:axId val="419038488"/>
+        <c:axId val="419038880"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="441473776"/>
+        <c:axId val="419038488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1577,7 +1577,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="441474168"/>
+        <c:crossAx val="419038880"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1585,7 +1585,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="441474168"/>
+        <c:axId val="419038880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1596,7 +1596,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="441473776"/>
+        <c:crossAx val="419038488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1838,11 +1838,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="441474952"/>
-        <c:axId val="441475344"/>
+        <c:axId val="419038096"/>
+        <c:axId val="419037704"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="441474952"/>
+        <c:axId val="419038096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1852,7 +1852,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="441475344"/>
+        <c:crossAx val="419037704"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1860,7 +1860,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="441475344"/>
+        <c:axId val="419037704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1871,7 +1871,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="441474952"/>
+        <c:crossAx val="419038096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -44211,7 +44211,7 @@
   </sheetPr>
   <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="A4" sqref="A4:L4"/>
     </sheetView>
   </sheetViews>
@@ -44386,7 +44386,7 @@
   </sheetPr>
   <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
@@ -44575,22 +44575,22 @@
     <row r="1" spans="1:13" ht="7.5" customHeight="1"/>
     <row r="2" spans="1:13" s="4" customFormat="1" ht="250.5" customHeight="1">
       <c r="A2" s="3"/>
-      <c r="B2" s="79" t="s">
+      <c r="B2" s="59" t="s">
         <v>36</v>
       </c>
-      <c r="C2" s="80"/>
-      <c r="D2" s="68" t="s">
+      <c r="C2" s="60"/>
+      <c r="D2" s="61" t="s">
         <v>37</v>
       </c>
-      <c r="E2" s="69"/>
-      <c r="F2" s="69"/>
-      <c r="G2" s="69"/>
-      <c r="H2" s="69"/>
-      <c r="I2" s="69"/>
-      <c r="J2" s="69"/>
-      <c r="K2" s="69"/>
-      <c r="L2" s="69"/>
-      <c r="M2" s="70"/>
+      <c r="E2" s="62"/>
+      <c r="F2" s="62"/>
+      <c r="G2" s="62"/>
+      <c r="H2" s="62"/>
+      <c r="I2" s="62"/>
+      <c r="J2" s="62"/>
+      <c r="K2" s="62"/>
+      <c r="L2" s="62"/>
+      <c r="M2" s="63"/>
     </row>
     <row r="3" spans="1:13" s="20" customFormat="1" ht="7.5" customHeight="1">
       <c r="A3" s="16"/>
@@ -44648,22 +44648,22 @@
     </row>
     <row r="7" spans="1:13" s="4" customFormat="1" ht="375" customHeight="1">
       <c r="A7" s="3"/>
-      <c r="B7" s="79" t="s">
+      <c r="B7" s="59" t="s">
         <v>30</v>
       </c>
-      <c r="C7" s="80"/>
-      <c r="D7" s="68" t="s">
+      <c r="C7" s="60"/>
+      <c r="D7" s="61" t="s">
         <v>61</v>
       </c>
-      <c r="E7" s="69"/>
-      <c r="F7" s="69"/>
-      <c r="G7" s="69"/>
-      <c r="H7" s="69"/>
-      <c r="I7" s="69"/>
-      <c r="J7" s="69"/>
-      <c r="K7" s="69"/>
-      <c r="L7" s="69"/>
-      <c r="M7" s="70"/>
+      <c r="E7" s="62"/>
+      <c r="F7" s="62"/>
+      <c r="G7" s="62"/>
+      <c r="H7" s="62"/>
+      <c r="I7" s="62"/>
+      <c r="J7" s="62"/>
+      <c r="K7" s="62"/>
+      <c r="L7" s="62"/>
+      <c r="M7" s="63"/>
     </row>
     <row r="8" spans="1:13" ht="8.25" customHeight="1">
       <c r="A8" s="5"/>
@@ -44674,112 +44674,112 @@
     </row>
     <row r="9" spans="1:13" s="8" customFormat="1" ht="18" customHeight="1">
       <c r="A9" s="7"/>
-      <c r="B9" s="59" t="s">
+      <c r="B9" s="68" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="60"/>
-      <c r="D9" s="60"/>
-      <c r="E9" s="60"/>
-      <c r="F9" s="60"/>
-      <c r="G9" s="60"/>
-      <c r="H9" s="60"/>
-      <c r="I9" s="60"/>
-      <c r="J9" s="60"/>
-      <c r="K9" s="60"/>
-      <c r="L9" s="60"/>
-      <c r="M9" s="61"/>
+      <c r="C9" s="69"/>
+      <c r="D9" s="69"/>
+      <c r="E9" s="69"/>
+      <c r="F9" s="69"/>
+      <c r="G9" s="69"/>
+      <c r="H9" s="69"/>
+      <c r="I9" s="69"/>
+      <c r="J9" s="69"/>
+      <c r="K9" s="69"/>
+      <c r="L9" s="69"/>
+      <c r="M9" s="70"/>
     </row>
     <row r="10" spans="1:13" s="8" customFormat="1" ht="28.5" customHeight="1">
       <c r="A10" s="7"/>
-      <c r="B10" s="74" t="s">
+      <c r="B10" s="64" t="s">
         <v>0</v>
       </c>
-      <c r="C10" s="74"/>
-      <c r="D10" s="74" t="s">
+      <c r="C10" s="64"/>
+      <c r="D10" s="64" t="s">
         <v>5</v>
       </c>
-      <c r="E10" s="81"/>
-      <c r="F10" s="74" t="s">
+      <c r="E10" s="67"/>
+      <c r="F10" s="64" t="s">
         <v>47</v>
       </c>
-      <c r="G10" s="74"/>
-      <c r="H10" s="75" t="s">
+      <c r="G10" s="64"/>
+      <c r="H10" s="80" t="s">
         <v>48</v>
       </c>
-      <c r="I10" s="76"/>
-      <c r="J10" s="74" t="s">
+      <c r="I10" s="81"/>
+      <c r="J10" s="64" t="s">
         <v>49</v>
       </c>
-      <c r="K10" s="74"/>
-      <c r="L10" s="74" t="s">
+      <c r="K10" s="64"/>
+      <c r="L10" s="64" t="s">
         <v>1</v>
       </c>
-      <c r="M10" s="74"/>
+      <c r="M10" s="64"/>
     </row>
     <row r="11" spans="1:13" ht="42.75" customHeight="1">
       <c r="A11" s="5"/>
-      <c r="B11" s="77"/>
-      <c r="C11" s="78"/>
-      <c r="D11" s="77"/>
-      <c r="E11" s="78"/>
-      <c r="F11" s="77"/>
-      <c r="G11" s="78"/>
-      <c r="H11" s="77"/>
-      <c r="I11" s="78"/>
-      <c r="J11" s="77"/>
-      <c r="K11" s="78"/>
-      <c r="L11" s="77"/>
-      <c r="M11" s="78"/>
+      <c r="B11" s="65"/>
+      <c r="C11" s="66"/>
+      <c r="D11" s="65"/>
+      <c r="E11" s="66"/>
+      <c r="F11" s="65"/>
+      <c r="G11" s="66"/>
+      <c r="H11" s="65"/>
+      <c r="I11" s="66"/>
+      <c r="J11" s="65"/>
+      <c r="K11" s="66"/>
+      <c r="L11" s="65"/>
+      <c r="M11" s="66"/>
     </row>
     <row r="13" spans="1:13" ht="16.5">
-      <c r="B13" s="59" t="s">
+      <c r="B13" s="68" t="s">
         <v>66</v>
       </c>
-      <c r="C13" s="60"/>
-      <c r="D13" s="60"/>
-      <c r="E13" s="60"/>
-      <c r="F13" s="60"/>
-      <c r="G13" s="60"/>
-      <c r="H13" s="60"/>
-      <c r="I13" s="60"/>
-      <c r="J13" s="60"/>
-      <c r="K13" s="60"/>
-      <c r="L13" s="60"/>
-      <c r="M13" s="61"/>
+      <c r="C13" s="69"/>
+      <c r="D13" s="69"/>
+      <c r="E13" s="69"/>
+      <c r="F13" s="69"/>
+      <c r="G13" s="69"/>
+      <c r="H13" s="69"/>
+      <c r="I13" s="69"/>
+      <c r="J13" s="69"/>
+      <c r="K13" s="69"/>
+      <c r="L13" s="69"/>
+      <c r="M13" s="70"/>
     </row>
     <row r="14" spans="1:13" ht="51" customHeight="1">
-      <c r="B14" s="65" t="s">
+      <c r="B14" s="74" t="s">
         <v>83</v>
       </c>
-      <c r="C14" s="66"/>
-      <c r="D14" s="66"/>
-      <c r="E14" s="66"/>
-      <c r="F14" s="66"/>
-      <c r="G14" s="66"/>
-      <c r="H14" s="66"/>
-      <c r="I14" s="66"/>
-      <c r="J14" s="66"/>
-      <c r="K14" s="66"/>
-      <c r="L14" s="66"/>
-      <c r="M14" s="67"/>
+      <c r="C14" s="75"/>
+      <c r="D14" s="75"/>
+      <c r="E14" s="75"/>
+      <c r="F14" s="75"/>
+      <c r="G14" s="75"/>
+      <c r="H14" s="75"/>
+      <c r="I14" s="75"/>
+      <c r="J14" s="75"/>
+      <c r="K14" s="75"/>
+      <c r="L14" s="75"/>
+      <c r="M14" s="76"/>
     </row>
     <row r="15" spans="1:13">
-      <c r="B15" s="71" t="s">
+      <c r="B15" s="77" t="s">
         <v>69</v>
       </c>
-      <c r="C15" s="72"/>
-      <c r="D15" s="72"/>
-      <c r="E15" s="72"/>
-      <c r="F15" s="72"/>
-      <c r="G15" s="73"/>
-      <c r="H15" s="71" t="s">
+      <c r="C15" s="78"/>
+      <c r="D15" s="78"/>
+      <c r="E15" s="78"/>
+      <c r="F15" s="78"/>
+      <c r="G15" s="79"/>
+      <c r="H15" s="77" t="s">
         <v>75</v>
       </c>
-      <c r="I15" s="72"/>
-      <c r="J15" s="72"/>
-      <c r="K15" s="72"/>
-      <c r="L15" s="72"/>
-      <c r="M15" s="73"/>
+      <c r="I15" s="78"/>
+      <c r="J15" s="78"/>
+      <c r="K15" s="78"/>
+      <c r="L15" s="78"/>
+      <c r="M15" s="79"/>
     </row>
     <row r="16" spans="1:13">
       <c r="B16" s="42"/>
@@ -45006,36 +45006,36 @@
       <c r="M31" s="50"/>
     </row>
     <row r="33" spans="2:13" ht="16.5">
-      <c r="B33" s="59" t="s">
+      <c r="B33" s="68" t="s">
         <v>76</v>
       </c>
-      <c r="C33" s="60"/>
-      <c r="D33" s="60"/>
-      <c r="E33" s="60"/>
-      <c r="F33" s="60"/>
-      <c r="G33" s="60"/>
-      <c r="H33" s="60"/>
-      <c r="I33" s="60"/>
-      <c r="J33" s="60"/>
-      <c r="K33" s="60"/>
-      <c r="L33" s="60"/>
-      <c r="M33" s="61"/>
+      <c r="C33" s="69"/>
+      <c r="D33" s="69"/>
+      <c r="E33" s="69"/>
+      <c r="F33" s="69"/>
+      <c r="G33" s="69"/>
+      <c r="H33" s="69"/>
+      <c r="I33" s="69"/>
+      <c r="J33" s="69"/>
+      <c r="K33" s="69"/>
+      <c r="L33" s="69"/>
+      <c r="M33" s="70"/>
     </row>
     <row r="34" spans="2:13" ht="33.75" customHeight="1">
-      <c r="B34" s="62" t="s">
+      <c r="B34" s="71" t="s">
         <v>82</v>
       </c>
-      <c r="C34" s="63"/>
-      <c r="D34" s="63"/>
-      <c r="E34" s="63"/>
-      <c r="F34" s="63"/>
-      <c r="G34" s="63"/>
-      <c r="H34" s="63"/>
-      <c r="I34" s="63"/>
-      <c r="J34" s="63"/>
-      <c r="K34" s="63"/>
-      <c r="L34" s="63"/>
-      <c r="M34" s="64"/>
+      <c r="C34" s="72"/>
+      <c r="D34" s="72"/>
+      <c r="E34" s="72"/>
+      <c r="F34" s="72"/>
+      <c r="G34" s="72"/>
+      <c r="H34" s="72"/>
+      <c r="I34" s="72"/>
+      <c r="J34" s="72"/>
+      <c r="K34" s="72"/>
+      <c r="L34" s="72"/>
+      <c r="M34" s="73"/>
     </row>
     <row r="35" spans="2:13">
       <c r="B35" s="42"/>
@@ -45263,6 +45263,17 @@
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="B33:M33"/>
+    <mergeCell ref="B34:M34"/>
+    <mergeCell ref="B14:M14"/>
+    <mergeCell ref="D7:M7"/>
+    <mergeCell ref="B9:M9"/>
+    <mergeCell ref="B13:M13"/>
+    <mergeCell ref="B15:G15"/>
+    <mergeCell ref="H15:M15"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="B11:C11"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B4:M4"/>
     <mergeCell ref="D2:M2"/>
@@ -45276,17 +45287,6 @@
     <mergeCell ref="J10:K10"/>
     <mergeCell ref="D10:E10"/>
     <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B33:M33"/>
-    <mergeCell ref="B34:M34"/>
-    <mergeCell ref="B14:M14"/>
-    <mergeCell ref="D7:M7"/>
-    <mergeCell ref="B9:M9"/>
-    <mergeCell ref="B13:M13"/>
-    <mergeCell ref="B15:G15"/>
-    <mergeCell ref="H15:M15"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="B11:C11"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
changed comment to recommendation
git-svn-id: svn://107.170.10.188:8080/Semoss/trunk@2574 ef391c1c-ee15-45f7-b1d6-dde3d27a2169
</commit_message>
<xml_diff>
--- a/export/Reports/Individual_System_LPI_Transition_Report_Template.xlsx
+++ b/export/Reports/Individual_System_LPI_Transition_Report_Template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="1110" windowWidth="15120" windowHeight="6405" tabRatio="834"/>
+    <workbookView xWindow="240" yWindow="1110" windowWidth="15120" windowHeight="6405" tabRatio="834" firstSheet="3" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="33" r:id="rId1"/>
@@ -157,9 +157,6 @@
   </si>
   <si>
     <t>Protocol</t>
-  </si>
-  <si>
-    <t>Comment</t>
   </si>
   <si>
     <t>Software Lifecycles</t>
@@ -400,6 +397,9 @@
   </si>
   <si>
     <t>This section displays the data objects that @SYSTEM@ is a source of record of and the numbers of systems which @SYSTEM@ sends the data to. Additionally, this section displays the data objects that @SYSTEM@ consumes, the other systems that are a source of the data object and the number of low probability systems they provide data for.</t>
+  </si>
+  <si>
+    <t>Recommendation</t>
   </si>
 </sst>
 </file>
@@ -973,33 +973,6 @@
     <xf numFmtId="0" fontId="25" fillId="6" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="5" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="7" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="10" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="3" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="5" borderId="5" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1027,6 +1000,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="4" borderId="5" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1036,10 +1018,28 @@
     <xf numFmtId="0" fontId="17" fillId="4" borderId="7" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="10" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="5" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="7" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="3" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1397,11 +1397,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="419035744"/>
-        <c:axId val="419036136"/>
+        <c:axId val="447537528"/>
+        <c:axId val="447537920"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="419035744"/>
+        <c:axId val="447537528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1411,7 +1411,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="419036136"/>
+        <c:crossAx val="447537920"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1419,7 +1419,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="419036136"/>
+        <c:axId val="447537920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1430,7 +1430,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="419035744"/>
+        <c:crossAx val="447537528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1563,11 +1563,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="419038488"/>
-        <c:axId val="419038880"/>
+        <c:axId val="409967408"/>
+        <c:axId val="409967016"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="419038488"/>
+        <c:axId val="409967408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1577,7 +1577,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="419038880"/>
+        <c:crossAx val="409967016"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1585,7 +1585,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="419038880"/>
+        <c:axId val="409967016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1596,7 +1596,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="419038488"/>
+        <c:crossAx val="409967408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1838,11 +1838,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="419038096"/>
-        <c:axId val="419037704"/>
+        <c:axId val="409967800"/>
+        <c:axId val="447538704"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="419038096"/>
+        <c:axId val="409967800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1852,7 +1852,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="419037704"/>
+        <c:crossAx val="447538704"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1860,7 +1860,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="419037704"/>
+        <c:axId val="447538704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1871,7 +1871,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="419038096"/>
+        <c:crossAx val="409967800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -44211,7 +44211,7 @@
   </sheetPr>
   <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="A4" sqref="A4:L4"/>
     </sheetView>
   </sheetViews>
@@ -44225,12 +44225,12 @@
   <sheetData>
     <row r="1" spans="1:12" s="1" customFormat="1" ht="7.5" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="32.25" customHeight="1">
       <c r="A2" s="51" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B2" s="52"/>
       <c r="C2" s="52"/>
@@ -44246,12 +44246,12 @@
     </row>
     <row r="3" spans="1:12" s="1" customFormat="1" ht="7.5" customHeight="1">
       <c r="A3" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="281.25" customHeight="1">
       <c r="A4" s="53" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B4" s="54"/>
       <c r="C4" s="54"/>
@@ -44267,12 +44267,12 @@
     </row>
     <row r="5" spans="1:12" s="1" customFormat="1" ht="7.5" customHeight="1">
       <c r="A5" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:12" s="32" customFormat="1" ht="29.25" customHeight="1">
       <c r="A6" s="51" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B6" s="52"/>
       <c r="C6" s="52"/>
@@ -44288,12 +44288,12 @@
     </row>
     <row r="7" spans="1:12" s="1" customFormat="1" ht="7.5" customHeight="1">
       <c r="A7" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="134.25" customHeight="1">
       <c r="A8" s="56" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B8" s="57"/>
       <c r="C8" s="57"/>
@@ -44398,21 +44398,21 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="41" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="39" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B3" s="39" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C3" s="38"/>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="40" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B4" s="40">
         <v>0</v>
@@ -44420,7 +44420,7 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="40" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B5" s="40">
         <v>0</v>
@@ -44428,7 +44428,7 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="40" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B6" s="40">
         <v>0</v>
@@ -44436,7 +44436,7 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="40" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B7" s="40">
         <v>0</v>
@@ -44444,20 +44444,20 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="41" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="39" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B11" s="39" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="40" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B12" s="40">
         <v>0</v>
@@ -44465,7 +44465,7 @@
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="40" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B13" s="40">
         <v>0</v>
@@ -44473,7 +44473,7 @@
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="40" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B14" s="40">
         <v>0</v>
@@ -44481,7 +44481,7 @@
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="40" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B15" s="40">
         <v>0</v>
@@ -44489,7 +44489,7 @@
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="41" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -44497,12 +44497,12 @@
         <v>2</v>
       </c>
       <c r="B19" s="39" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="40" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B20" s="40">
         <v>0</v>
@@ -44510,7 +44510,7 @@
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="40" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B21" s="40">
         <v>0</v>
@@ -44518,7 +44518,7 @@
     </row>
     <row r="22" spans="1:2">
       <c r="A22" s="40" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B22" s="40">
         <v>0</v>
@@ -44526,7 +44526,7 @@
     </row>
     <row r="23" spans="1:2">
       <c r="A23" s="40" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B23" s="40">
         <v>0</v>
@@ -44534,7 +44534,7 @@
     </row>
     <row r="24" spans="1:2">
       <c r="A24" s="40" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B24" s="40">
         <v>0</v>
@@ -44575,22 +44575,22 @@
     <row r="1" spans="1:13" ht="7.5" customHeight="1"/>
     <row r="2" spans="1:13" s="4" customFormat="1" ht="250.5" customHeight="1">
       <c r="A2" s="3"/>
-      <c r="B2" s="59" t="s">
+      <c r="B2" s="79" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" s="80"/>
+      <c r="D2" s="68" t="s">
         <v>36</v>
       </c>
-      <c r="C2" s="60"/>
-      <c r="D2" s="61" t="s">
-        <v>37</v>
-      </c>
-      <c r="E2" s="62"/>
-      <c r="F2" s="62"/>
-      <c r="G2" s="62"/>
-      <c r="H2" s="62"/>
-      <c r="I2" s="62"/>
-      <c r="J2" s="62"/>
-      <c r="K2" s="62"/>
-      <c r="L2" s="62"/>
-      <c r="M2" s="63"/>
+      <c r="E2" s="69"/>
+      <c r="F2" s="69"/>
+      <c r="G2" s="69"/>
+      <c r="H2" s="69"/>
+      <c r="I2" s="69"/>
+      <c r="J2" s="69"/>
+      <c r="K2" s="69"/>
+      <c r="L2" s="69"/>
+      <c r="M2" s="70"/>
     </row>
     <row r="3" spans="1:13" s="20" customFormat="1" ht="7.5" customHeight="1">
       <c r="A3" s="16"/>
@@ -44610,7 +44610,7 @@
     <row r="4" spans="1:13" ht="32.25" customHeight="1">
       <c r="A4" s="5"/>
       <c r="B4" s="51" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C4" s="52"/>
       <c r="D4" s="52"/>
@@ -44648,22 +44648,22 @@
     </row>
     <row r="7" spans="1:13" s="4" customFormat="1" ht="375" customHeight="1">
       <c r="A7" s="3"/>
-      <c r="B7" s="59" t="s">
-        <v>30</v>
+      <c r="B7" s="79" t="s">
+        <v>29</v>
       </c>
-      <c r="C7" s="60"/>
-      <c r="D7" s="61" t="s">
-        <v>61</v>
+      <c r="C7" s="80"/>
+      <c r="D7" s="68" t="s">
+        <v>60</v>
       </c>
-      <c r="E7" s="62"/>
-      <c r="F7" s="62"/>
-      <c r="G7" s="62"/>
-      <c r="H7" s="62"/>
-      <c r="I7" s="62"/>
-      <c r="J7" s="62"/>
-      <c r="K7" s="62"/>
-      <c r="L7" s="62"/>
-      <c r="M7" s="63"/>
+      <c r="E7" s="69"/>
+      <c r="F7" s="69"/>
+      <c r="G7" s="69"/>
+      <c r="H7" s="69"/>
+      <c r="I7" s="69"/>
+      <c r="J7" s="69"/>
+      <c r="K7" s="69"/>
+      <c r="L7" s="69"/>
+      <c r="M7" s="70"/>
     </row>
     <row r="8" spans="1:13" ht="8.25" customHeight="1">
       <c r="A8" s="5"/>
@@ -44674,112 +44674,112 @@
     </row>
     <row r="9" spans="1:13" s="8" customFormat="1" ht="18" customHeight="1">
       <c r="A9" s="7"/>
-      <c r="B9" s="68" t="s">
+      <c r="B9" s="59" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="69"/>
-      <c r="D9" s="69"/>
-      <c r="E9" s="69"/>
-      <c r="F9" s="69"/>
-      <c r="G9" s="69"/>
-      <c r="H9" s="69"/>
-      <c r="I9" s="69"/>
-      <c r="J9" s="69"/>
-      <c r="K9" s="69"/>
-      <c r="L9" s="69"/>
-      <c r="M9" s="70"/>
+      <c r="C9" s="60"/>
+      <c r="D9" s="60"/>
+      <c r="E9" s="60"/>
+      <c r="F9" s="60"/>
+      <c r="G9" s="60"/>
+      <c r="H9" s="60"/>
+      <c r="I9" s="60"/>
+      <c r="J9" s="60"/>
+      <c r="K9" s="60"/>
+      <c r="L9" s="60"/>
+      <c r="M9" s="61"/>
     </row>
     <row r="10" spans="1:13" s="8" customFormat="1" ht="28.5" customHeight="1">
       <c r="A10" s="7"/>
-      <c r="B10" s="64" t="s">
+      <c r="B10" s="74" t="s">
         <v>0</v>
       </c>
-      <c r="C10" s="64"/>
-      <c r="D10" s="64" t="s">
+      <c r="C10" s="74"/>
+      <c r="D10" s="74" t="s">
         <v>5</v>
       </c>
-      <c r="E10" s="67"/>
-      <c r="F10" s="64" t="s">
+      <c r="E10" s="81"/>
+      <c r="F10" s="74" t="s">
+        <v>46</v>
+      </c>
+      <c r="G10" s="74"/>
+      <c r="H10" s="75" t="s">
         <v>47</v>
       </c>
-      <c r="G10" s="64"/>
-      <c r="H10" s="80" t="s">
+      <c r="I10" s="76"/>
+      <c r="J10" s="74" t="s">
         <v>48</v>
       </c>
-      <c r="I10" s="81"/>
-      <c r="J10" s="64" t="s">
-        <v>49</v>
-      </c>
-      <c r="K10" s="64"/>
-      <c r="L10" s="64" t="s">
+      <c r="K10" s="74"/>
+      <c r="L10" s="74" t="s">
         <v>1</v>
       </c>
-      <c r="M10" s="64"/>
+      <c r="M10" s="74"/>
     </row>
     <row r="11" spans="1:13" ht="42.75" customHeight="1">
       <c r="A11" s="5"/>
-      <c r="B11" s="65"/>
-      <c r="C11" s="66"/>
-      <c r="D11" s="65"/>
-      <c r="E11" s="66"/>
-      <c r="F11" s="65"/>
-      <c r="G11" s="66"/>
-      <c r="H11" s="65"/>
-      <c r="I11" s="66"/>
-      <c r="J11" s="65"/>
-      <c r="K11" s="66"/>
-      <c r="L11" s="65"/>
-      <c r="M11" s="66"/>
+      <c r="B11" s="77"/>
+      <c r="C11" s="78"/>
+      <c r="D11" s="77"/>
+      <c r="E11" s="78"/>
+      <c r="F11" s="77"/>
+      <c r="G11" s="78"/>
+      <c r="H11" s="77"/>
+      <c r="I11" s="78"/>
+      <c r="J11" s="77"/>
+      <c r="K11" s="78"/>
+      <c r="L11" s="77"/>
+      <c r="M11" s="78"/>
     </row>
     <row r="13" spans="1:13" ht="16.5">
-      <c r="B13" s="68" t="s">
-        <v>66</v>
+      <c r="B13" s="59" t="s">
+        <v>65</v>
       </c>
-      <c r="C13" s="69"/>
-      <c r="D13" s="69"/>
-      <c r="E13" s="69"/>
-      <c r="F13" s="69"/>
-      <c r="G13" s="69"/>
-      <c r="H13" s="69"/>
-      <c r="I13" s="69"/>
-      <c r="J13" s="69"/>
-      <c r="K13" s="69"/>
-      <c r="L13" s="69"/>
-      <c r="M13" s="70"/>
+      <c r="C13" s="60"/>
+      <c r="D13" s="60"/>
+      <c r="E13" s="60"/>
+      <c r="F13" s="60"/>
+      <c r="G13" s="60"/>
+      <c r="H13" s="60"/>
+      <c r="I13" s="60"/>
+      <c r="J13" s="60"/>
+      <c r="K13" s="60"/>
+      <c r="L13" s="60"/>
+      <c r="M13" s="61"/>
     </row>
     <row r="14" spans="1:13" ht="51" customHeight="1">
-      <c r="B14" s="74" t="s">
-        <v>83</v>
+      <c r="B14" s="65" t="s">
+        <v>82</v>
       </c>
-      <c r="C14" s="75"/>
-      <c r="D14" s="75"/>
-      <c r="E14" s="75"/>
-      <c r="F14" s="75"/>
-      <c r="G14" s="75"/>
-      <c r="H14" s="75"/>
-      <c r="I14" s="75"/>
-      <c r="J14" s="75"/>
-      <c r="K14" s="75"/>
-      <c r="L14" s="75"/>
-      <c r="M14" s="76"/>
+      <c r="C14" s="66"/>
+      <c r="D14" s="66"/>
+      <c r="E14" s="66"/>
+      <c r="F14" s="66"/>
+      <c r="G14" s="66"/>
+      <c r="H14" s="66"/>
+      <c r="I14" s="66"/>
+      <c r="J14" s="66"/>
+      <c r="K14" s="66"/>
+      <c r="L14" s="66"/>
+      <c r="M14" s="67"/>
     </row>
     <row r="15" spans="1:13">
-      <c r="B15" s="77" t="s">
-        <v>69</v>
+      <c r="B15" s="71" t="s">
+        <v>68</v>
       </c>
-      <c r="C15" s="78"/>
-      <c r="D15" s="78"/>
-      <c r="E15" s="78"/>
-      <c r="F15" s="78"/>
-      <c r="G15" s="79"/>
-      <c r="H15" s="77" t="s">
-        <v>75</v>
+      <c r="C15" s="72"/>
+      <c r="D15" s="72"/>
+      <c r="E15" s="72"/>
+      <c r="F15" s="72"/>
+      <c r="G15" s="73"/>
+      <c r="H15" s="71" t="s">
+        <v>74</v>
       </c>
-      <c r="I15" s="78"/>
-      <c r="J15" s="78"/>
-      <c r="K15" s="78"/>
-      <c r="L15" s="78"/>
-      <c r="M15" s="79"/>
+      <c r="I15" s="72"/>
+      <c r="J15" s="72"/>
+      <c r="K15" s="72"/>
+      <c r="L15" s="72"/>
+      <c r="M15" s="73"/>
     </row>
     <row r="16" spans="1:13">
       <c r="B16" s="42"/>
@@ -45006,36 +45006,36 @@
       <c r="M31" s="50"/>
     </row>
     <row r="33" spans="2:13" ht="16.5">
-      <c r="B33" s="68" t="s">
-        <v>76</v>
+      <c r="B33" s="59" t="s">
+        <v>75</v>
       </c>
-      <c r="C33" s="69"/>
-      <c r="D33" s="69"/>
-      <c r="E33" s="69"/>
-      <c r="F33" s="69"/>
-      <c r="G33" s="69"/>
-      <c r="H33" s="69"/>
-      <c r="I33" s="69"/>
-      <c r="J33" s="69"/>
-      <c r="K33" s="69"/>
-      <c r="L33" s="69"/>
-      <c r="M33" s="70"/>
+      <c r="C33" s="60"/>
+      <c r="D33" s="60"/>
+      <c r="E33" s="60"/>
+      <c r="F33" s="60"/>
+      <c r="G33" s="60"/>
+      <c r="H33" s="60"/>
+      <c r="I33" s="60"/>
+      <c r="J33" s="60"/>
+      <c r="K33" s="60"/>
+      <c r="L33" s="60"/>
+      <c r="M33" s="61"/>
     </row>
     <row r="34" spans="2:13" ht="33.75" customHeight="1">
-      <c r="B34" s="71" t="s">
-        <v>82</v>
+      <c r="B34" s="62" t="s">
+        <v>81</v>
       </c>
-      <c r="C34" s="72"/>
-      <c r="D34" s="72"/>
-      <c r="E34" s="72"/>
-      <c r="F34" s="72"/>
-      <c r="G34" s="72"/>
-      <c r="H34" s="72"/>
-      <c r="I34" s="72"/>
-      <c r="J34" s="72"/>
-      <c r="K34" s="72"/>
-      <c r="L34" s="72"/>
-      <c r="M34" s="73"/>
+      <c r="C34" s="63"/>
+      <c r="D34" s="63"/>
+      <c r="E34" s="63"/>
+      <c r="F34" s="63"/>
+      <c r="G34" s="63"/>
+      <c r="H34" s="63"/>
+      <c r="I34" s="63"/>
+      <c r="J34" s="63"/>
+      <c r="K34" s="63"/>
+      <c r="L34" s="63"/>
+      <c r="M34" s="64"/>
     </row>
     <row r="35" spans="2:13">
       <c r="B35" s="42"/>
@@ -45263,17 +45263,6 @@
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="B33:M33"/>
-    <mergeCell ref="B34:M34"/>
-    <mergeCell ref="B14:M14"/>
-    <mergeCell ref="D7:M7"/>
-    <mergeCell ref="B9:M9"/>
-    <mergeCell ref="B13:M13"/>
-    <mergeCell ref="B15:G15"/>
-    <mergeCell ref="H15:M15"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="B11:C11"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B4:M4"/>
     <mergeCell ref="D2:M2"/>
@@ -45287,6 +45276,17 @@
     <mergeCell ref="J10:K10"/>
     <mergeCell ref="D10:E10"/>
     <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B33:M33"/>
+    <mergeCell ref="B34:M34"/>
+    <mergeCell ref="B14:M14"/>
+    <mergeCell ref="D7:M7"/>
+    <mergeCell ref="B9:M9"/>
+    <mergeCell ref="B13:M13"/>
+    <mergeCell ref="B15:G15"/>
+    <mergeCell ref="H15:M15"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="B11:C11"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -45320,12 +45320,12 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="18" customHeight="1">
       <c r="A2" s="82" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B2" s="82"/>
       <c r="C2" s="82"/>
@@ -45336,7 +45336,7 @@
     </row>
     <row r="3" spans="1:7" ht="18" customHeight="1">
       <c r="A3" s="88" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B3" s="88"/>
       <c r="C3" s="88"/>
@@ -45347,12 +45347,12 @@
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="25.5" customHeight="1">
       <c r="A5" s="89" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B5" s="90"/>
       <c r="C5" s="90"/>
@@ -45363,16 +45363,16 @@
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="18.75" customHeight="1">
       <c r="A7" s="86" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B7" s="87"/>
       <c r="C7" s="83" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D7" s="84"/>
       <c r="E7" s="84"/>
@@ -45381,30 +45381,30 @@
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="25.5">
       <c r="A9" s="35" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="35" t="s">
+        <v>49</v>
+      </c>
+      <c r="C9" s="35" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="35" t="s">
-        <v>50</v>
-      </c>
-      <c r="C9" s="35" t="s">
-        <v>28</v>
-      </c>
-      <c r="D9" s="35" t="s">
+      <c r="E9" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="E9" s="35" t="s">
+      <c r="F9" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="F9" s="35" t="s">
-        <v>20</v>
-      </c>
       <c r="G9" s="35" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -45418,7 +45418,7 @@
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -45460,7 +45460,7 @@
   <sheetData>
     <row r="2" spans="1:7" ht="18" customHeight="1">
       <c r="A2" s="92" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B2" s="93"/>
       <c r="C2" s="93"/>
@@ -45482,7 +45482,7 @@
     </row>
     <row r="5" spans="1:7" ht="25.5" customHeight="1">
       <c r="A5" s="89" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B5" s="90"/>
       <c r="C5" s="90"/>
@@ -45493,11 +45493,11 @@
     </row>
     <row r="7" spans="1:7" ht="18.75" customHeight="1">
       <c r="A7" s="88" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B7" s="88"/>
       <c r="C7" s="95" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D7" s="95"/>
       <c r="E7" s="95"/>
@@ -45506,25 +45506,25 @@
     </row>
     <row r="9" spans="1:7" ht="25.5">
       <c r="A9" s="35" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B9" s="35" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C9" s="35" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D9" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="E9" s="35" t="s">
+      <c r="F9" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="F9" s="35" t="s">
-        <v>20</v>
-      </c>
       <c r="G9" s="35" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -45571,7 +45571,7 @@
   <sheetData>
     <row r="2" spans="1:10" ht="18" customHeight="1">
       <c r="A2" s="99" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B2" s="99"/>
       <c r="C2" s="99"/>
@@ -45592,7 +45592,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="96" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C4" s="97"/>
       <c r="D4" s="97"/>
@@ -45633,12 +45633,12 @@
         <v>2022</v>
       </c>
       <c r="J6" s="35" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="41.25" customHeight="1">
       <c r="A7" s="35" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B7" s="24">
         <v>0</v>
@@ -45670,7 +45670,7 @@
     </row>
     <row r="8" spans="1:10" ht="41.25" customHeight="1">
       <c r="A8" s="35" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B8" s="24">
         <v>0</v>
@@ -45702,7 +45702,7 @@
     </row>
     <row r="10" spans="1:10" ht="41.25" customHeight="1">
       <c r="A10" s="35" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B10" s="25">
         <v>0</v>
@@ -45710,7 +45710,7 @@
     </row>
     <row r="11" spans="1:10" ht="41.25" customHeight="1">
       <c r="A11" s="35" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B11" s="25">
         <v>0</v>
@@ -45750,7 +45750,7 @@
     <row r="1" spans="1:10" ht="18" customHeight="1"/>
     <row r="2" spans="1:10" ht="18" customHeight="1">
       <c r="A2" s="99" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B2" s="99"/>
       <c r="C2" s="99"/>
@@ -45767,7 +45767,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="100" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C4" s="101"/>
       <c r="D4" s="101"/>
@@ -45783,7 +45783,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="35" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -45821,7 +45821,7 @@
   <sheetData>
     <row r="2" spans="1:2" ht="18">
       <c r="A2" s="99" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B2" s="99"/>
     </row>
@@ -45834,7 +45834,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -45884,7 +45884,7 @@
   <sheetData>
     <row r="2" spans="1:3" ht="18">
       <c r="A2" s="99" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B2" s="99"/>
       <c r="C2" s="99"/>
@@ -45899,7 +45899,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="96" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C4" s="98"/>
     </row>
@@ -45916,7 +45916,7 @@
         <v>6</v>
       </c>
       <c r="C6" s="35" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -45942,8 +45942,8 @@
   </sheetPr>
   <dimension ref="A1:M8"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" zoomScalePageLayoutView="80" workbookViewId="0">
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -45967,7 +45967,7 @@
     <row r="1" spans="1:13" ht="18" customHeight="1"/>
     <row r="2" spans="1:13" ht="18" customHeight="1">
       <c r="A2" s="99" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B2" s="99"/>
       <c r="C2" s="99"/>
@@ -45989,7 +45989,7 @@
       <c r="B4" s="104"/>
       <c r="C4" s="105"/>
       <c r="D4" s="106" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E4" s="107"/>
       <c r="F4" s="107"/>
@@ -46009,7 +46009,7 @@
         <v>10</v>
       </c>
       <c r="C6" s="35" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D6" s="35" t="s">
         <v>11</v>
@@ -46027,19 +46027,19 @@
         <v>14</v>
       </c>
       <c r="I6" s="35" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J6" s="35" t="s">
         <v>9</v>
       </c>
       <c r="K6" s="35" t="s">
-        <v>15</v>
+        <v>84</v>
       </c>
       <c r="L6" s="36" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M6" s="36" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:13">
@@ -46059,7 +46059,7 @@
     </row>
     <row r="8" spans="1:13">
       <c r="K8" s="27" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L8" s="26"/>
       <c r="M8" s="26"/>

</xml_diff>

<commit_message>
updated the LPI and LPNI reports
git-svn-id: svn://107.170.10.188:8080/Semoss/trunk@2627 ef391c1c-ee15-45f7-b1d6-dde3d27a2169
</commit_message>
<xml_diff>
--- a/export/Reports/Individual_System_LPI_Transition_Report_Template.xlsx
+++ b/export/Reports/Individual_System_LPI_Transition_Report_Template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="1110" windowWidth="15120" windowHeight="6405" tabRatio="834" firstSheet="3" activeTab="8"/>
+    <workbookView xWindow="240" yWindow="1110" windowWidth="15120" windowHeight="6405" tabRatio="834"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="33" r:id="rId1"/>
@@ -81,7 +81,7 @@
     <definedName name="_xlnm.Print_Titles" localSheetId="2">'Software Lifecycles'!$9:$9</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="6">'SOR Overlap With DHMSM'!$6:$6</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="5">'System Data'!$6:$6</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="8">'System Interfaces'!$6:$6</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="8">'System Interfaces'!$9:$9</definedName>
     <definedName name="Priority3">[6]Data1!$B$4:$B$6</definedName>
     <definedName name="ProcContractMonths">'[2]New Timeline'!$A$22</definedName>
     <definedName name="RangeBLU">[7]BLUBackEnd!$G$5:$G$49</definedName>
@@ -112,7 +112,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="90">
   <si>
     <t>Garrison / Theater</t>
   </si>
@@ -309,12 +309,6 @@
     <t>SOR Overlap with DHMSM</t>
   </si>
   <si>
-    <t xml:space="preserve"> - In 2011, MHS leadership initiated the DoD Health IT (HIT) Transition Application Plan (TAP) project. The project is designed to yield a comprehensive migration strategy with which to effectively and efficiently transition existing MHS program, projects and initiatives (PPI) to the future-state electronic health record (EHR) environment. The plan will synchronize the MHS’ technical, functional, infrastructure, and financial management processes of transitioning clinical and business functionalities to the future-state EHR.
-  - A March 14, 2014 memorandum signed by the by the Assistant Secretary of Defense for Health Affairs (ASD/HA) directed all DHA and Services stakeholders to provide information required to make transition decisions for the legacy systems in their portfolios. The TAP team, working directly with the Defense Health Clinical Systems (DHCS) and Defense Health Services (DHSS) Program Executive Offices, in addition to the tri-Services, collected functional, technical, and program management data for all systems identified in connection with the ASD/HA memorandum.
-- Using data provided by the DHA PEOs and Services to characterize the legacy enterprise, the TAP team provided transition recommendations for all identified legacy systems to the Functional Advisory Council (FAC). Based upon the clinical and business capabilities expected to be delviered by the future-state EHR solution and the analysis of the legacy systems provided by OTM, the FAC made decisions on how to transition the legacy systems in the DHA and Services portfolios to the future-state environment. The legacy systems were categorized as either having a low or high probability of being replaced by the future-state EHR solution.
-- This report focuses on the analysis of low probability systems that will require integration (LPI) with the future-state EHR. These systems will endure into the future and need to be modernized in order to maintain compliance with relevant DHA standards and ensure interoperability with the future-state EHR.</t>
-  </si>
-  <si>
     <t>Contents</t>
   </si>
   <si>
@@ -337,9 +331,6 @@
   </si>
   <si>
     <t>This section displays the cost to upgrade software and hardware that @SYSTEM@ uses as the modules reach end-of-life.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">This section displays @SYSTEM@ that are source of record for the data objects that DHMSM capabilities consume. </t>
   </si>
   <si>
     <t>System Maturity</t>
@@ -401,6 +392,30 @@
   <si>
     <t>Recommendation</t>
   </si>
+  <si>
+    <t xml:space="preserve"> - In 2011, MHS leadership initiated the DoD Health IT (HIT) Transition Application Plan (TAP) project. The project is designed to yield a comprehensive migration strategy with which to effectively and efficiently transition existing MHS program, projects and initiatives (PPI) to the future-state electronic health record (EHR) environment. The plan will synchronize the MHS’ technical, functional, infrastructure, and financial management processes of transitioning clinical and business functionalities to the future-state EHR.
+  - A March 14, 2014 memorandum signed by the Assistant Secretary of Defense for Health Affairs (ASD/HA) directed all DHA and Services stakeholders to provide information required to make transition decisions for the legacy systems in their portfolios. The TAP team, working directly with the Defense Health Clinical Systems (DHCS) and Defense Health Services (DHSS) Program Executive Offices, in addition to the tri-Services, collected functional, technical, and program management data for all systems identified in connection with the ASD/HA memorandum.
+- Using data provided by the DHA PEOs and Services to characterize the legacy enterprise, the TAP team provided transition recommendations for all identified legacy systems to the Functional Advisory Council (FAC). Based upon the clinical and business capabilities expected to be delivered by the future-state EHR solution and the analysis of the legacy systems provided by OTM, the FAC made decisions on how to transition the legacy systems in the DHA and Services portfolios to the future-state environment. The legacy systems were categorized as either having a low or high probability of being replaced by the future-state EHR solution.
+- This report focuses on the analysis of low probability systems that will require integration (LPI) with the future-state EHR. These systems will endure into the future and need to be modernized in order to maintain compliance with relevant DHA standards and ensure interoperability with the future-state EHR.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This section displays the data objects that @SYSTEM@ is the source of record for and that the DHMSM capability will be required to consume. </t>
+  </si>
+  <si>
+    <t>Legend</t>
+  </si>
+  <si>
+    <t>Direct Integration</t>
+  </si>
+  <si>
+    <t>Key</t>
+  </si>
+  <si>
+    <t>Indirect Integration</t>
+  </si>
+  <si>
+    <t>Removed Legacy Interfaces</t>
+  </si>
 </sst>
 </file>
 
@@ -410,7 +425,7 @@
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="27">
+  <fonts count="29">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -586,8 +601,20 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <name val="Impact"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -627,6 +654,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF366092"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -847,7 +880,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="109">
+  <cellXfs count="115">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -949,6 +982,9 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="48" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="9" xfId="48" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="13" xfId="48" applyBorder="1"/>
+    <xf numFmtId="0" fontId="28" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="7" borderId="5" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -972,6 +1008,33 @@
     </xf>
     <xf numFmtId="0" fontId="25" fillId="6" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="5" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="7" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="10" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="3" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="5" borderId="5" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1000,15 +1063,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="4" borderId="5" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1018,28 +1072,10 @@
     <xf numFmtId="0" fontId="17" fillId="4" borderId="7" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="10" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="5" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="7" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="3" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1105,6 +1141,30 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="8" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1113,15 +1173,6 @@
     </xf>
     <xf numFmtId="0" fontId="18" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="51">
@@ -1397,11 +1448,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="447537528"/>
-        <c:axId val="447537920"/>
+        <c:axId val="449411048"/>
+        <c:axId val="449411440"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="447537528"/>
+        <c:axId val="449411048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1411,7 +1462,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="447537920"/>
+        <c:crossAx val="449411440"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1419,7 +1470,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="447537920"/>
+        <c:axId val="449411440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1430,7 +1481,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="447537528"/>
+        <c:crossAx val="449411048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1563,11 +1614,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="409967408"/>
-        <c:axId val="409967016"/>
+        <c:axId val="417811168"/>
+        <c:axId val="417810776"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="409967408"/>
+        <c:axId val="417811168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1577,7 +1628,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="409967016"/>
+        <c:crossAx val="417810776"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1585,7 +1636,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="409967016"/>
+        <c:axId val="417810776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1596,7 +1647,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="409967408"/>
+        <c:crossAx val="417811168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1838,11 +1889,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="409967800"/>
-        <c:axId val="447538704"/>
+        <c:axId val="449412224"/>
+        <c:axId val="449412616"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="409967800"/>
+        <c:axId val="449412224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1852,7 +1903,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="447538704"/>
+        <c:crossAx val="449412616"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1860,7 +1911,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="447538704"/>
+        <c:axId val="449412616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1871,7 +1922,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="409967800"/>
+        <c:crossAx val="449412224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1982,6 +2033,201 @@
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1447800</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>229072</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1371798</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>1022840</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="18" name="Picture 17"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4000500" y="1267297"/>
+          <a:ext cx="2286198" cy="793768"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>200026</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>110190</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>940605</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>1141723</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="20" name="Picture 19"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7591426" y="1148415"/>
+          <a:ext cx="2531279" cy="1031533"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>462145</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>1194762</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="22" name="Picture 21"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12001500" y="1095375"/>
+          <a:ext cx="2538595" cy="1137612"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>70068</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>547921</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="25" name="Picture 24"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1885950" y="2324100"/>
+          <a:ext cx="6623268" cy="490771"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>228600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1467048</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>1022368</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1733550" y="1266825"/>
+          <a:ext cx="2286198" cy="793768"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -44208,10 +44454,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="6"/>
+    <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="A4" sqref="A4:L4"/>
     </sheetView>
   </sheetViews>
@@ -44229,20 +44476,20 @@
       </c>
     </row>
     <row r="2" spans="1:12" ht="32.25" customHeight="1">
-      <c r="A2" s="51" t="s">
+      <c r="A2" s="52" t="s">
         <v>55</v>
       </c>
-      <c r="B2" s="52"/>
-      <c r="C2" s="52"/>
-      <c r="D2" s="52"/>
-      <c r="E2" s="52"/>
-      <c r="F2" s="52"/>
-      <c r="G2" s="52"/>
-      <c r="H2" s="52"/>
-      <c r="I2" s="52"/>
-      <c r="J2" s="52"/>
-      <c r="K2" s="52"/>
-      <c r="L2" s="52"/>
+      <c r="B2" s="53"/>
+      <c r="C2" s="53"/>
+      <c r="D2" s="53"/>
+      <c r="E2" s="53"/>
+      <c r="F2" s="53"/>
+      <c r="G2" s="53"/>
+      <c r="H2" s="53"/>
+      <c r="I2" s="53"/>
+      <c r="J2" s="53"/>
+      <c r="K2" s="53"/>
+      <c r="L2" s="53"/>
     </row>
     <row r="3" spans="1:12" s="1" customFormat="1" ht="7.5" customHeight="1">
       <c r="A3" s="1" t="s">
@@ -44250,20 +44497,20 @@
       </c>
     </row>
     <row r="4" spans="1:12" ht="281.25" customHeight="1">
-      <c r="A4" s="53" t="s">
-        <v>57</v>
+      <c r="A4" s="54" t="s">
+        <v>83</v>
       </c>
-      <c r="B4" s="54"/>
-      <c r="C4" s="54"/>
-      <c r="D4" s="54"/>
-      <c r="E4" s="54"/>
-      <c r="F4" s="54"/>
-      <c r="G4" s="54"/>
-      <c r="H4" s="54"/>
-      <c r="I4" s="54"/>
-      <c r="J4" s="54"/>
-      <c r="K4" s="54"/>
-      <c r="L4" s="55"/>
+      <c r="B4" s="55"/>
+      <c r="C4" s="55"/>
+      <c r="D4" s="55"/>
+      <c r="E4" s="55"/>
+      <c r="F4" s="55"/>
+      <c r="G4" s="55"/>
+      <c r="H4" s="55"/>
+      <c r="I4" s="55"/>
+      <c r="J4" s="55"/>
+      <c r="K4" s="55"/>
+      <c r="L4" s="56"/>
     </row>
     <row r="5" spans="1:12" s="1" customFormat="1" ht="7.5" customHeight="1">
       <c r="A5" s="1" t="s">
@@ -44271,20 +44518,20 @@
       </c>
     </row>
     <row r="6" spans="1:12" s="32" customFormat="1" ht="29.25" customHeight="1">
-      <c r="A6" s="51" t="s">
-        <v>58</v>
+      <c r="A6" s="52" t="s">
+        <v>57</v>
       </c>
-      <c r="B6" s="52"/>
-      <c r="C6" s="52"/>
-      <c r="D6" s="52"/>
-      <c r="E6" s="52"/>
-      <c r="F6" s="52"/>
-      <c r="G6" s="52"/>
-      <c r="H6" s="52"/>
-      <c r="I6" s="52"/>
-      <c r="J6" s="52"/>
-      <c r="K6" s="52"/>
-      <c r="L6" s="52"/>
+      <c r="B6" s="53"/>
+      <c r="C6" s="53"/>
+      <c r="D6" s="53"/>
+      <c r="E6" s="53"/>
+      <c r="F6" s="53"/>
+      <c r="G6" s="53"/>
+      <c r="H6" s="53"/>
+      <c r="I6" s="53"/>
+      <c r="J6" s="53"/>
+      <c r="K6" s="53"/>
+      <c r="L6" s="53"/>
     </row>
     <row r="7" spans="1:12" s="1" customFormat="1" ht="7.5" customHeight="1">
       <c r="A7" s="1" t="s">
@@ -44292,20 +44539,20 @@
       </c>
     </row>
     <row r="8" spans="1:12" ht="134.25" customHeight="1">
-      <c r="A8" s="56" t="s">
-        <v>59</v>
+      <c r="A8" s="57" t="s">
+        <v>58</v>
       </c>
-      <c r="B8" s="57"/>
-      <c r="C8" s="57"/>
-      <c r="D8" s="57"/>
-      <c r="E8" s="57"/>
-      <c r="F8" s="57"/>
-      <c r="G8" s="57"/>
-      <c r="H8" s="57"/>
-      <c r="I8" s="57"/>
-      <c r="J8" s="57"/>
-      <c r="K8" s="57"/>
-      <c r="L8" s="58"/>
+      <c r="B8" s="58"/>
+      <c r="C8" s="58"/>
+      <c r="D8" s="58"/>
+      <c r="E8" s="58"/>
+      <c r="F8" s="58"/>
+      <c r="G8" s="58"/>
+      <c r="H8" s="58"/>
+      <c r="I8" s="58"/>
+      <c r="J8" s="58"/>
+      <c r="K8" s="58"/>
+      <c r="L8" s="59"/>
     </row>
     <row r="9" spans="1:12">
       <c r="A9" s="33"/>
@@ -44371,7 +44618,7 @@
     <mergeCell ref="A8:L8"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup scale="62" orientation="portrait" r:id="rId1"/>
+  <pageSetup scale="62" fitToHeight="0" orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0">
     <oddHeader>&amp;C&amp;F
 &amp;A</oddHeader>
@@ -44398,21 +44645,21 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="41" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="39" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B3" s="39" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C3" s="38"/>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="40" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B4" s="40">
         <v>0</v>
@@ -44420,7 +44667,7 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="40" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B5" s="40">
         <v>0</v>
@@ -44428,7 +44675,7 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="40" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B6" s="40">
         <v>0</v>
@@ -44436,7 +44683,7 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="40" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B7" s="40">
         <v>0</v>
@@ -44444,20 +44691,20 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="41" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="39" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B11" s="39" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="40" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B12" s="40">
         <v>0</v>
@@ -44465,7 +44712,7 @@
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="40" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B13" s="40">
         <v>0</v>
@@ -44473,7 +44720,7 @@
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="40" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B14" s="40">
         <v>0</v>
@@ -44481,7 +44728,7 @@
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="40" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B15" s="40">
         <v>0</v>
@@ -44489,7 +44736,7 @@
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="41" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -44497,12 +44744,12 @@
         <v>2</v>
       </c>
       <c r="B19" s="39" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="40" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B20" s="40">
         <v>0</v>
@@ -44510,7 +44757,7 @@
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="40" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B21" s="40">
         <v>0</v>
@@ -44518,7 +44765,7 @@
     </row>
     <row r="22" spans="1:2">
       <c r="A22" s="40" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B22" s="40">
         <v>0</v>
@@ -44526,7 +44773,7 @@
     </row>
     <row r="23" spans="1:2">
       <c r="A23" s="40" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B23" s="40">
         <v>0</v>
@@ -44534,7 +44781,7 @@
     </row>
     <row r="24" spans="1:2">
       <c r="A24" s="40" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B24" s="40">
         <v>0</v>
@@ -44554,9 +44801,7 @@
   </sheetPr>
   <dimension ref="A1:M50"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7:M7"/>
-    </sheetView>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -44575,22 +44820,22 @@
     <row r="1" spans="1:13" ht="7.5" customHeight="1"/>
     <row r="2" spans="1:13" s="4" customFormat="1" ht="250.5" customHeight="1">
       <c r="A2" s="3"/>
-      <c r="B2" s="79" t="s">
+      <c r="B2" s="60" t="s">
         <v>35</v>
       </c>
-      <c r="C2" s="80"/>
-      <c r="D2" s="68" t="s">
+      <c r="C2" s="61"/>
+      <c r="D2" s="62" t="s">
         <v>36</v>
       </c>
-      <c r="E2" s="69"/>
-      <c r="F2" s="69"/>
-      <c r="G2" s="69"/>
-      <c r="H2" s="69"/>
-      <c r="I2" s="69"/>
-      <c r="J2" s="69"/>
-      <c r="K2" s="69"/>
-      <c r="L2" s="69"/>
-      <c r="M2" s="70"/>
+      <c r="E2" s="63"/>
+      <c r="F2" s="63"/>
+      <c r="G2" s="63"/>
+      <c r="H2" s="63"/>
+      <c r="I2" s="63"/>
+      <c r="J2" s="63"/>
+      <c r="K2" s="63"/>
+      <c r="L2" s="63"/>
+      <c r="M2" s="64"/>
     </row>
     <row r="3" spans="1:13" s="20" customFormat="1" ht="7.5" customHeight="1">
       <c r="A3" s="16"/>
@@ -44609,20 +44854,20 @@
     </row>
     <row r="4" spans="1:13" ht="32.25" customHeight="1">
       <c r="A4" s="5"/>
-      <c r="B4" s="51" t="s">
+      <c r="B4" s="52" t="s">
         <v>34</v>
       </c>
-      <c r="C4" s="52"/>
-      <c r="D4" s="52"/>
-      <c r="E4" s="52"/>
-      <c r="F4" s="52"/>
-      <c r="G4" s="52"/>
-      <c r="H4" s="52"/>
-      <c r="I4" s="52"/>
-      <c r="J4" s="52"/>
-      <c r="K4" s="52"/>
-      <c r="L4" s="52"/>
-      <c r="M4" s="52"/>
+      <c r="C4" s="53"/>
+      <c r="D4" s="53"/>
+      <c r="E4" s="53"/>
+      <c r="F4" s="53"/>
+      <c r="G4" s="53"/>
+      <c r="H4" s="53"/>
+      <c r="I4" s="53"/>
+      <c r="J4" s="53"/>
+      <c r="K4" s="53"/>
+      <c r="L4" s="53"/>
+      <c r="M4" s="53"/>
     </row>
     <row r="5" spans="1:13" ht="7.5" customHeight="1">
       <c r="A5" s="5"/>
@@ -44648,22 +44893,22 @@
     </row>
     <row r="7" spans="1:13" s="4" customFormat="1" ht="375" customHeight="1">
       <c r="A7" s="3"/>
-      <c r="B7" s="79" t="s">
+      <c r="B7" s="60" t="s">
         <v>29</v>
       </c>
-      <c r="C7" s="80"/>
-      <c r="D7" s="68" t="s">
-        <v>60</v>
+      <c r="C7" s="61"/>
+      <c r="D7" s="62" t="s">
+        <v>59</v>
       </c>
-      <c r="E7" s="69"/>
-      <c r="F7" s="69"/>
-      <c r="G7" s="69"/>
-      <c r="H7" s="69"/>
-      <c r="I7" s="69"/>
-      <c r="J7" s="69"/>
-      <c r="K7" s="69"/>
-      <c r="L7" s="69"/>
-      <c r="M7" s="70"/>
+      <c r="E7" s="63"/>
+      <c r="F7" s="63"/>
+      <c r="G7" s="63"/>
+      <c r="H7" s="63"/>
+      <c r="I7" s="63"/>
+      <c r="J7" s="63"/>
+      <c r="K7" s="63"/>
+      <c r="L7" s="63"/>
+      <c r="M7" s="64"/>
     </row>
     <row r="8" spans="1:13" ht="8.25" customHeight="1">
       <c r="A8" s="5"/>
@@ -44674,112 +44919,112 @@
     </row>
     <row r="9" spans="1:13" s="8" customFormat="1" ht="18" customHeight="1">
       <c r="A9" s="7"/>
-      <c r="B9" s="59" t="s">
+      <c r="B9" s="69" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="60"/>
-      <c r="D9" s="60"/>
-      <c r="E9" s="60"/>
-      <c r="F9" s="60"/>
-      <c r="G9" s="60"/>
-      <c r="H9" s="60"/>
-      <c r="I9" s="60"/>
-      <c r="J9" s="60"/>
-      <c r="K9" s="60"/>
-      <c r="L9" s="60"/>
-      <c r="M9" s="61"/>
+      <c r="C9" s="70"/>
+      <c r="D9" s="70"/>
+      <c r="E9" s="70"/>
+      <c r="F9" s="70"/>
+      <c r="G9" s="70"/>
+      <c r="H9" s="70"/>
+      <c r="I9" s="70"/>
+      <c r="J9" s="70"/>
+      <c r="K9" s="70"/>
+      <c r="L9" s="70"/>
+      <c r="M9" s="71"/>
     </row>
     <row r="10" spans="1:13" s="8" customFormat="1" ht="28.5" customHeight="1">
       <c r="A10" s="7"/>
-      <c r="B10" s="74" t="s">
+      <c r="B10" s="65" t="s">
         <v>0</v>
       </c>
-      <c r="C10" s="74"/>
-      <c r="D10" s="74" t="s">
+      <c r="C10" s="65"/>
+      <c r="D10" s="65" t="s">
         <v>5</v>
       </c>
-      <c r="E10" s="81"/>
-      <c r="F10" s="74" t="s">
+      <c r="E10" s="68"/>
+      <c r="F10" s="65" t="s">
         <v>46</v>
       </c>
-      <c r="G10" s="74"/>
-      <c r="H10" s="75" t="s">
+      <c r="G10" s="65"/>
+      <c r="H10" s="81" t="s">
         <v>47</v>
       </c>
-      <c r="I10" s="76"/>
-      <c r="J10" s="74" t="s">
+      <c r="I10" s="82"/>
+      <c r="J10" s="65" t="s">
         <v>48</v>
       </c>
-      <c r="K10" s="74"/>
-      <c r="L10" s="74" t="s">
+      <c r="K10" s="65"/>
+      <c r="L10" s="65" t="s">
         <v>1</v>
       </c>
-      <c r="M10" s="74"/>
+      <c r="M10" s="65"/>
     </row>
     <row r="11" spans="1:13" ht="42.75" customHeight="1">
       <c r="A11" s="5"/>
-      <c r="B11" s="77"/>
-      <c r="C11" s="78"/>
-      <c r="D11" s="77"/>
-      <c r="E11" s="78"/>
-      <c r="F11" s="77"/>
-      <c r="G11" s="78"/>
-      <c r="H11" s="77"/>
-      <c r="I11" s="78"/>
-      <c r="J11" s="77"/>
-      <c r="K11" s="78"/>
-      <c r="L11" s="77"/>
-      <c r="M11" s="78"/>
+      <c r="B11" s="66"/>
+      <c r="C11" s="67"/>
+      <c r="D11" s="66"/>
+      <c r="E11" s="67"/>
+      <c r="F11" s="66"/>
+      <c r="G11" s="67"/>
+      <c r="H11" s="66"/>
+      <c r="I11" s="67"/>
+      <c r="J11" s="66"/>
+      <c r="K11" s="67"/>
+      <c r="L11" s="66"/>
+      <c r="M11" s="67"/>
     </row>
     <row r="13" spans="1:13" ht="16.5">
-      <c r="B13" s="59" t="s">
-        <v>65</v>
+      <c r="B13" s="69" t="s">
+        <v>63</v>
       </c>
-      <c r="C13" s="60"/>
-      <c r="D13" s="60"/>
-      <c r="E13" s="60"/>
-      <c r="F13" s="60"/>
-      <c r="G13" s="60"/>
-      <c r="H13" s="60"/>
-      <c r="I13" s="60"/>
-      <c r="J13" s="60"/>
-      <c r="K13" s="60"/>
-      <c r="L13" s="60"/>
-      <c r="M13" s="61"/>
+      <c r="C13" s="70"/>
+      <c r="D13" s="70"/>
+      <c r="E13" s="70"/>
+      <c r="F13" s="70"/>
+      <c r="G13" s="70"/>
+      <c r="H13" s="70"/>
+      <c r="I13" s="70"/>
+      <c r="J13" s="70"/>
+      <c r="K13" s="70"/>
+      <c r="L13" s="70"/>
+      <c r="M13" s="71"/>
     </row>
     <row r="14" spans="1:13" ht="51" customHeight="1">
-      <c r="B14" s="65" t="s">
-        <v>82</v>
+      <c r="B14" s="75" t="s">
+        <v>80</v>
       </c>
-      <c r="C14" s="66"/>
-      <c r="D14" s="66"/>
-      <c r="E14" s="66"/>
-      <c r="F14" s="66"/>
-      <c r="G14" s="66"/>
-      <c r="H14" s="66"/>
-      <c r="I14" s="66"/>
-      <c r="J14" s="66"/>
-      <c r="K14" s="66"/>
-      <c r="L14" s="66"/>
-      <c r="M14" s="67"/>
+      <c r="C14" s="76"/>
+      <c r="D14" s="76"/>
+      <c r="E14" s="76"/>
+      <c r="F14" s="76"/>
+      <c r="G14" s="76"/>
+      <c r="H14" s="76"/>
+      <c r="I14" s="76"/>
+      <c r="J14" s="76"/>
+      <c r="K14" s="76"/>
+      <c r="L14" s="76"/>
+      <c r="M14" s="77"/>
     </row>
     <row r="15" spans="1:13">
-      <c r="B15" s="71" t="s">
-        <v>68</v>
+      <c r="B15" s="78" t="s">
+        <v>66</v>
       </c>
-      <c r="C15" s="72"/>
-      <c r="D15" s="72"/>
-      <c r="E15" s="72"/>
-      <c r="F15" s="72"/>
-      <c r="G15" s="73"/>
-      <c r="H15" s="71" t="s">
-        <v>74</v>
+      <c r="C15" s="79"/>
+      <c r="D15" s="79"/>
+      <c r="E15" s="79"/>
+      <c r="F15" s="79"/>
+      <c r="G15" s="80"/>
+      <c r="H15" s="78" t="s">
+        <v>72</v>
       </c>
-      <c r="I15" s="72"/>
-      <c r="J15" s="72"/>
-      <c r="K15" s="72"/>
-      <c r="L15" s="72"/>
-      <c r="M15" s="73"/>
+      <c r="I15" s="79"/>
+      <c r="J15" s="79"/>
+      <c r="K15" s="79"/>
+      <c r="L15" s="79"/>
+      <c r="M15" s="80"/>
     </row>
     <row r="16" spans="1:13">
       <c r="B16" s="42"/>
@@ -45006,36 +45251,36 @@
       <c r="M31" s="50"/>
     </row>
     <row r="33" spans="2:13" ht="16.5">
-      <c r="B33" s="59" t="s">
-        <v>75</v>
+      <c r="B33" s="69" t="s">
+        <v>73</v>
       </c>
-      <c r="C33" s="60"/>
-      <c r="D33" s="60"/>
-      <c r="E33" s="60"/>
-      <c r="F33" s="60"/>
-      <c r="G33" s="60"/>
-      <c r="H33" s="60"/>
-      <c r="I33" s="60"/>
-      <c r="J33" s="60"/>
-      <c r="K33" s="60"/>
-      <c r="L33" s="60"/>
-      <c r="M33" s="61"/>
+      <c r="C33" s="70"/>
+      <c r="D33" s="70"/>
+      <c r="E33" s="70"/>
+      <c r="F33" s="70"/>
+      <c r="G33" s="70"/>
+      <c r="H33" s="70"/>
+      <c r="I33" s="70"/>
+      <c r="J33" s="70"/>
+      <c r="K33" s="70"/>
+      <c r="L33" s="70"/>
+      <c r="M33" s="71"/>
     </row>
     <row r="34" spans="2:13" ht="33.75" customHeight="1">
-      <c r="B34" s="62" t="s">
-        <v>81</v>
+      <c r="B34" s="72" t="s">
+        <v>79</v>
       </c>
-      <c r="C34" s="63"/>
-      <c r="D34" s="63"/>
-      <c r="E34" s="63"/>
-      <c r="F34" s="63"/>
-      <c r="G34" s="63"/>
-      <c r="H34" s="63"/>
-      <c r="I34" s="63"/>
-      <c r="J34" s="63"/>
-      <c r="K34" s="63"/>
-      <c r="L34" s="63"/>
-      <c r="M34" s="64"/>
+      <c r="C34" s="73"/>
+      <c r="D34" s="73"/>
+      <c r="E34" s="73"/>
+      <c r="F34" s="73"/>
+      <c r="G34" s="73"/>
+      <c r="H34" s="73"/>
+      <c r="I34" s="73"/>
+      <c r="J34" s="73"/>
+      <c r="K34" s="73"/>
+      <c r="L34" s="73"/>
+      <c r="M34" s="74"/>
     </row>
     <row r="35" spans="2:13">
       <c r="B35" s="42"/>
@@ -45263,6 +45508,17 @@
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="B33:M33"/>
+    <mergeCell ref="B34:M34"/>
+    <mergeCell ref="B14:M14"/>
+    <mergeCell ref="D7:M7"/>
+    <mergeCell ref="B9:M9"/>
+    <mergeCell ref="B13:M13"/>
+    <mergeCell ref="B15:G15"/>
+    <mergeCell ref="H15:M15"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="B11:C11"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B4:M4"/>
     <mergeCell ref="D2:M2"/>
@@ -45276,21 +45532,10 @@
     <mergeCell ref="J10:K10"/>
     <mergeCell ref="D10:E10"/>
     <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B33:M33"/>
-    <mergeCell ref="B34:M34"/>
-    <mergeCell ref="B14:M14"/>
-    <mergeCell ref="D7:M7"/>
-    <mergeCell ref="B9:M9"/>
-    <mergeCell ref="B13:M13"/>
-    <mergeCell ref="B15:G15"/>
-    <mergeCell ref="H15:M15"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="B11:C11"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup fitToWidth="0" orientation="portrait" r:id="rId1"/>
+  <pageSetup scale="91" fitToWidth="0" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
@@ -45299,6 +45544,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF366092"/>
+    <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:G11"/>
   <sheetViews>
@@ -45324,26 +45570,26 @@
       </c>
     </row>
     <row r="2" spans="1:7" ht="18" customHeight="1">
-      <c r="A2" s="82" t="s">
+      <c r="A2" s="83" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="82"/>
-      <c r="C2" s="82"/>
-      <c r="D2" s="82"/>
-      <c r="E2" s="82"/>
-      <c r="F2" s="82"/>
-      <c r="G2" s="82"/>
+      <c r="B2" s="83"/>
+      <c r="C2" s="83"/>
+      <c r="D2" s="83"/>
+      <c r="E2" s="83"/>
+      <c r="F2" s="83"/>
+      <c r="G2" s="83"/>
     </row>
     <row r="3" spans="1:7" ht="18" customHeight="1">
-      <c r="A3" s="88" t="s">
+      <c r="A3" s="89" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="88"/>
-      <c r="C3" s="88"/>
-      <c r="D3" s="88"/>
-      <c r="E3" s="88"/>
-      <c r="F3" s="88"/>
-      <c r="G3" s="88"/>
+      <c r="B3" s="89"/>
+      <c r="C3" s="89"/>
+      <c r="D3" s="89"/>
+      <c r="E3" s="89"/>
+      <c r="F3" s="89"/>
+      <c r="G3" s="89"/>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="1" t="s">
@@ -45351,15 +45597,15 @@
       </c>
     </row>
     <row r="5" spans="1:7" ht="25.5" customHeight="1">
-      <c r="A5" s="89" t="s">
-        <v>61</v>
+      <c r="A5" s="90" t="s">
+        <v>60</v>
       </c>
-      <c r="B5" s="90"/>
-      <c r="C5" s="90"/>
-      <c r="D5" s="90"/>
-      <c r="E5" s="90"/>
-      <c r="F5" s="90"/>
-      <c r="G5" s="91"/>
+      <c r="B5" s="91"/>
+      <c r="C5" s="91"/>
+      <c r="D5" s="91"/>
+      <c r="E5" s="91"/>
+      <c r="F5" s="91"/>
+      <c r="G5" s="92"/>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="1" t="s">
@@ -45367,17 +45613,17 @@
       </c>
     </row>
     <row r="7" spans="1:7" ht="18.75" customHeight="1">
-      <c r="A7" s="86" t="s">
+      <c r="A7" s="87" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="87"/>
-      <c r="C7" s="83" t="s">
+      <c r="B7" s="88"/>
+      <c r="C7" s="84" t="s">
         <v>52</v>
       </c>
-      <c r="D7" s="84"/>
-      <c r="E7" s="84"/>
-      <c r="F7" s="84"/>
-      <c r="G7" s="85"/>
+      <c r="D7" s="85"/>
+      <c r="E7" s="85"/>
+      <c r="F7" s="85"/>
+      <c r="G7" s="86"/>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="1" t="s">
@@ -45430,7 +45676,7 @@
     <mergeCell ref="A5:G5"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup scale="89" orientation="portrait" r:id="rId1"/>
+  <pageSetup scale="87" fitToHeight="0" orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
@@ -45439,11 +45685,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF366092"/>
+    <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A2:G10"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -45459,50 +45706,50 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:7" ht="18" customHeight="1">
-      <c r="A2" s="92" t="s">
+      <c r="A2" s="93" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="93"/>
-      <c r="C2" s="93"/>
-      <c r="D2" s="93"/>
-      <c r="E2" s="93"/>
-      <c r="F2" s="93"/>
-      <c r="G2" s="94"/>
+      <c r="B2" s="94"/>
+      <c r="C2" s="94"/>
+      <c r="D2" s="94"/>
+      <c r="E2" s="94"/>
+      <c r="F2" s="94"/>
+      <c r="G2" s="95"/>
     </row>
     <row r="3" spans="1:7" ht="18" customHeight="1">
-      <c r="A3" s="88" t="s">
+      <c r="A3" s="89" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="88"/>
-      <c r="C3" s="88"/>
-      <c r="D3" s="88"/>
-      <c r="E3" s="88"/>
-      <c r="F3" s="88"/>
-      <c r="G3" s="88"/>
+      <c r="B3" s="89"/>
+      <c r="C3" s="89"/>
+      <c r="D3" s="89"/>
+      <c r="E3" s="89"/>
+      <c r="F3" s="89"/>
+      <c r="G3" s="89"/>
     </row>
     <row r="5" spans="1:7" ht="25.5" customHeight="1">
-      <c r="A5" s="89" t="s">
-        <v>62</v>
+      <c r="A5" s="90" t="s">
+        <v>61</v>
       </c>
-      <c r="B5" s="90"/>
-      <c r="C5" s="90"/>
-      <c r="D5" s="90"/>
-      <c r="E5" s="90"/>
-      <c r="F5" s="90"/>
-      <c r="G5" s="91"/>
+      <c r="B5" s="91"/>
+      <c r="C5" s="91"/>
+      <c r="D5" s="91"/>
+      <c r="E5" s="91"/>
+      <c r="F5" s="91"/>
+      <c r="G5" s="92"/>
     </row>
     <row r="7" spans="1:7" ht="18.75" customHeight="1">
-      <c r="A7" s="88" t="s">
+      <c r="A7" s="89" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="88"/>
-      <c r="C7" s="95" t="s">
+      <c r="B7" s="89"/>
+      <c r="C7" s="96" t="s">
         <v>53</v>
       </c>
-      <c r="D7" s="95"/>
-      <c r="E7" s="95"/>
-      <c r="F7" s="95"/>
-      <c r="G7" s="95"/>
+      <c r="D7" s="96"/>
+      <c r="E7" s="96"/>
+      <c r="F7" s="96"/>
+      <c r="G7" s="96"/>
     </row>
     <row r="9" spans="1:7" ht="25.5">
       <c r="A9" s="35" t="s">
@@ -45545,7 +45792,7 @@
     <mergeCell ref="A5:G5"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup scale="89" orientation="portrait" r:id="rId1"/>
+  <pageSetup scale="87" fitToHeight="0" orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
@@ -45570,18 +45817,18 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:10" ht="18" customHeight="1">
-      <c r="A2" s="99" t="s">
+      <c r="A2" s="100" t="s">
         <v>37</v>
       </c>
-      <c r="B2" s="99"/>
-      <c r="C2" s="99"/>
-      <c r="D2" s="99"/>
-      <c r="E2" s="99"/>
-      <c r="F2" s="99"/>
-      <c r="G2" s="99"/>
-      <c r="H2" s="99"/>
-      <c r="I2" s="99"/>
-      <c r="J2" s="99"/>
+      <c r="B2" s="100"/>
+      <c r="C2" s="100"/>
+      <c r="D2" s="100"/>
+      <c r="E2" s="100"/>
+      <c r="F2" s="100"/>
+      <c r="G2" s="100"/>
+      <c r="H2" s="100"/>
+      <c r="I2" s="100"/>
+      <c r="J2" s="100"/>
     </row>
     <row r="3" spans="1:10" ht="18">
       <c r="A3" s="12"/>
@@ -45591,17 +45838,17 @@
       <c r="A4" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="96" t="s">
-        <v>63</v>
+      <c r="B4" s="97" t="s">
+        <v>62</v>
       </c>
-      <c r="C4" s="97"/>
-      <c r="D4" s="97"/>
-      <c r="E4" s="97"/>
-      <c r="F4" s="97"/>
-      <c r="G4" s="97"/>
-      <c r="H4" s="97"/>
-      <c r="I4" s="97"/>
-      <c r="J4" s="98"/>
+      <c r="C4" s="98"/>
+      <c r="D4" s="98"/>
+      <c r="E4" s="98"/>
+      <c r="F4" s="98"/>
+      <c r="G4" s="98"/>
+      <c r="H4" s="98"/>
+      <c r="I4" s="98"/>
+      <c r="J4" s="99"/>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="2"/>
@@ -45749,34 +45996,34 @@
   <sheetData>
     <row r="1" spans="1:10" ht="18" customHeight="1"/>
     <row r="2" spans="1:10" ht="18" customHeight="1">
-      <c r="A2" s="99" t="s">
+      <c r="A2" s="100" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="99"/>
-      <c r="C2" s="99"/>
-      <c r="D2" s="99"/>
-      <c r="E2" s="99"/>
-      <c r="F2" s="99"/>
-      <c r="G2" s="99"/>
-      <c r="H2" s="99"/>
-      <c r="I2" s="99"/>
-      <c r="J2" s="99"/>
+      <c r="B2" s="100"/>
+      <c r="C2" s="100"/>
+      <c r="D2" s="100"/>
+      <c r="E2" s="100"/>
+      <c r="F2" s="100"/>
+      <c r="G2" s="100"/>
+      <c r="H2" s="100"/>
+      <c r="I2" s="100"/>
+      <c r="J2" s="100"/>
     </row>
     <row r="4" spans="1:10" ht="53.25" customHeight="1">
       <c r="A4" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="100" t="s">
-        <v>83</v>
+      <c r="B4" s="101" t="s">
+        <v>81</v>
       </c>
-      <c r="C4" s="101"/>
-      <c r="D4" s="101"/>
-      <c r="E4" s="101"/>
-      <c r="F4" s="101"/>
-      <c r="G4" s="101"/>
-      <c r="H4" s="101"/>
-      <c r="I4" s="101"/>
-      <c r="J4" s="102"/>
+      <c r="C4" s="102"/>
+      <c r="D4" s="102"/>
+      <c r="E4" s="102"/>
+      <c r="F4" s="102"/>
+      <c r="G4" s="102"/>
+      <c r="H4" s="102"/>
+      <c r="I4" s="102"/>
+      <c r="J4" s="103"/>
     </row>
     <row r="6" spans="1:10" ht="39.75" customHeight="1">
       <c r="A6" s="35" t="s">
@@ -45805,11 +46052,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF366092"/>
+    <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A2:B7"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -45820,10 +46068,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:2" ht="18">
-      <c r="A2" s="99" t="s">
+      <c r="A2" s="100" t="s">
         <v>56</v>
       </c>
-      <c r="B2" s="99"/>
+      <c r="B2" s="100"/>
     </row>
     <row r="3" spans="1:2" ht="18">
       <c r="A3" s="12"/>
@@ -45858,7 +46106,7 @@
     <mergeCell ref="A2:B2"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup scale="99" orientation="portrait" r:id="rId1"/>
+  <pageSetup fitToHeight="0" orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
@@ -45867,11 +46115,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF366092"/>
+    <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A2:C7"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -45883,25 +46132,25 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:3" ht="18">
-      <c r="A2" s="99" t="s">
+      <c r="A2" s="100" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="99"/>
-      <c r="C2" s="99"/>
+      <c r="B2" s="100"/>
+      <c r="C2" s="100"/>
     </row>
     <row r="3" spans="1:3" ht="18">
       <c r="A3" s="12"/>
       <c r="B3" s="12"/>
       <c r="C3" s="12"/>
     </row>
-    <row r="4" spans="1:3" ht="18">
+    <row r="4" spans="1:3" ht="25.5" customHeight="1">
       <c r="A4" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="96" t="s">
-        <v>64</v>
+      <c r="B4" s="97" t="s">
+        <v>84</v>
       </c>
-      <c r="C4" s="98"/>
+      <c r="C4" s="99"/>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="2"/>
@@ -45930,7 +46179,7 @@
     <mergeCell ref="B4:C4"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup scale="69" orientation="portrait" r:id="rId1"/>
+  <pageSetup scale="78" fitToHeight="0" orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
@@ -45939,11 +46188,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF366092"/>
+    <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:M8"/>
+  <dimension ref="A1:M11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+    <sheetView topLeftCell="B1" zoomScaleNormal="100" zoomScalePageLayoutView="80" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -45966,112 +46216,152 @@
   <sheetData>
     <row r="1" spans="1:13" ht="18" customHeight="1"/>
     <row r="2" spans="1:13" ht="18" customHeight="1">
-      <c r="A2" s="99" t="s">
+      <c r="A2" s="100" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="99"/>
-      <c r="C2" s="99"/>
-      <c r="D2" s="99"/>
-      <c r="E2" s="99"/>
-      <c r="F2" s="99"/>
-      <c r="G2" s="99"/>
-      <c r="H2" s="99"/>
-      <c r="I2" s="99"/>
-      <c r="J2" s="99"/>
-      <c r="K2" s="99"/>
-      <c r="L2" s="99"/>
-      <c r="M2" s="99"/>
+      <c r="B2" s="100"/>
+      <c r="C2" s="100"/>
+      <c r="D2" s="100"/>
+      <c r="E2" s="100"/>
+      <c r="F2" s="100"/>
+      <c r="G2" s="100"/>
+      <c r="H2" s="100"/>
+      <c r="I2" s="100"/>
+      <c r="J2" s="100"/>
+      <c r="K2" s="100"/>
+      <c r="L2" s="100"/>
+      <c r="M2" s="100"/>
     </row>
     <row r="4" spans="1:13" ht="20.25" customHeight="1">
-      <c r="A4" s="103" t="s">
+      <c r="A4" s="112" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="104"/>
-      <c r="C4" s="105"/>
-      <c r="D4" s="106" t="s">
+      <c r="B4" s="113"/>
+      <c r="C4" s="114"/>
+      <c r="D4" s="104" t="s">
         <v>41</v>
       </c>
-      <c r="E4" s="107"/>
-      <c r="F4" s="107"/>
-      <c r="G4" s="107"/>
-      <c r="H4" s="107"/>
-      <c r="I4" s="107"/>
-      <c r="J4" s="107"/>
-      <c r="K4" s="107"/>
-      <c r="L4" s="107"/>
-      <c r="M4" s="108"/>
+      <c r="E4" s="105"/>
+      <c r="F4" s="105"/>
+      <c r="G4" s="105"/>
+      <c r="H4" s="105"/>
+      <c r="I4" s="105"/>
+      <c r="J4" s="105"/>
+      <c r="K4" s="105"/>
+      <c r="L4" s="105"/>
+      <c r="M4" s="106"/>
     </row>
-    <row r="6" spans="1:13" ht="39.75" customHeight="1">
-      <c r="A6" s="35" t="s">
+    <row r="6" spans="1:13" ht="96.75" customHeight="1">
+      <c r="A6" s="107" t="s">
+        <v>85</v>
+      </c>
+      <c r="B6" s="51" t="s">
+        <v>86</v>
+      </c>
+      <c r="C6" s="108"/>
+      <c r="D6" s="108"/>
+      <c r="E6" s="108"/>
+      <c r="F6" s="51" t="s">
+        <v>88</v>
+      </c>
+      <c r="G6" s="108"/>
+      <c r="H6" s="108"/>
+      <c r="I6" s="108"/>
+      <c r="J6" s="51" t="s">
+        <v>89</v>
+      </c>
+      <c r="K6" s="108"/>
+      <c r="L6" s="108"/>
+      <c r="M6" s="108"/>
+    </row>
+    <row r="7" spans="1:13" ht="45" customHeight="1">
+      <c r="A7" s="107"/>
+      <c r="B7" s="51" t="s">
+        <v>87</v>
+      </c>
+      <c r="C7" s="109"/>
+      <c r="D7" s="110"/>
+      <c r="E7" s="110"/>
+      <c r="F7" s="110"/>
+      <c r="G7" s="111"/>
+    </row>
+    <row r="9" spans="1:13" ht="39.75" customHeight="1">
+      <c r="A9" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="35" t="s">
+      <c r="B9" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="35" t="s">
+      <c r="C9" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="D6" s="35" t="s">
+      <c r="D9" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="35" t="s">
+      <c r="E9" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="F6" s="35" t="s">
+      <c r="F9" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="G6" s="35" t="s">
+      <c r="G9" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="H6" s="35" t="s">
+      <c r="H9" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="I6" s="35" t="s">
+      <c r="I9" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="J6" s="35" t="s">
+      <c r="J9" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="K6" s="35" t="s">
-        <v>84</v>
+      <c r="K9" s="35" t="s">
+        <v>82</v>
       </c>
-      <c r="L6" s="36" t="s">
+      <c r="L9" s="36" t="s">
         <v>44</v>
       </c>
-      <c r="M6" s="36" t="s">
+      <c r="M9" s="36" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:13">
-      <c r="A7" s="14"/>
-      <c r="B7" s="14"/>
-      <c r="C7" s="23"/>
-      <c r="D7" s="14"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="23"/>
-      <c r="G7" s="14"/>
-      <c r="H7" s="14"/>
-      <c r="I7" s="23"/>
-      <c r="J7" s="23"/>
-      <c r="K7" s="14"/>
-      <c r="L7" s="22"/>
-      <c r="M7" s="22"/>
+    <row r="10" spans="1:13">
+      <c r="A10" s="14"/>
+      <c r="B10" s="14"/>
+      <c r="C10" s="23"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="23"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="14"/>
+      <c r="I10" s="23"/>
+      <c r="J10" s="23"/>
+      <c r="K10" s="14"/>
+      <c r="L10" s="22"/>
+      <c r="M10" s="22"/>
     </row>
-    <row r="8" spans="1:13">
-      <c r="K8" s="27" t="s">
+    <row r="11" spans="1:13">
+      <c r="K11" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="L8" s="26"/>
-      <c r="M8" s="26"/>
+      <c r="L11" s="26"/>
+      <c r="M11" s="26"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="A4:C4"/>
+  <mergeCells count="8">
     <mergeCell ref="A2:M2"/>
     <mergeCell ref="D4:M4"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="G6:I6"/>
+    <mergeCell ref="K6:M6"/>
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="A4:C4"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup scale="48" orientation="landscape" r:id="rId1"/>
+  <pageSetup scale="53" fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Changed Instructions tab to say Report Overview
git-svn-id: svn://107.170.10.188:8080/Semoss/trunk@3350 ef391c1c-ee15-45f7-b1d6-dde3d27a2169
</commit_message>
<xml_diff>
--- a/export/Reports/Individual_System_LPI_Transition_Report_Template.xlsx
+++ b/export/Reports/Individual_System_LPI_Transition_Report_Template.xlsx
@@ -4,10 +4,10 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="1110" windowWidth="15120" windowHeight="6405" tabRatio="834" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="1110" windowWidth="15120" windowHeight="6405" tabRatio="834"/>
   </bookViews>
   <sheets>
-    <sheet name="Instructions" sheetId="33" r:id="rId1"/>
+    <sheet name="Report Overview" sheetId="33" r:id="rId1"/>
     <sheet name="System Overview" sheetId="21" r:id="rId2"/>
     <sheet name="Software Lifecycles" sheetId="22" r:id="rId3"/>
     <sheet name="Hardware Lifecycles" sheetId="23" r:id="rId4"/>
@@ -981,6 +981,33 @@
     <xf numFmtId="0" fontId="24" fillId="6" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="5" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="7" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="10" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="3" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="5" borderId="5" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1008,15 +1035,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="4" borderId="5" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1026,28 +1044,10 @@
     <xf numFmtId="0" fontId="17" fillId="4" borderId="7" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="10" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="5" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="7" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="3" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1411,11 +1411,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="213359232"/>
-        <c:axId val="213644032"/>
+        <c:axId val="200572288"/>
+        <c:axId val="201316992"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="213359232"/>
+        <c:axId val="200572288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1425,7 +1425,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="213644032"/>
+        <c:crossAx val="201316992"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1433,7 +1433,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="213644032"/>
+        <c:axId val="201316992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1444,7 +1444,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="213359232"/>
+        <c:crossAx val="200572288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1577,11 +1577,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="228386688"/>
-        <c:axId val="228388224"/>
+        <c:axId val="205313920"/>
+        <c:axId val="205373440"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="228386688"/>
+        <c:axId val="205313920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1591,7 +1591,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="228388224"/>
+        <c:crossAx val="205373440"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1599,7 +1599,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="228388224"/>
+        <c:axId val="205373440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1610,7 +1610,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="228386688"/>
+        <c:crossAx val="205313920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1891,11 +1891,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="240522752"/>
-        <c:axId val="241903104"/>
+        <c:axId val="210647680"/>
+        <c:axId val="210662144"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="240522752"/>
+        <c:axId val="210647680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1905,7 +1905,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="241903104"/>
+        <c:crossAx val="210662144"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1913,7 +1913,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="241903104"/>
+        <c:axId val="210662144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1924,7 +1924,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="240522752"/>
+        <c:crossAx val="210647680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -44460,7 +44460,7 @@
   </sheetPr>
   <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
@@ -44657,22 +44657,22 @@
     <row r="1" spans="1:13" ht="7.5" customHeight="1"/>
     <row r="2" spans="1:13" s="4" customFormat="1" ht="250.5" customHeight="1">
       <c r="A2" s="3"/>
-      <c r="B2" s="81" t="s">
+      <c r="B2" s="61" t="s">
         <v>33</v>
       </c>
-      <c r="C2" s="82"/>
-      <c r="D2" s="70" t="s">
+      <c r="C2" s="62"/>
+      <c r="D2" s="63" t="s">
         <v>34</v>
       </c>
-      <c r="E2" s="71"/>
-      <c r="F2" s="71"/>
-      <c r="G2" s="71"/>
-      <c r="H2" s="71"/>
-      <c r="I2" s="71"/>
-      <c r="J2" s="71"/>
-      <c r="K2" s="71"/>
-      <c r="L2" s="71"/>
-      <c r="M2" s="72"/>
+      <c r="E2" s="64"/>
+      <c r="F2" s="64"/>
+      <c r="G2" s="64"/>
+      <c r="H2" s="64"/>
+      <c r="I2" s="64"/>
+      <c r="J2" s="64"/>
+      <c r="K2" s="64"/>
+      <c r="L2" s="64"/>
+      <c r="M2" s="65"/>
     </row>
     <row r="3" spans="1:13" s="20" customFormat="1" ht="7.5" customHeight="1">
       <c r="A3" s="16"/>
@@ -44730,22 +44730,22 @@
     </row>
     <row r="7" spans="1:13" s="4" customFormat="1" ht="375" customHeight="1">
       <c r="A7" s="3"/>
-      <c r="B7" s="81" t="s">
+      <c r="B7" s="61" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="82"/>
-      <c r="D7" s="70" t="s">
+      <c r="C7" s="62"/>
+      <c r="D7" s="63" t="s">
         <v>48</v>
       </c>
-      <c r="E7" s="71"/>
-      <c r="F7" s="71"/>
-      <c r="G7" s="71"/>
-      <c r="H7" s="71"/>
-      <c r="I7" s="71"/>
-      <c r="J7" s="71"/>
-      <c r="K7" s="71"/>
-      <c r="L7" s="71"/>
-      <c r="M7" s="72"/>
+      <c r="E7" s="64"/>
+      <c r="F7" s="64"/>
+      <c r="G7" s="64"/>
+      <c r="H7" s="64"/>
+      <c r="I7" s="64"/>
+      <c r="J7" s="64"/>
+      <c r="K7" s="64"/>
+      <c r="L7" s="64"/>
+      <c r="M7" s="65"/>
     </row>
     <row r="8" spans="1:13" ht="8.25" customHeight="1">
       <c r="A8" s="5"/>
@@ -44756,112 +44756,112 @@
     </row>
     <row r="9" spans="1:13" s="8" customFormat="1" ht="18" customHeight="1">
       <c r="A9" s="7"/>
-      <c r="B9" s="61" t="s">
+      <c r="B9" s="70" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="62"/>
-      <c r="D9" s="62"/>
-      <c r="E9" s="62"/>
-      <c r="F9" s="62"/>
-      <c r="G9" s="62"/>
-      <c r="H9" s="62"/>
-      <c r="I9" s="62"/>
-      <c r="J9" s="62"/>
-      <c r="K9" s="62"/>
-      <c r="L9" s="62"/>
-      <c r="M9" s="63"/>
+      <c r="C9" s="71"/>
+      <c r="D9" s="71"/>
+      <c r="E9" s="71"/>
+      <c r="F9" s="71"/>
+      <c r="G9" s="71"/>
+      <c r="H9" s="71"/>
+      <c r="I9" s="71"/>
+      <c r="J9" s="71"/>
+      <c r="K9" s="71"/>
+      <c r="L9" s="71"/>
+      <c r="M9" s="72"/>
     </row>
     <row r="10" spans="1:13" s="8" customFormat="1" ht="28.5" customHeight="1">
       <c r="A10" s="7"/>
-      <c r="B10" s="76" t="s">
+      <c r="B10" s="66" t="s">
         <v>0</v>
       </c>
-      <c r="C10" s="76"/>
-      <c r="D10" s="76" t="s">
+      <c r="C10" s="66"/>
+      <c r="D10" s="66" t="s">
         <v>5</v>
       </c>
-      <c r="E10" s="83"/>
-      <c r="F10" s="76" t="s">
+      <c r="E10" s="69"/>
+      <c r="F10" s="66" t="s">
         <v>38</v>
       </c>
-      <c r="G10" s="76"/>
-      <c r="H10" s="77" t="s">
+      <c r="G10" s="66"/>
+      <c r="H10" s="82" t="s">
         <v>39</v>
       </c>
-      <c r="I10" s="78"/>
-      <c r="J10" s="76" t="s">
+      <c r="I10" s="83"/>
+      <c r="J10" s="66" t="s">
         <v>40</v>
       </c>
-      <c r="K10" s="76"/>
-      <c r="L10" s="76" t="s">
+      <c r="K10" s="66"/>
+      <c r="L10" s="66" t="s">
         <v>1</v>
       </c>
-      <c r="M10" s="76"/>
+      <c r="M10" s="66"/>
     </row>
     <row r="11" spans="1:13" ht="42.75" customHeight="1">
       <c r="A11" s="5"/>
-      <c r="B11" s="79"/>
-      <c r="C11" s="80"/>
-      <c r="D11" s="79"/>
-      <c r="E11" s="80"/>
-      <c r="F11" s="79"/>
-      <c r="G11" s="80"/>
-      <c r="H11" s="79"/>
-      <c r="I11" s="80"/>
-      <c r="J11" s="79"/>
-      <c r="K11" s="80"/>
-      <c r="L11" s="79"/>
-      <c r="M11" s="80"/>
+      <c r="B11" s="67"/>
+      <c r="C11" s="68"/>
+      <c r="D11" s="67"/>
+      <c r="E11" s="68"/>
+      <c r="F11" s="67"/>
+      <c r="G11" s="68"/>
+      <c r="H11" s="67"/>
+      <c r="I11" s="68"/>
+      <c r="J11" s="67"/>
+      <c r="K11" s="68"/>
+      <c r="L11" s="67"/>
+      <c r="M11" s="68"/>
     </row>
     <row r="13" spans="1:13" ht="16.5">
-      <c r="B13" s="61" t="s">
+      <c r="B13" s="70" t="s">
         <v>49</v>
       </c>
-      <c r="C13" s="62"/>
-      <c r="D13" s="62"/>
-      <c r="E13" s="62"/>
-      <c r="F13" s="62"/>
-      <c r="G13" s="62"/>
-      <c r="H13" s="62"/>
-      <c r="I13" s="62"/>
-      <c r="J13" s="62"/>
-      <c r="K13" s="62"/>
-      <c r="L13" s="62"/>
-      <c r="M13" s="63"/>
+      <c r="C13" s="71"/>
+      <c r="D13" s="71"/>
+      <c r="E13" s="71"/>
+      <c r="F13" s="71"/>
+      <c r="G13" s="71"/>
+      <c r="H13" s="71"/>
+      <c r="I13" s="71"/>
+      <c r="J13" s="71"/>
+      <c r="K13" s="71"/>
+      <c r="L13" s="71"/>
+      <c r="M13" s="72"/>
     </row>
     <row r="14" spans="1:13" ht="51" customHeight="1">
-      <c r="B14" s="67" t="s">
+      <c r="B14" s="76" t="s">
         <v>66</v>
       </c>
-      <c r="C14" s="68"/>
-      <c r="D14" s="68"/>
-      <c r="E14" s="68"/>
-      <c r="F14" s="68"/>
-      <c r="G14" s="68"/>
-      <c r="H14" s="68"/>
-      <c r="I14" s="68"/>
-      <c r="J14" s="68"/>
-      <c r="K14" s="68"/>
-      <c r="L14" s="68"/>
-      <c r="M14" s="69"/>
+      <c r="C14" s="77"/>
+      <c r="D14" s="77"/>
+      <c r="E14" s="77"/>
+      <c r="F14" s="77"/>
+      <c r="G14" s="77"/>
+      <c r="H14" s="77"/>
+      <c r="I14" s="77"/>
+      <c r="J14" s="77"/>
+      <c r="K14" s="77"/>
+      <c r="L14" s="77"/>
+      <c r="M14" s="78"/>
     </row>
     <row r="15" spans="1:13">
-      <c r="B15" s="73" t="s">
+      <c r="B15" s="79" t="s">
         <v>52</v>
       </c>
-      <c r="C15" s="74"/>
-      <c r="D15" s="74"/>
-      <c r="E15" s="74"/>
-      <c r="F15" s="74"/>
-      <c r="G15" s="75"/>
-      <c r="H15" s="73" t="s">
+      <c r="C15" s="80"/>
+      <c r="D15" s="80"/>
+      <c r="E15" s="80"/>
+      <c r="F15" s="80"/>
+      <c r="G15" s="81"/>
+      <c r="H15" s="79" t="s">
         <v>58</v>
       </c>
-      <c r="I15" s="74"/>
-      <c r="J15" s="74"/>
-      <c r="K15" s="74"/>
-      <c r="L15" s="74"/>
-      <c r="M15" s="75"/>
+      <c r="I15" s="80"/>
+      <c r="J15" s="80"/>
+      <c r="K15" s="80"/>
+      <c r="L15" s="80"/>
+      <c r="M15" s="81"/>
     </row>
     <row r="16" spans="1:13">
       <c r="B16" s="40"/>
@@ -45088,36 +45088,36 @@
       <c r="M31" s="48"/>
     </row>
     <row r="33" spans="2:13" ht="16.5">
-      <c r="B33" s="61" t="s">
+      <c r="B33" s="70" t="s">
         <v>59</v>
       </c>
-      <c r="C33" s="62"/>
-      <c r="D33" s="62"/>
-      <c r="E33" s="62"/>
-      <c r="F33" s="62"/>
-      <c r="G33" s="62"/>
-      <c r="H33" s="62"/>
-      <c r="I33" s="62"/>
-      <c r="J33" s="62"/>
-      <c r="K33" s="62"/>
-      <c r="L33" s="62"/>
-      <c r="M33" s="63"/>
+      <c r="C33" s="71"/>
+      <c r="D33" s="71"/>
+      <c r="E33" s="71"/>
+      <c r="F33" s="71"/>
+      <c r="G33" s="71"/>
+      <c r="H33" s="71"/>
+      <c r="I33" s="71"/>
+      <c r="J33" s="71"/>
+      <c r="K33" s="71"/>
+      <c r="L33" s="71"/>
+      <c r="M33" s="72"/>
     </row>
     <row r="34" spans="2:13" ht="33.75" customHeight="1">
-      <c r="B34" s="64" t="s">
+      <c r="B34" s="73" t="s">
         <v>65</v>
       </c>
-      <c r="C34" s="65"/>
-      <c r="D34" s="65"/>
-      <c r="E34" s="65"/>
-      <c r="F34" s="65"/>
-      <c r="G34" s="65"/>
-      <c r="H34" s="65"/>
-      <c r="I34" s="65"/>
-      <c r="J34" s="65"/>
-      <c r="K34" s="65"/>
-      <c r="L34" s="65"/>
-      <c r="M34" s="66"/>
+      <c r="C34" s="74"/>
+      <c r="D34" s="74"/>
+      <c r="E34" s="74"/>
+      <c r="F34" s="74"/>
+      <c r="G34" s="74"/>
+      <c r="H34" s="74"/>
+      <c r="I34" s="74"/>
+      <c r="J34" s="74"/>
+      <c r="K34" s="74"/>
+      <c r="L34" s="74"/>
+      <c r="M34" s="75"/>
     </row>
     <row r="35" spans="2:13">
       <c r="B35" s="40"/>
@@ -45345,6 +45345,17 @@
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="B33:M33"/>
+    <mergeCell ref="B34:M34"/>
+    <mergeCell ref="B14:M14"/>
+    <mergeCell ref="D7:M7"/>
+    <mergeCell ref="B9:M9"/>
+    <mergeCell ref="B13:M13"/>
+    <mergeCell ref="B15:G15"/>
+    <mergeCell ref="H15:M15"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="B11:C11"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B4:M4"/>
     <mergeCell ref="D2:M2"/>
@@ -45358,17 +45369,6 @@
     <mergeCell ref="J10:K10"/>
     <mergeCell ref="D10:E10"/>
     <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B33:M33"/>
-    <mergeCell ref="B34:M34"/>
-    <mergeCell ref="B14:M14"/>
-    <mergeCell ref="D7:M7"/>
-    <mergeCell ref="B9:M9"/>
-    <mergeCell ref="B13:M13"/>
-    <mergeCell ref="B15:G15"/>
-    <mergeCell ref="H15:M15"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="B11:C11"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -45642,7 +45642,7 @@
   </sheetPr>
   <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="80" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="80" workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Modified SOR DHMSM Overlap tab
git-svn-id: svn://107.170.10.188:8080/Semoss/trunk@3351 ef391c1c-ee15-45f7-b1d6-dde3d27a2169

Former-commit-id: 3b205fe907251597b1e4ba93279e7fcdfbbb567d
</commit_message>
<xml_diff>
--- a/export/Reports/Individual_System_LPI_Transition_Report_Template.xlsx
+++ b/export/Reports/Individual_System_LPI_Transition_Report_Template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="1110" windowWidth="15120" windowHeight="6405" tabRatio="834"/>
+    <workbookView xWindow="240" yWindow="1110" windowWidth="15120" windowHeight="6405" tabRatio="834" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Report Overview" sheetId="33" r:id="rId1"/>
@@ -200,9 +200,6 @@
     <t>System Interfaces</t>
   </si>
   <si>
-    <t>This section displays data objects for which @SYSTEM@ is Source of Record (SOR) and which of those that DHMSM is also SOR for.</t>
-  </si>
-  <si>
     <t>System Name</t>
   </si>
   <si>
@@ -390,6 +387,9 @@
   </si>
   <si>
     <t>This section displays the data objects that @SYSTEM@ creates, reads, or modifies. This information is used in concert with the @SYSTEM@ interface control documents to define what data @SYSTEM@ is a source of record of and what data @SYSTEM@ consumes.</t>
+  </si>
+  <si>
+    <t>This section displays data objects for which @SYSTEM@ is Source of Record (SOR) and which of those DHMSM is expected to become the SOR for in the future.</t>
   </si>
 </sst>
 </file>
@@ -981,33 +981,6 @@
     <xf numFmtId="0" fontId="24" fillId="6" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="5" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="7" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="10" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="3" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="5" borderId="5" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1035,6 +1008,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="4" borderId="5" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1044,10 +1026,28 @@
     <xf numFmtId="0" fontId="17" fillId="4" borderId="7" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="10" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="5" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="7" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="3" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1411,11 +1411,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="200572288"/>
-        <c:axId val="201316992"/>
+        <c:axId val="236982656"/>
+        <c:axId val="236984960"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="200572288"/>
+        <c:axId val="236982656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1425,7 +1425,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="201316992"/>
+        <c:crossAx val="236984960"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1433,7 +1433,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="201316992"/>
+        <c:axId val="236984960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1444,7 +1444,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="200572288"/>
+        <c:crossAx val="236982656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1577,11 +1577,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="205313920"/>
-        <c:axId val="205373440"/>
+        <c:axId val="405357696"/>
+        <c:axId val="405359232"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="205313920"/>
+        <c:axId val="405357696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1591,7 +1591,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="205373440"/>
+        <c:crossAx val="405359232"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1599,7 +1599,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="205373440"/>
+        <c:axId val="405359232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1610,7 +1610,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="205313920"/>
+        <c:crossAx val="405357696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1891,11 +1891,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="210647680"/>
-        <c:axId val="210662144"/>
+        <c:axId val="130611456"/>
+        <c:axId val="174440448"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="210647680"/>
+        <c:axId val="130611456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1905,7 +1905,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="210662144"/>
+        <c:crossAx val="174440448"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1913,7 +1913,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="210662144"/>
+        <c:axId val="174440448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1924,7 +1924,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="210647680"/>
+        <c:crossAx val="130611456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -44460,7 +44460,7 @@
   </sheetPr>
   <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView topLeftCell="A5" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
@@ -44474,12 +44474,12 @@
   <sheetData>
     <row r="1" spans="1:12" s="1" customFormat="1" ht="7.5" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="32.25" customHeight="1">
       <c r="A2" s="53" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B2" s="54"/>
       <c r="C2" s="54"/>
@@ -44495,12 +44495,12 @@
     </row>
     <row r="3" spans="1:12" s="1" customFormat="1" ht="7.5" customHeight="1">
       <c r="A3" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="281.25" customHeight="1">
       <c r="A4" s="55" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B4" s="56"/>
       <c r="C4" s="56"/>
@@ -44516,12 +44516,12 @@
     </row>
     <row r="5" spans="1:12" s="1" customFormat="1" ht="7.5" customHeight="1">
       <c r="A5" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:12" s="30" customFormat="1" ht="29.25" customHeight="1">
       <c r="A6" s="53" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B6" s="54"/>
       <c r="C6" s="54"/>
@@ -44537,12 +44537,12 @@
     </row>
     <row r="7" spans="1:12" s="1" customFormat="1" ht="7.5" customHeight="1">
       <c r="A7" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="134.25" customHeight="1">
       <c r="A8" s="58" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B8" s="59"/>
       <c r="C8" s="59"/>
@@ -44657,22 +44657,22 @@
     <row r="1" spans="1:13" ht="7.5" customHeight="1"/>
     <row r="2" spans="1:13" s="4" customFormat="1" ht="250.5" customHeight="1">
       <c r="A2" s="3"/>
-      <c r="B2" s="61" t="s">
+      <c r="B2" s="81" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="82"/>
+      <c r="D2" s="70" t="s">
         <v>33</v>
       </c>
-      <c r="C2" s="62"/>
-      <c r="D2" s="63" t="s">
-        <v>34</v>
-      </c>
-      <c r="E2" s="64"/>
-      <c r="F2" s="64"/>
-      <c r="G2" s="64"/>
-      <c r="H2" s="64"/>
-      <c r="I2" s="64"/>
-      <c r="J2" s="64"/>
-      <c r="K2" s="64"/>
-      <c r="L2" s="64"/>
-      <c r="M2" s="65"/>
+      <c r="E2" s="71"/>
+      <c r="F2" s="71"/>
+      <c r="G2" s="71"/>
+      <c r="H2" s="71"/>
+      <c r="I2" s="71"/>
+      <c r="J2" s="71"/>
+      <c r="K2" s="71"/>
+      <c r="L2" s="71"/>
+      <c r="M2" s="72"/>
     </row>
     <row r="3" spans="1:13" s="20" customFormat="1" ht="7.5" customHeight="1">
       <c r="A3" s="16"/>
@@ -44692,7 +44692,7 @@
     <row r="4" spans="1:13" ht="32.25" customHeight="1">
       <c r="A4" s="5"/>
       <c r="B4" s="53" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C4" s="54"/>
       <c r="D4" s="54"/>
@@ -44730,22 +44730,22 @@
     </row>
     <row r="7" spans="1:13" s="4" customFormat="1" ht="375" customHeight="1">
       <c r="A7" s="3"/>
-      <c r="B7" s="61" t="s">
+      <c r="B7" s="81" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="62"/>
-      <c r="D7" s="63" t="s">
-        <v>48</v>
+      <c r="C7" s="82"/>
+      <c r="D7" s="70" t="s">
+        <v>47</v>
       </c>
-      <c r="E7" s="64"/>
-      <c r="F7" s="64"/>
-      <c r="G7" s="64"/>
-      <c r="H7" s="64"/>
-      <c r="I7" s="64"/>
-      <c r="J7" s="64"/>
-      <c r="K7" s="64"/>
-      <c r="L7" s="64"/>
-      <c r="M7" s="65"/>
+      <c r="E7" s="71"/>
+      <c r="F7" s="71"/>
+      <c r="G7" s="71"/>
+      <c r="H7" s="71"/>
+      <c r="I7" s="71"/>
+      <c r="J7" s="71"/>
+      <c r="K7" s="71"/>
+      <c r="L7" s="71"/>
+      <c r="M7" s="72"/>
     </row>
     <row r="8" spans="1:13" ht="8.25" customHeight="1">
       <c r="A8" s="5"/>
@@ -44756,112 +44756,112 @@
     </row>
     <row r="9" spans="1:13" s="8" customFormat="1" ht="18" customHeight="1">
       <c r="A9" s="7"/>
-      <c r="B9" s="70" t="s">
+      <c r="B9" s="61" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="71"/>
-      <c r="D9" s="71"/>
-      <c r="E9" s="71"/>
-      <c r="F9" s="71"/>
-      <c r="G9" s="71"/>
-      <c r="H9" s="71"/>
-      <c r="I9" s="71"/>
-      <c r="J9" s="71"/>
-      <c r="K9" s="71"/>
-      <c r="L9" s="71"/>
-      <c r="M9" s="72"/>
+      <c r="C9" s="62"/>
+      <c r="D9" s="62"/>
+      <c r="E9" s="62"/>
+      <c r="F9" s="62"/>
+      <c r="G9" s="62"/>
+      <c r="H9" s="62"/>
+      <c r="I9" s="62"/>
+      <c r="J9" s="62"/>
+      <c r="K9" s="62"/>
+      <c r="L9" s="62"/>
+      <c r="M9" s="63"/>
     </row>
     <row r="10" spans="1:13" s="8" customFormat="1" ht="28.5" customHeight="1">
       <c r="A10" s="7"/>
-      <c r="B10" s="66" t="s">
+      <c r="B10" s="76" t="s">
         <v>0</v>
       </c>
-      <c r="C10" s="66"/>
-      <c r="D10" s="66" t="s">
+      <c r="C10" s="76"/>
+      <c r="D10" s="76" t="s">
         <v>5</v>
       </c>
-      <c r="E10" s="69"/>
-      <c r="F10" s="66" t="s">
+      <c r="E10" s="83"/>
+      <c r="F10" s="76" t="s">
+        <v>37</v>
+      </c>
+      <c r="G10" s="76"/>
+      <c r="H10" s="77" t="s">
         <v>38</v>
       </c>
-      <c r="G10" s="66"/>
-      <c r="H10" s="82" t="s">
+      <c r="I10" s="78"/>
+      <c r="J10" s="76" t="s">
         <v>39</v>
       </c>
-      <c r="I10" s="83"/>
-      <c r="J10" s="66" t="s">
-        <v>40</v>
-      </c>
-      <c r="K10" s="66"/>
-      <c r="L10" s="66" t="s">
+      <c r="K10" s="76"/>
+      <c r="L10" s="76" t="s">
         <v>1</v>
       </c>
-      <c r="M10" s="66"/>
+      <c r="M10" s="76"/>
     </row>
     <row r="11" spans="1:13" ht="42.75" customHeight="1">
       <c r="A11" s="5"/>
-      <c r="B11" s="67"/>
-      <c r="C11" s="68"/>
-      <c r="D11" s="67"/>
-      <c r="E11" s="68"/>
-      <c r="F11" s="67"/>
-      <c r="G11" s="68"/>
-      <c r="H11" s="67"/>
-      <c r="I11" s="68"/>
-      <c r="J11" s="67"/>
-      <c r="K11" s="68"/>
-      <c r="L11" s="67"/>
-      <c r="M11" s="68"/>
+      <c r="B11" s="79"/>
+      <c r="C11" s="80"/>
+      <c r="D11" s="79"/>
+      <c r="E11" s="80"/>
+      <c r="F11" s="79"/>
+      <c r="G11" s="80"/>
+      <c r="H11" s="79"/>
+      <c r="I11" s="80"/>
+      <c r="J11" s="79"/>
+      <c r="K11" s="80"/>
+      <c r="L11" s="79"/>
+      <c r="M11" s="80"/>
     </row>
     <row r="13" spans="1:13" ht="16.5">
-      <c r="B13" s="70" t="s">
-        <v>49</v>
+      <c r="B13" s="61" t="s">
+        <v>48</v>
       </c>
-      <c r="C13" s="71"/>
-      <c r="D13" s="71"/>
-      <c r="E13" s="71"/>
-      <c r="F13" s="71"/>
-      <c r="G13" s="71"/>
-      <c r="H13" s="71"/>
-      <c r="I13" s="71"/>
-      <c r="J13" s="71"/>
-      <c r="K13" s="71"/>
-      <c r="L13" s="71"/>
-      <c r="M13" s="72"/>
+      <c r="C13" s="62"/>
+      <c r="D13" s="62"/>
+      <c r="E13" s="62"/>
+      <c r="F13" s="62"/>
+      <c r="G13" s="62"/>
+      <c r="H13" s="62"/>
+      <c r="I13" s="62"/>
+      <c r="J13" s="62"/>
+      <c r="K13" s="62"/>
+      <c r="L13" s="62"/>
+      <c r="M13" s="63"/>
     </row>
     <row r="14" spans="1:13" ht="51" customHeight="1">
-      <c r="B14" s="76" t="s">
-        <v>66</v>
+      <c r="B14" s="67" t="s">
+        <v>65</v>
       </c>
-      <c r="C14" s="77"/>
-      <c r="D14" s="77"/>
-      <c r="E14" s="77"/>
-      <c r="F14" s="77"/>
-      <c r="G14" s="77"/>
-      <c r="H14" s="77"/>
-      <c r="I14" s="77"/>
-      <c r="J14" s="77"/>
-      <c r="K14" s="77"/>
-      <c r="L14" s="77"/>
-      <c r="M14" s="78"/>
+      <c r="C14" s="68"/>
+      <c r="D14" s="68"/>
+      <c r="E14" s="68"/>
+      <c r="F14" s="68"/>
+      <c r="G14" s="68"/>
+      <c r="H14" s="68"/>
+      <c r="I14" s="68"/>
+      <c r="J14" s="68"/>
+      <c r="K14" s="68"/>
+      <c r="L14" s="68"/>
+      <c r="M14" s="69"/>
     </row>
     <row r="15" spans="1:13">
-      <c r="B15" s="79" t="s">
-        <v>52</v>
+      <c r="B15" s="73" t="s">
+        <v>51</v>
       </c>
-      <c r="C15" s="80"/>
-      <c r="D15" s="80"/>
-      <c r="E15" s="80"/>
-      <c r="F15" s="80"/>
-      <c r="G15" s="81"/>
-      <c r="H15" s="79" t="s">
-        <v>58</v>
+      <c r="C15" s="74"/>
+      <c r="D15" s="74"/>
+      <c r="E15" s="74"/>
+      <c r="F15" s="74"/>
+      <c r="G15" s="75"/>
+      <c r="H15" s="73" t="s">
+        <v>57</v>
       </c>
-      <c r="I15" s="80"/>
-      <c r="J15" s="80"/>
-      <c r="K15" s="80"/>
-      <c r="L15" s="80"/>
-      <c r="M15" s="81"/>
+      <c r="I15" s="74"/>
+      <c r="J15" s="74"/>
+      <c r="K15" s="74"/>
+      <c r="L15" s="74"/>
+      <c r="M15" s="75"/>
     </row>
     <row r="16" spans="1:13">
       <c r="B16" s="40"/>
@@ -45088,36 +45088,36 @@
       <c r="M31" s="48"/>
     </row>
     <row r="33" spans="2:13" ht="16.5">
-      <c r="B33" s="70" t="s">
-        <v>59</v>
+      <c r="B33" s="61" t="s">
+        <v>58</v>
       </c>
-      <c r="C33" s="71"/>
-      <c r="D33" s="71"/>
-      <c r="E33" s="71"/>
-      <c r="F33" s="71"/>
-      <c r="G33" s="71"/>
-      <c r="H33" s="71"/>
-      <c r="I33" s="71"/>
-      <c r="J33" s="71"/>
-      <c r="K33" s="71"/>
-      <c r="L33" s="71"/>
-      <c r="M33" s="72"/>
+      <c r="C33" s="62"/>
+      <c r="D33" s="62"/>
+      <c r="E33" s="62"/>
+      <c r="F33" s="62"/>
+      <c r="G33" s="62"/>
+      <c r="H33" s="62"/>
+      <c r="I33" s="62"/>
+      <c r="J33" s="62"/>
+      <c r="K33" s="62"/>
+      <c r="L33" s="62"/>
+      <c r="M33" s="63"/>
     </row>
     <row r="34" spans="2:13" ht="33.75" customHeight="1">
-      <c r="B34" s="73" t="s">
-        <v>65</v>
+      <c r="B34" s="64" t="s">
+        <v>64</v>
       </c>
-      <c r="C34" s="74"/>
-      <c r="D34" s="74"/>
-      <c r="E34" s="74"/>
-      <c r="F34" s="74"/>
-      <c r="G34" s="74"/>
-      <c r="H34" s="74"/>
-      <c r="I34" s="74"/>
-      <c r="J34" s="74"/>
-      <c r="K34" s="74"/>
-      <c r="L34" s="74"/>
-      <c r="M34" s="75"/>
+      <c r="C34" s="65"/>
+      <c r="D34" s="65"/>
+      <c r="E34" s="65"/>
+      <c r="F34" s="65"/>
+      <c r="G34" s="65"/>
+      <c r="H34" s="65"/>
+      <c r="I34" s="65"/>
+      <c r="J34" s="65"/>
+      <c r="K34" s="65"/>
+      <c r="L34" s="65"/>
+      <c r="M34" s="66"/>
     </row>
     <row r="35" spans="2:13">
       <c r="B35" s="40"/>
@@ -45345,17 +45345,6 @@
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="B33:M33"/>
-    <mergeCell ref="B34:M34"/>
-    <mergeCell ref="B14:M14"/>
-    <mergeCell ref="D7:M7"/>
-    <mergeCell ref="B9:M9"/>
-    <mergeCell ref="B13:M13"/>
-    <mergeCell ref="B15:G15"/>
-    <mergeCell ref="H15:M15"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="B11:C11"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B4:M4"/>
     <mergeCell ref="D2:M2"/>
@@ -45369,6 +45358,17 @@
     <mergeCell ref="J10:K10"/>
     <mergeCell ref="D10:E10"/>
     <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B33:M33"/>
+    <mergeCell ref="B34:M34"/>
+    <mergeCell ref="B14:M14"/>
+    <mergeCell ref="D7:M7"/>
+    <mergeCell ref="B9:M9"/>
+    <mergeCell ref="B13:M13"/>
+    <mergeCell ref="B15:G15"/>
+    <mergeCell ref="H15:M15"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="B11:C11"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -45403,7 +45403,7 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="18" customHeight="1">
@@ -45430,12 +45430,12 @@
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="67.5" customHeight="1">
       <c r="A5" s="91" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B5" s="92"/>
       <c r="C5" s="92"/>
@@ -45446,7 +45446,7 @@
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="18.75" customHeight="1">
@@ -45455,7 +45455,7 @@
       </c>
       <c r="B7" s="89"/>
       <c r="C7" s="85" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D7" s="86"/>
       <c r="E7" s="86"/>
@@ -45464,7 +45464,7 @@
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="25.5">
@@ -45472,7 +45472,7 @@
         <v>15</v>
       </c>
       <c r="B9" s="33" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C9" s="33" t="s">
         <v>26</v>
@@ -45501,7 +45501,7 @@
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -45566,7 +45566,7 @@
     </row>
     <row r="5" spans="1:7" ht="67.5" customHeight="1">
       <c r="A5" s="91" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B5" s="92"/>
       <c r="C5" s="92"/>
@@ -45581,7 +45581,7 @@
       </c>
       <c r="B7" s="90"/>
       <c r="C7" s="97" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D7" s="97"/>
       <c r="E7" s="97"/>
@@ -45593,7 +45593,7 @@
         <v>22</v>
       </c>
       <c r="B9" s="33" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C9" s="33" t="s">
         <v>26</v>
@@ -45674,7 +45674,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="99" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C4" s="100"/>
       <c r="D4" s="100"/>
@@ -45690,7 +45690,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="33" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -45729,7 +45729,7 @@
   <sheetData>
     <row r="2" spans="1:10" ht="18" customHeight="1">
       <c r="A2" s="98" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B2" s="98"/>
       <c r="C2" s="98"/>
@@ -45746,7 +45746,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="99" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C4" s="100"/>
       <c r="D4" s="101"/>
@@ -45759,10 +45759,10 @@
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="33" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B6" s="33" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -45787,8 +45787,8 @@
   </sheetPr>
   <dimension ref="A2:B7"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -45800,7 +45800,7 @@
   <sheetData>
     <row r="2" spans="1:2" ht="18">
       <c r="A2" s="98" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B2" s="98"/>
     </row>
@@ -45813,7 +45813,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>31</v>
+        <v>83</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -45897,7 +45897,7 @@
       <c r="B4" s="111"/>
       <c r="C4" s="112"/>
       <c r="D4" s="102" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E4" s="103"/>
       <c r="F4" s="103"/>
@@ -45911,22 +45911,22 @@
     </row>
     <row r="6" spans="1:13" ht="96.75" customHeight="1">
       <c r="A6" s="105" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B6" s="49" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C6" s="106"/>
       <c r="D6" s="106"/>
       <c r="E6" s="106"/>
       <c r="F6" s="49" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G6" s="106"/>
       <c r="H6" s="106"/>
       <c r="I6" s="106"/>
       <c r="J6" s="49" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="K6" s="106"/>
       <c r="L6" s="106"/>
@@ -45935,7 +45935,7 @@
     <row r="7" spans="1:13" ht="45" customHeight="1">
       <c r="A7" s="105"/>
       <c r="B7" s="49" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C7" s="107"/>
       <c r="D7" s="108"/>
@@ -45975,13 +45975,13 @@
         <v>8</v>
       </c>
       <c r="K9" s="33" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="L9" s="34" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="M9" s="34" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:13">
@@ -46043,21 +46043,21 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="39" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="37" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B3" s="37" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C3" s="36"/>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="38" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B4" s="38">
         <v>0</v>
@@ -46065,7 +46065,7 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="38" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B5" s="38">
         <v>0</v>
@@ -46073,7 +46073,7 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="38" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B6" s="38">
         <v>0</v>
@@ -46081,7 +46081,7 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="38" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B7" s="38">
         <v>0</v>
@@ -46089,20 +46089,20 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="39" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="37" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B11" s="37" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="38" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B12" s="38">
         <v>0</v>
@@ -46110,7 +46110,7 @@
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="38" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B13" s="38">
         <v>0</v>
@@ -46118,7 +46118,7 @@
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="38" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B14" s="38">
         <v>0</v>
@@ -46126,7 +46126,7 @@
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="38" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B15" s="38">
         <v>0</v>
@@ -46134,7 +46134,7 @@
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="39" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -46142,12 +46142,12 @@
         <v>2</v>
       </c>
       <c r="B19" s="37" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="38" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B20" s="38">
         <v>0</v>
@@ -46155,7 +46155,7 @@
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="38" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B21" s="38">
         <v>0</v>
@@ -46163,7 +46163,7 @@
     </row>
     <row r="22" spans="1:2">
       <c r="A22" s="38" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B22" s="38">
         <v>0</v>
@@ -46171,7 +46171,7 @@
     </row>
     <row r="23" spans="1:2">
       <c r="A23" s="38" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B23" s="38">
         <v>0</v>
@@ -46179,7 +46179,7 @@
     </row>
     <row r="24" spans="1:2">
       <c r="A24" s="38" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B24" s="38">
         <v>0</v>
@@ -46187,7 +46187,7 @@
     </row>
     <row r="25" spans="1:2">
       <c r="A25" s="38" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B25" s="38">
         <v>0</v>

</xml_diff>